<commit_message>
Listed ADCIN 16 as having the STM32's internal temperature sensor.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="449">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1362,6 +1362,9 @@
   </si>
   <si>
     <t>Motor 3?</t>
+  </si>
+  <si>
+    <t>Internal temperature sensor</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -3104,8 +3107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3260,6 +3263,9 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Moved U12_DRDY from X0D13 (X0_P1F) to X1D25 (X1_P1J).
The trace for this is a lot cleaner to run.
It also puts U12_DRDY on the same core as the I2C bus, which we want.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -1705,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,9 +2205,6 @@
       <c r="D15" t="s">
         <v>100</v>
       </c>
-      <c r="E15" t="s">
-        <v>417</v>
-      </c>
       <c r="H15" t="s">
         <v>283</v>
       </c>
@@ -2570,6 +2567,9 @@
       </c>
       <c r="J27" t="s">
         <v>104</v>
+      </c>
+      <c r="K27" t="s">
+        <v>417</v>
       </c>
       <c r="L27" t="s">
         <v>442</v>
@@ -3107,7 +3107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Big shuffling of the XMOS serial interfaces...
STM32_U1_RX moved to X0D12 (X0P1E).
STM32_U1_TX moved to X0D22 (X0P1G).
STM32_TIM3_CH2 (PB5) connected to X0D13 (X0P1F) for a 32MHz clock input to the XMOS for UART clocking.
U13_SA0 turns out to just be an address input. Disconnected from XMOS and connected to +3V3.
U13_INT1 moved to X1D10 (X1P1C) and U13_INT2 moved to X1D11 (X1P1D). This gets the U13 interrupt pins onto the I2C core, resolving that part of Issue #2.
uSD_SS assigned to X1D34 (X1P1K).
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="452">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -134,9 +134,6 @@
     <t>ADCIN 25</t>
   </si>
   <si>
-    <t>Timer outputs in 50+ pin range</t>
-  </si>
-  <si>
     <t>Signal</t>
   </si>
   <si>
@@ -785,9 +782,6 @@
     <t>UNCONNECTED SIGNALS</t>
   </si>
   <si>
-    <t>U13_SA0</t>
-  </si>
-  <si>
     <t>U13_INT2</t>
   </si>
   <si>
@@ -1365,6 +1359,21 @@
   </si>
   <si>
     <t>Internal temperature sensor</t>
+  </si>
+  <si>
+    <t>Timer outputs</t>
+  </si>
+  <si>
+    <t>PB5</t>
+  </si>
+  <si>
+    <t>XMOS UART Clock Input</t>
+  </si>
+  <si>
+    <t>STM32_TIM3_CH2</t>
+  </si>
+  <si>
+    <t>uSD_SS</t>
   </si>
 </sst>
 </file>
@@ -1705,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1723,7 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
@@ -1728,1374 +1737,1374 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="J3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F4" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E8" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F8" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I8" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="J8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N8" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E9" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F9" t="s">
+        <v>417</v>
+      </c>
+      <c r="H9" t="s">
+        <v>275</v>
+      </c>
+      <c r="I9" t="s">
+        <v>359</v>
+      </c>
+      <c r="J9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K9" t="s">
+        <v>226</v>
+      </c>
+      <c r="N9" t="s">
         <v>419</v>
-      </c>
-      <c r="H9" t="s">
-        <v>277</v>
-      </c>
-      <c r="I9" t="s">
-        <v>361</v>
-      </c>
-      <c r="J9" t="s">
-        <v>186</v>
-      </c>
-      <c r="K9" t="s">
-        <v>227</v>
-      </c>
-      <c r="N9" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I11" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N11" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I12" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="J12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K12" t="s">
-        <v>248</v>
-      </c>
-      <c r="L12" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="N12" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K13" t="s">
-        <v>247</v>
-      </c>
-      <c r="L13" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="N13" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
-        <v>256</v>
+        <v>247</v>
+      </c>
+      <c r="F14" t="s">
+        <v>250</v>
       </c>
       <c r="H14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L14" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="N14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="E15" t="s">
+        <v>450</v>
       </c>
       <c r="H15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I15" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L15" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="N15" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I16" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J16" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L16" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H17" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I17" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J17" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="L17" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I18" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J18" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L18" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I19" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L19" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E20" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H20" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I20" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J20" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="L20" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H21" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I21" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J21" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="L21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E22" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H22" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I22" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J22" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="L22" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E23" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I23" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J23" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="L23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>255</v>
+        <v>246</v>
+      </c>
+      <c r="F24" t="s">
+        <v>249</v>
       </c>
       <c r="H24" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I24" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K24" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="L24" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H25" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L25" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" t="s">
-        <v>257</v>
+        <v>102</v>
       </c>
       <c r="H26" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I26" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K26" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L26" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H27" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I27" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K27" t="s">
-        <v>417</v>
-      </c>
-      <c r="L27" t="s">
-        <v>442</v>
+        <v>415</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D28" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I28" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J28" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C29" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D29" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H29" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I29" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J29" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D30" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H30" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I30" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J30" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H31" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I31" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J31" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C32" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D32" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H32" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I32" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J32" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D33" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H33" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I33" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J33" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H34" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I34" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J34" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C35" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D35" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H35" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I35" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J35" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C36" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H36" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I36" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J36" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="K36" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C37" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E37" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H37" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K37" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H38" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I38" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J38" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K38" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H39" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I39" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J39" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K39" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C40" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H40" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I40" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J40" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="K40" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I41" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J41" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K41" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C44" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E44" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C45" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D45" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3105,28 +3114,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
         <v>25</v>
@@ -3179,10 +3188,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3190,10 +3199,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3201,7 +3210,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3209,7 +3218,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3265,7 +3274,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3278,10 +3287,10 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3289,10 +3298,10 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3300,10 +3309,10 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3311,10 +3320,10 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3322,7 +3331,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3330,7 +3339,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3345,154 +3354,168 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>447</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32">
         <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33">
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34">
         <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35">
         <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36">
         <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37">
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38">
         <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39">
         <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40">
         <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41">
         <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42">
         <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43">
         <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s">
+        <v>448</v>
+      </c>
+      <c r="D44" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -3517,19 +3540,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
-        <v>76</v>
-      </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3540,10 +3563,10 @@
         <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3554,10 +3577,10 @@
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3565,7 +3588,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3573,7 +3596,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,7 +3604,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3589,7 +3612,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3597,7 +3620,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3605,7 +3628,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3613,7 +3636,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3621,7 +3644,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3629,10 +3652,10 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3640,10 +3663,10 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3651,10 +3674,10 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3662,10 +3685,10 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
         <v>86</v>
-      </c>
-      <c r="E15" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -3690,38 +3713,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
         <v>109</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
         <v>112</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>113</v>
-      </c>
-      <c r="C3" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3741,16 +3764,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3758,7 +3781,7 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3766,7 +3789,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3774,10 +3797,10 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3785,10 +3808,10 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3796,10 +3819,10 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,10 +3830,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3818,10 +3841,10 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3829,10 +3852,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3840,10 +3863,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3851,10 +3874,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3862,7 +3885,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3870,7 +3893,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3878,7 +3901,7 @@
         <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3886,7 +3909,7 @@
         <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,10 +3917,10 @@
         <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3905,10 +3928,10 @@
         <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3916,10 +3939,10 @@
         <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3927,10 +3950,10 @@
         <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3938,10 +3961,10 @@
         <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C20" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3949,10 +3972,10 @@
         <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3960,10 +3983,10 @@
         <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C22" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,10 +3994,10 @@
         <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3982,13 +4005,13 @@
         <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3996,13 +4019,13 @@
         <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D25" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -4010,10 +4033,10 @@
         <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4021,10 +4044,10 @@
         <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4032,10 +4055,10 @@
         <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4043,7 +4066,7 @@
         <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4071,10 +4094,10 @@
         <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4082,10 +4105,10 @@
         <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4093,10 +4116,10 @@
         <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4104,10 +4127,10 @@
         <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C37" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -4115,10 +4138,10 @@
         <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4126,10 +4149,10 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4137,10 +4160,10 @@
         <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C40" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4148,10 +4171,10 @@
         <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4159,10 +4182,10 @@
         <v>100</v>
       </c>
       <c r="B42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4170,10 +4193,10 @@
         <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4181,10 +4204,10 @@
         <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C44" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4192,10 +4215,10 @@
         <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -4203,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -4211,7 +4234,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4219,7 +4242,7 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -4227,7 +4250,7 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -4235,7 +4258,7 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -4243,7 +4266,7 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -4251,7 +4274,7 @@
         <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -4259,7 +4282,7 @@
         <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -4267,7 +4290,7 @@
         <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -4275,7 +4298,7 @@
         <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -4283,7 +4306,7 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -4291,7 +4314,7 @@
         <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -4299,7 +4322,7 @@
         <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -4307,7 +4330,7 @@
         <v>124</v>
       </c>
       <c r="B59" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -4315,7 +4338,7 @@
         <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -4323,7 +4346,7 @@
         <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -4331,7 +4354,7 @@
         <v>119</v>
       </c>
       <c r="B62" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -4339,7 +4362,7 @@
         <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -4347,7 +4370,7 @@
         <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -4355,7 +4378,7 @@
         <v>112</v>
       </c>
       <c r="B65" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revised motor PWM connections to XMOS for alignment purposes.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -1715,7 +1715,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,6 +2191,9 @@
       <c r="J14" t="s">
         <v>98</v>
       </c>
+      <c r="K14" t="s">
+        <v>413</v>
+      </c>
       <c r="L14" t="s">
         <v>440</v>
       </c>
@@ -2519,9 +2522,6 @@
       <c r="J25" t="s">
         <v>101</v>
       </c>
-      <c r="K25" t="s">
-        <v>412</v>
-      </c>
       <c r="L25" t="s">
         <v>440</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>102</v>
       </c>
       <c r="K26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L26" t="s">
         <v>440</v>

</xml_diff>

<commit_message>
Assigned XMOS pins for IC5 interrupts.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="451">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1338,9 +1338,6 @@
   </si>
   <si>
     <t>Encoder?</t>
-  </si>
-  <si>
-    <t>PWM/encoder?</t>
   </si>
   <si>
     <t>SPI_MISO</t>
@@ -1715,7 +1712,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,9 +2191,6 @@
       <c r="K14" t="s">
         <v>413</v>
       </c>
-      <c r="L14" t="s">
-        <v>440</v>
-      </c>
       <c r="N14" t="s">
         <v>424</v>
       </c>
@@ -2215,7 +2209,7 @@
         <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H15" t="s">
         <v>281</v>
@@ -2226,8 +2220,8 @@
       <c r="J15" t="s">
         <v>99</v>
       </c>
-      <c r="L15" t="s">
-        <v>440</v>
+      <c r="K15" t="s">
+        <v>419</v>
       </c>
       <c r="N15" t="s">
         <v>425</v>
@@ -2496,9 +2490,6 @@
       <c r="K24" t="s">
         <v>414</v>
       </c>
-      <c r="L24" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2522,8 +2513,8 @@
       <c r="J25" t="s">
         <v>101</v>
       </c>
-      <c r="L25" t="s">
-        <v>440</v>
+      <c r="K25" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2551,9 +2542,6 @@
       <c r="K26" t="s">
         <v>412</v>
       </c>
-      <c r="L26" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2791,7 +2779,7 @@
         <v>104</v>
       </c>
       <c r="K36" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2820,7 +2808,7 @@
         <v>243</v>
       </c>
       <c r="K37" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2849,7 +2837,7 @@
         <v>392</v>
       </c>
       <c r="K38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2878,7 +2866,7 @@
         <v>393</v>
       </c>
       <c r="K39" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3210,7 +3198,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3274,7 +3262,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3339,7 +3327,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,7 +3342,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,10 +3500,10 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
+        <v>447</v>
+      </c>
+      <c r="D44" t="s">
         <v>448</v>
-      </c>
-      <c r="D44" t="s">
-        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oops, IC5 interrupt pins were backwards. Fixed.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -1712,7 +1712,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,7 +2221,7 @@
         <v>99</v>
       </c>
       <c r="K15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="N15" t="s">
         <v>425</v>
@@ -2514,7 +2514,7 @@
         <v>101</v>
       </c>
       <c r="K25" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
So SPI needs to be on specific pins to boot off flash, and it's ugly.
Old traces have been ripped up.
New pin assignments for SPI and servo/PWM connections made.
On the plus side, this moves the servo and motor PWM signals to the same core, which means one less thread.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="451">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1712,7 +1712,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="M36" sqref="M36:M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,11 +1721,13 @@
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
     <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="14" width="23" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" customWidth="1"/>
     <col min="16" max="16" width="14.140625" customWidth="1"/>
@@ -1784,7 +1786,7 @@
         <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="H2" t="s">
         <v>268</v>
@@ -1813,7 +1815,7 @@
         <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>431</v>
+        <v>251</v>
       </c>
       <c r="H3" t="s">
         <v>269</v>
@@ -1993,9 +1995,6 @@
       <c r="K8" t="s">
         <v>227</v>
       </c>
-      <c r="N8" t="s">
-        <v>418</v>
-      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2028,9 +2027,6 @@
       <c r="K9" t="s">
         <v>226</v>
       </c>
-      <c r="N9" t="s">
-        <v>419</v>
-      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -2110,7 +2106,7 @@
         <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="H12" t="s">
         <v>278</v>
@@ -2142,7 +2138,7 @@
         <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="H13" t="s">
         <v>279</v>
@@ -2189,7 +2185,7 @@
         <v>98</v>
       </c>
       <c r="K14" t="s">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="N14" t="s">
         <v>424</v>
@@ -2488,7 +2484,7 @@
         <v>100</v>
       </c>
       <c r="K24" t="s">
-        <v>414</v>
+        <v>428</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2530,6 +2526,9 @@
       <c r="D26" t="s">
         <v>102</v>
       </c>
+      <c r="E26" t="s">
+        <v>416</v>
+      </c>
       <c r="H26" t="s">
         <v>292</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>102</v>
       </c>
       <c r="K26" t="s">
-        <v>412</v>
+        <v>426</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2767,7 +2766,7 @@
         <v>104</v>
       </c>
       <c r="E36" t="s">
-        <v>427</v>
+        <v>450</v>
       </c>
       <c r="H36" t="s">
         <v>302</v>
@@ -2779,7 +2778,7 @@
         <v>104</v>
       </c>
       <c r="K36" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2795,9 +2794,6 @@
       <c r="D37" t="s">
         <v>243</v>
       </c>
-      <c r="E37" t="s">
-        <v>426</v>
-      </c>
       <c r="H37" t="s">
         <v>303</v>
       </c>
@@ -2808,7 +2804,7 @@
         <v>243</v>
       </c>
       <c r="K37" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2837,7 +2833,7 @@
         <v>392</v>
       </c>
       <c r="K38" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2866,7 +2862,7 @@
         <v>393</v>
       </c>
       <c r="K39" t="s">
-        <v>441</v>
+        <v>412</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2895,7 +2891,7 @@
         <v>394</v>
       </c>
       <c r="K40" t="s">
-        <v>251</v>
+        <v>413</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2924,7 +2920,7 @@
         <v>395</v>
       </c>
       <c r="K41" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Further shuffling of PWM/servo pins. Moved the IC5 interrupt pins this time as well.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -1712,7 +1712,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36:M41"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,7 +2217,7 @@
         <v>99</v>
       </c>
       <c r="K15" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="N15" t="s">
         <v>425</v>
@@ -2510,7 +2510,7 @@
         <v>101</v>
       </c>
       <c r="K25" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2778,7 +2778,7 @@
         <v>104</v>
       </c>
       <c r="K36" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2804,7 +2804,7 @@
         <v>243</v>
       </c>
       <c r="K37" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2833,7 +2833,7 @@
         <v>392</v>
       </c>
       <c r="K38" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2862,7 +2862,7 @@
         <v>393</v>
       </c>
       <c r="K39" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>394</v>
       </c>
       <c r="K40" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2920,7 +2920,7 @@
         <v>395</v>
       </c>
       <c r="K41" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Resolved the U14 SS pin location issue.
Nuke-from-orbit fix: U14 moved to the I2C bus because it supports both.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="450">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1266,9 +1266,6 @@
   </si>
   <si>
     <t>U12_DRDY</t>
-  </si>
-  <si>
-    <t>GYRO_SS</t>
   </si>
   <si>
     <t>Gadgeteer</t>
@@ -1712,7 +1709,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,7 +1783,7 @@
         <v>94</v>
       </c>
       <c r="E2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H2" t="s">
         <v>268</v>
@@ -1844,10 +1841,10 @@
         <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H4" t="s">
         <v>270</v>
@@ -1876,10 +1873,10 @@
         <v>181</v>
       </c>
       <c r="E5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H5" t="s">
         <v>271</v>
@@ -1908,10 +1905,10 @@
         <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H6" t="s">
         <v>272</v>
@@ -1943,10 +1940,10 @@
         <v>183</v>
       </c>
       <c r="E7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H7" t="s">
         <v>273</v>
@@ -1978,10 +1975,10 @@
         <v>184</v>
       </c>
       <c r="E8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H8" t="s">
         <v>274</v>
@@ -2010,10 +2007,10 @@
         <v>185</v>
       </c>
       <c r="E9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H9" t="s">
         <v>275</v>
@@ -2042,10 +2039,10 @@
         <v>186</v>
       </c>
       <c r="E10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H10" t="s">
         <v>276</v>
@@ -2060,7 +2057,7 @@
         <v>225</v>
       </c>
       <c r="N10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2089,7 +2086,7 @@
         <v>224</v>
       </c>
       <c r="N11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2106,7 +2103,7 @@
         <v>96</v>
       </c>
       <c r="E12" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H12" t="s">
         <v>278</v>
@@ -2121,7 +2118,7 @@
         <v>255</v>
       </c>
       <c r="N12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2138,7 +2135,7 @@
         <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H13" t="s">
         <v>279</v>
@@ -2153,7 +2150,7 @@
         <v>254</v>
       </c>
       <c r="N13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2185,10 +2182,10 @@
         <v>98</v>
       </c>
       <c r="K14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="N14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2205,7 +2202,7 @@
         <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H15" t="s">
         <v>281</v>
@@ -2217,10 +2214,10 @@
         <v>99</v>
       </c>
       <c r="K15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="N15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2249,7 +2246,7 @@
         <v>404</v>
       </c>
       <c r="L16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2278,7 +2275,7 @@
         <v>405</v>
       </c>
       <c r="L17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2307,7 +2304,7 @@
         <v>406</v>
       </c>
       <c r="L18" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2336,7 +2333,7 @@
         <v>407</v>
       </c>
       <c r="L19" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2365,7 +2362,7 @@
         <v>408</v>
       </c>
       <c r="L20" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2394,7 +2391,7 @@
         <v>409</v>
       </c>
       <c r="L21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2423,7 +2420,7 @@
         <v>410</v>
       </c>
       <c r="L22" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2452,7 +2449,7 @@
         <v>411</v>
       </c>
       <c r="L23" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2484,7 +2481,7 @@
         <v>100</v>
       </c>
       <c r="K24" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2510,7 +2507,7 @@
         <v>101</v>
       </c>
       <c r="K25" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2526,9 +2523,6 @@
       <c r="D26" t="s">
         <v>102</v>
       </c>
-      <c r="E26" t="s">
-        <v>416</v>
-      </c>
       <c r="H26" t="s">
         <v>292</v>
       </c>
@@ -2539,7 +2533,7 @@
         <v>102</v>
       </c>
       <c r="K26" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2766,7 +2760,7 @@
         <v>104</v>
       </c>
       <c r="E36" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H36" t="s">
         <v>302</v>
@@ -2778,7 +2772,7 @@
         <v>104</v>
       </c>
       <c r="K36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2891,7 +2885,7 @@
         <v>394</v>
       </c>
       <c r="K40" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2920,7 +2914,7 @@
         <v>395</v>
       </c>
       <c r="K41" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3194,7 +3188,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3258,7 +3252,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3323,7 +3317,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3338,7 +3332,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3496,10 +3490,10 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
+        <v>446</v>
+      </c>
+      <c r="D44" t="s">
         <v>447</v>
-      </c>
-      <c r="D44" t="s">
-        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved the UART timer.
Was on TIM3_CH2 (PB5), now TIM3_CH1 on PE3.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="451">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1368,6 +1368,9 @@
   </si>
   <si>
     <t>uSD_SS</t>
+  </si>
+  <si>
+    <t>PE3</t>
   </si>
 </sst>
 </file>
@@ -1708,7 +1711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -3092,10 +3095,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3492,7 +3495,18 @@
       <c r="C44" t="s">
         <v>446</v>
       </c>
-      <c r="D44" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>450</v>
+      </c>
+      <c r="D45" t="s">
         <v>447</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Shifted Arduino ADC connections to free up DAC output pins.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="452">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1349,9 +1349,6 @@
     <t>Motor 0</t>
   </si>
   <si>
-    <t>Motor 3?</t>
-  </si>
-  <si>
     <t>Internal temperature sensor</t>
   </si>
   <si>
@@ -1371,6 +1368,12 @@
   </si>
   <si>
     <t>PE3</t>
+  </si>
+  <si>
+    <t>PC4</t>
+  </si>
+  <si>
+    <t>PC5</t>
   </si>
 </sst>
 </file>
@@ -2205,7 +2208,7 @@
         <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H15" t="s">
         <v>281</v>
@@ -2763,7 +2766,7 @@
         <v>104</v>
       </c>
       <c r="E36" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H36" t="s">
         <v>302</v>
@@ -3097,8 +3100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3152,17 +3155,11 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3172,7 +3169,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3183,7 +3180,7 @@
         <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3191,7 +3188,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>442</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3199,7 +3196,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3238,16 +3235,22 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
+      <c r="C16" t="s">
+        <v>450</v>
+      </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="C17" t="s">
+        <v>451</v>
+      </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3255,7 +3258,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3312,7 +3315,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>442</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,13 +3323,16 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>443</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -3335,7 +3341,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3493,7 +3499,7 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,10 +3510,10 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D45" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DAC headers JP22 and JP23.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -3100,8 +3100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Supply voltage monitor circuit added.
Analog input connected to ADC channel 25 (PE10).
Enable input to SVM connected to PE11.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="455">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1374,6 +1374,15 @@
   </si>
   <si>
     <t>PC5</t>
+  </si>
+  <si>
+    <t>DAC0</t>
+  </si>
+  <si>
+    <t>DAC1</t>
+  </si>
+  <si>
+    <t>Supply voltage monitor</t>
   </si>
 </sst>
 </file>
@@ -3101,7 +3110,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3155,11 +3164,17 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="D6" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="D7" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3337,6 +3352,9 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
U14 interrupt pins connected to XMOS.
Most of the neighboring traces have been shifted slightly in order to maintain power/ground plane integrity.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -1723,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,9 +1937,6 @@
       <c r="K6" t="s">
         <v>229</v>
       </c>
-      <c r="N6" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1972,9 +1969,6 @@
       <c r="K7" t="s">
         <v>228</v>
       </c>
-      <c r="N7" t="s">
-        <v>257</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2434,6 +2428,9 @@
       <c r="J22" t="s">
         <v>410</v>
       </c>
+      <c r="K22" t="s">
+        <v>257</v>
+      </c>
       <c r="L22" t="s">
         <v>438</v>
       </c>
@@ -2462,6 +2459,9 @@
       </c>
       <c r="J23" t="s">
         <v>411</v>
+      </c>
+      <c r="K23" t="s">
+        <v>256</v>
       </c>
       <c r="L23" t="s">
         <v>438</v>
@@ -3109,7 +3109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Moved Arduino D2 and D4 to free SPI pins for AMIS-39101.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="453">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -255,12 +255,6 @@
   </si>
   <si>
     <t>PD9</t>
-  </si>
-  <si>
-    <t>PE14</t>
-  </si>
-  <si>
-    <t>PE15</t>
   </si>
   <si>
     <t>PD10</t>
@@ -1723,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,1353 +1745,1353 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E1" t="s">
         <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K1" t="s">
         <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="N1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F4" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="J4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="J5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F8" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F9" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="I9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="J10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I11" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N11" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K12" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="N12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H13" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="J14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K14" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="N14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I15" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="J15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K15" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="N15" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I16" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J16" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="L16" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I17" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="J17" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L17" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I18" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J18" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H19" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I19" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="L19" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C20" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H20" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I20" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J20" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L20" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E21" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H21" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="J21" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L21" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E22" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H22" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I22" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J22" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="K22" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L22" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H23" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J23" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="K23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L23" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I24" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K24" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B25" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C25" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H25" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I25" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C26" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I26" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K26" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H27" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I27" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K27" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D28" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H28" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I28" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J28" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H29" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I29" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="J29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D30" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H30" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I30" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J30" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H31" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I31" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J31" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C32" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D32" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H32" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I32" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="J32" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C33" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D33" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H33" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I33" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J33" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C34" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D34" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H34" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I34" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J34" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C35" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D35" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H35" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I35" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J35" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H36" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I36" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K36" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C37" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H37" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K37" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C38" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H38" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I38" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="J38" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K38" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C39" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E39" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H39" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I39" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J39" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K39" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D40" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E40" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H40" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I40" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J40" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K40" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D41" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E41" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H41" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I41" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J41" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K41" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C42" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D42" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E42" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C43" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D43" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C44" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D44" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E44" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C45" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D45" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -3165,7 +3159,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3173,7 +3167,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3251,7 +3245,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
@@ -3262,7 +3256,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D17" t="s">
         <v>67</v>
@@ -3273,7 +3267,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3330,7 +3324,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3338,7 +3332,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3346,7 +3340,7 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,12 +3348,12 @@
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3517,7 +3511,7 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3528,10 +3522,10 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D45" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -3543,8 +3537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3568,7 +3562,7 @@
         <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3582,7 +3576,7 @@
         <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3596,7 +3590,7 @@
         <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3604,7 +3598,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3620,7 +3614,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3644,7 +3638,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3652,7 +3646,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3671,7 +3665,7 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3682,7 +3676,7 @@
         <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3690,10 +3684,10 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3701,10 +3695,10 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3729,38 +3723,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
         <v>111</v>
-      </c>
-      <c r="B3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3780,16 +3774,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,7 +3791,7 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,7 +3799,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3813,10 +3807,10 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3824,10 +3818,10 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,10 +3829,10 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,10 +3840,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3857,10 +3851,10 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3868,10 +3862,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3879,10 +3873,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C10" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3890,10 +3884,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3901,7 +3895,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3909,7 +3903,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3917,7 +3911,7 @@
         <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3925,7 +3919,7 @@
         <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3933,10 +3927,10 @@
         <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3944,10 +3938,10 @@
         <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C17" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3955,10 +3949,10 @@
         <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3966,10 +3960,10 @@
         <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3977,10 +3971,10 @@
         <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3988,10 +3982,10 @@
         <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C21" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3999,10 +3993,10 @@
         <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C22" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4010,10 +4004,10 @@
         <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4021,13 +4015,13 @@
         <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D24" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4035,13 +4029,13 @@
         <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D25" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -4049,10 +4043,10 @@
         <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4060,10 +4054,10 @@
         <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4071,10 +4065,10 @@
         <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4082,7 +4076,7 @@
         <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4110,10 +4104,10 @@
         <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4121,10 +4115,10 @@
         <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C35" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4132,10 +4126,10 @@
         <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4143,10 +4137,10 @@
         <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C37" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -4154,10 +4148,10 @@
         <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C38" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4165,10 +4159,10 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4176,10 +4170,10 @@
         <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C40" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4187,10 +4181,10 @@
         <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C41" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4198,10 +4192,10 @@
         <v>100</v>
       </c>
       <c r="B42" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C42" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4209,10 +4203,10 @@
         <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C43" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4220,10 +4214,10 @@
         <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C44" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4231,10 +4225,10 @@
         <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C45" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -4242,7 +4236,7 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -4250,7 +4244,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4258,7 +4252,7 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -4266,7 +4260,7 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -4274,7 +4268,7 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -4282,7 +4276,7 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -4290,7 +4284,7 @@
         <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -4298,7 +4292,7 @@
         <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -4306,7 +4300,7 @@
         <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -4314,7 +4308,7 @@
         <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -4322,7 +4316,7 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -4330,7 +4324,7 @@
         <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -4338,7 +4332,7 @@
         <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -4346,7 +4340,7 @@
         <v>124</v>
       </c>
       <c r="B59" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -4354,7 +4348,7 @@
         <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -4362,7 +4356,7 @@
         <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -4370,7 +4364,7 @@
         <v>119</v>
       </c>
       <c r="B62" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -4378,7 +4372,7 @@
         <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -4386,7 +4380,7 @@
         <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -4394,7 +4388,7 @@
         <v>112</v>
       </c>
       <c r="B65" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved XMOS UART clock back to STM32_TIM3_CH2.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="454">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Arduino 3</t>
   </si>
   <si>
-    <t>Arduino 5</t>
-  </si>
-  <si>
     <t>Arduino 6</t>
   </si>
   <si>
@@ -1377,6 +1374,12 @@
   </si>
   <si>
     <t>Supply voltage monitor</t>
+  </si>
+  <si>
+    <t>PB13, PD0</t>
+  </si>
+  <si>
+    <t>Arduino 5 OR Arduino 10</t>
   </si>
 </sst>
 </file>
@@ -1717,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,1353 +1748,1353 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E1" t="s">
         <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K1" t="s">
         <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="N14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="N15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I19" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L19" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="L20" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L21" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I22" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L22" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I23" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L23" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I24" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K24" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I25" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I26" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K26" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K27" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D30" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J30" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I31" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J31" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I32" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J33" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D34" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I34" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J34" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D35" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J35" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K36" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H37" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I37" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K37" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C38" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I38" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J38" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K38" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J39" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K39" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C40" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I40" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J40" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K40" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C41" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J41" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K41" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C43" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C44" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C45" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3104,7 +3107,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3159,7 +3162,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3167,7 +3170,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3245,7 +3248,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
@@ -3256,7 +3259,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D17" t="s">
         <v>67</v>
@@ -3267,7 +3270,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3324,7 +3327,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3332,7 +3335,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3340,7 +3343,7 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3348,12 +3351,12 @@
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3378,10 +3381,10 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>452</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>453</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3395,7 +3398,7 @@
         <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3409,7 +3412,7 @@
         <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3423,7 +3426,7 @@
         <v>51</v>
       </c>
       <c r="D36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3511,6 +3514,9 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
+        <v>442</v>
+      </c>
+      <c r="D44" t="s">
         <v>443</v>
       </c>
     </row>
@@ -3522,10 +3528,7 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>447</v>
-      </c>
-      <c r="D45" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>
@@ -3537,7 +3540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -3550,19 +3553,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
-        <v>75</v>
-      </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3573,10 +3576,10 @@
         <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3587,10 +3590,10 @@
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3638,7 +3641,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3646,7 +3649,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3665,7 +3668,7 @@
         <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3676,7 +3679,7 @@
         <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3684,10 +3687,10 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3695,10 +3698,10 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s">
         <v>83</v>
-      </c>
-      <c r="E15" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3723,38 +3726,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>107</v>
-      </c>
-      <c r="C2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
         <v>109</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3774,16 +3777,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3791,7 +3794,7 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3799,7 +3802,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3807,10 +3810,10 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3818,10 +3821,10 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3829,10 +3832,10 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3840,10 +3843,10 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3851,10 +3854,10 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3862,10 +3865,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3873,10 +3876,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3884,10 +3887,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3895,7 +3898,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3903,7 +3906,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3911,7 +3914,7 @@
         <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3919,7 +3922,7 @@
         <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3927,10 +3930,10 @@
         <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3938,10 +3941,10 @@
         <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3949,10 +3952,10 @@
         <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3960,10 +3963,10 @@
         <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,10 +3974,10 @@
         <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3982,10 +3985,10 @@
         <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3993,10 +3996,10 @@
         <v>96</v>
       </c>
       <c r="B22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4004,10 +4007,10 @@
         <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4015,13 +4018,13 @@
         <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4029,13 +4032,13 @@
         <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -4043,10 +4046,10 @@
         <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4054,10 +4057,10 @@
         <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4065,10 +4068,10 @@
         <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4076,7 +4079,7 @@
         <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4104,10 +4107,10 @@
         <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4115,10 +4118,10 @@
         <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4126,10 +4129,10 @@
         <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -4137,10 +4140,10 @@
         <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -4148,10 +4151,10 @@
         <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4159,10 +4162,10 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4170,10 +4173,10 @@
         <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4181,10 +4184,10 @@
         <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4192,10 +4195,10 @@
         <v>100</v>
       </c>
       <c r="B42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4203,10 +4206,10 @@
         <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4214,10 +4217,10 @@
         <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4225,10 +4228,10 @@
         <v>95</v>
       </c>
       <c r="B45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -4236,7 +4239,7 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -4244,7 +4247,7 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4252,7 +4255,7 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -4260,7 +4263,7 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -4268,7 +4271,7 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -4276,7 +4279,7 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -4284,7 +4287,7 @@
         <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -4292,7 +4295,7 @@
         <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -4300,7 +4303,7 @@
         <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -4308,7 +4311,7 @@
         <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -4316,7 +4319,7 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -4324,7 +4327,7 @@
         <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -4332,7 +4335,7 @@
         <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -4340,7 +4343,7 @@
         <v>124</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -4348,7 +4351,7 @@
         <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -4356,7 +4359,7 @@
         <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -4364,7 +4367,7 @@
         <v>119</v>
       </c>
       <c r="B62" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -4372,7 +4375,7 @@
         <v>117</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -4380,7 +4383,7 @@
         <v>114</v>
       </c>
       <c r="B64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -4388,7 +4391,7 @@
         <v>112</v>
       </c>
       <c r="B65" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added missing STM32 signals to Arduino connections tab.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="482">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1449,6 +1449,21 @@
   </si>
   <si>
     <t>DAC 2</t>
+  </si>
+  <si>
+    <t>PB1/PC4</t>
+  </si>
+  <si>
+    <t>PB0/PC5</t>
+  </si>
+  <si>
+    <t>PA0</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>3.3V</t>
   </si>
 </sst>
 </file>
@@ -3175,7 +3190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -3609,8 +3624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,6 +3792,9 @@
       <c r="A16">
         <v>14</v>
       </c>
+      <c r="D16" t="s">
+        <v>481</v>
+      </c>
       <c r="E16" t="s">
         <v>454</v>
       </c>
@@ -3785,6 +3803,9 @@
       <c r="A17">
         <v>15</v>
       </c>
+      <c r="D17" t="s">
+        <v>479</v>
+      </c>
       <c r="E17" t="s">
         <v>455</v>
       </c>
@@ -3793,6 +3814,9 @@
       <c r="A18">
         <v>16</v>
       </c>
+      <c r="D18" t="s">
+        <v>480</v>
+      </c>
       <c r="E18" t="s">
         <v>456</v>
       </c>
@@ -3801,6 +3825,9 @@
       <c r="A19">
         <v>17</v>
       </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
       <c r="E19" t="s">
         <v>457</v>
       </c>
@@ -3809,6 +3836,9 @@
       <c r="A20">
         <v>18</v>
       </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
       <c r="E20" t="s">
         <v>458</v>
       </c>
@@ -3817,6 +3847,9 @@
       <c r="A21">
         <v>19</v>
       </c>
+      <c r="D21" t="s">
+        <v>477</v>
+      </c>
       <c r="E21" t="s">
         <v>459</v>
       </c>
@@ -3824,6 +3857,9 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>478</v>
       </c>
       <c r="E22" t="s">
         <v>460</v>

</xml_diff>

<commit_message>
Deleted long-obsolete "Old XMOS" tab.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,21 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
     <sheet name="STM32 Connections" sheetId="2" r:id="rId2"/>
     <sheet name="Arduino Connections" sheetId="3" r:id="rId3"/>
     <sheet name="I2C" sheetId="4" r:id="rId4"/>
-    <sheet name="Old XMOS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="458">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -623,66 +622,6 @@
     <t>P8B7</t>
   </si>
   <si>
-    <t>P32A0</t>
-  </si>
-  <si>
-    <t>P32A1</t>
-  </si>
-  <si>
-    <t>P32A2</t>
-  </si>
-  <si>
-    <t>P32A3</t>
-  </si>
-  <si>
-    <t>P32A4</t>
-  </si>
-  <si>
-    <t>P32A5</t>
-  </si>
-  <si>
-    <t>P32A6</t>
-  </si>
-  <si>
-    <t>P32A7</t>
-  </si>
-  <si>
-    <t>P32A8</t>
-  </si>
-  <si>
-    <t>P32A9</t>
-  </si>
-  <si>
-    <t>P32A10</t>
-  </si>
-  <si>
-    <t>P32A11</t>
-  </si>
-  <si>
-    <t>P32A12</t>
-  </si>
-  <si>
-    <t>P32A13</t>
-  </si>
-  <si>
-    <t>P32A14</t>
-  </si>
-  <si>
-    <t>P32A15</t>
-  </si>
-  <si>
-    <t>P32A16</t>
-  </si>
-  <si>
-    <t>P32A17</t>
-  </si>
-  <si>
-    <t>P32A18</t>
-  </si>
-  <si>
-    <t>P32A19</t>
-  </si>
-  <si>
     <t>JP5_0</t>
   </si>
   <si>
@@ -731,15 +670,6 @@
     <t>P8D7</t>
   </si>
   <si>
-    <t>SPI</t>
-  </si>
-  <si>
-    <t>P4E2</t>
-  </si>
-  <si>
-    <t>P4E3</t>
-  </si>
-  <si>
     <t>P1L</t>
   </si>
   <si>
@@ -765,9 +695,6 @@
   </si>
   <si>
     <t>EEPROM_SS</t>
-  </si>
-  <si>
-    <t>SPI?</t>
   </si>
   <si>
     <t>UNCONNECTED SIGNALS</t>
@@ -1832,7 +1759,7 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="C1" t="s">
         <v>111</v>
@@ -1844,10 +1771,10 @@
         <v>38</v>
       </c>
       <c r="F1" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="H1" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="I1" t="s">
         <v>111</v>
@@ -1859,10 +1786,10 @@
         <v>38</v>
       </c>
       <c r="L1" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="N1" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1873,25 +1800,25 @@
         <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="D2" t="s">
         <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="H2" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="I2" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="J2" t="s">
         <v>91</v>
       </c>
       <c r="K2" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1902,25 +1829,25 @@
         <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="D3" t="s">
         <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="H3" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="I3" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="J3" t="s">
         <v>92</v>
       </c>
       <c r="K3" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1931,28 +1858,28 @@
         <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="D4" t="s">
         <v>177</v>
       </c>
       <c r="E4" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="F4" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="H4" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="I4" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="J4" t="s">
         <v>177</v>
       </c>
       <c r="K4" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1963,28 +1890,28 @@
         <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="D5" t="s">
         <v>178</v>
       </c>
       <c r="E5" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="F5" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="H5" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="I5" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="J5" t="s">
         <v>178</v>
       </c>
       <c r="K5" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1995,28 +1922,28 @@
         <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="D6" t="s">
         <v>179</v>
       </c>
       <c r="E6" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
       <c r="F6" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="H6" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="I6" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="J6" t="s">
         <v>179</v>
       </c>
       <c r="K6" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -2027,28 +1954,28 @@
         <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="D7" t="s">
         <v>180</v>
       </c>
       <c r="E7" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="F7" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="H7" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="I7" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="J7" t="s">
         <v>180</v>
       </c>
       <c r="K7" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2059,28 +1986,28 @@
         <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="D8" t="s">
         <v>181</v>
       </c>
       <c r="E8" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
       <c r="F8" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="H8" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="I8" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="J8" t="s">
         <v>181</v>
       </c>
       <c r="K8" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2091,28 +2018,28 @@
         <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="D9" t="s">
         <v>182</v>
       </c>
       <c r="E9" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="F9" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="H9" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="I9" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="J9" t="s">
         <v>182</v>
       </c>
       <c r="K9" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2123,31 +2050,31 @@
         <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="D10" t="s">
         <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="F10" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="H10" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="I10" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="J10" t="s">
         <v>183</v>
       </c>
       <c r="K10" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="N10" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2158,25 +2085,25 @@
         <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="D11" t="s">
         <v>184</v>
       </c>
       <c r="H11" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="I11" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="J11" t="s">
         <v>184</v>
       </c>
       <c r="K11" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="N11" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2187,28 +2114,28 @@
         <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="D12" t="s">
         <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="H12" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="I12" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="J12" t="s">
         <v>93</v>
       </c>
       <c r="K12" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="N12" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2219,28 +2146,28 @@
         <v>123</v>
       </c>
       <c r="C13" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="D13" t="s">
         <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
       <c r="H13" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="I13" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="J13" t="s">
         <v>94</v>
       </c>
       <c r="K13" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="N13" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2251,31 +2178,31 @@
         <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="D14" t="s">
         <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="F14" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="H14" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="I14" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="J14" t="s">
         <v>95</v>
       </c>
       <c r="K14" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="N14" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2286,28 +2213,28 @@
         <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="D15" t="s">
         <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
       <c r="H15" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="I15" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="J15" t="s">
         <v>96</v>
       </c>
       <c r="K15" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="N15" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2318,25 +2245,25 @@
         <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="D16" t="s">
         <v>193</v>
       </c>
       <c r="E16" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="H16" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="I16" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="J16" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
       <c r="L16" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2347,25 +2274,25 @@
         <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="D17" t="s">
         <v>194</v>
       </c>
       <c r="E17" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="H17" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="I17" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="J17" t="s">
-        <v>402</v>
+        <v>378</v>
       </c>
       <c r="L17" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2376,25 +2303,25 @@
         <v>128</v>
       </c>
       <c r="C18" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="D18" t="s">
         <v>195</v>
       </c>
       <c r="E18" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="H18" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="I18" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="J18" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="L18" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2405,25 +2332,25 @@
         <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="D19" t="s">
         <v>196</v>
       </c>
       <c r="E19" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="H19" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="I19" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="J19" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="L19" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2434,25 +2361,25 @@
         <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="D20" t="s">
         <v>197</v>
       </c>
       <c r="E20" t="s">
+        <v>235</v>
+      </c>
+      <c r="H20" t="s">
         <v>259</v>
       </c>
-      <c r="H20" t="s">
-        <v>283</v>
-      </c>
       <c r="I20" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="J20" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
       <c r="L20" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2463,25 +2390,25 @@
         <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="D21" t="s">
         <v>198</v>
       </c>
       <c r="E21" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="H21" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="I21" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="J21" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
       <c r="L21" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2492,28 +2419,28 @@
         <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="D22" t="s">
         <v>199</v>
       </c>
       <c r="E22" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="H22" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="I22" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="J22" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="K22" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="L22" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2524,28 +2451,28 @@
         <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="D23" t="s">
         <v>200</v>
       </c>
       <c r="E23" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="H23" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="I23" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="J23" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="K23" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="L23" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -2556,28 +2483,28 @@
         <v>134</v>
       </c>
       <c r="C24" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="D24" t="s">
         <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="F24" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="H24" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="I24" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="J24" t="s">
         <v>97</v>
       </c>
       <c r="K24" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2588,22 +2515,22 @@
         <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="D25" t="s">
         <v>98</v>
       </c>
       <c r="H25" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="I25" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="J25" t="s">
         <v>98</v>
       </c>
       <c r="K25" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2614,22 +2541,22 @@
         <v>136</v>
       </c>
       <c r="C26" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="D26" t="s">
         <v>99</v>
       </c>
       <c r="H26" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="I26" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="J26" t="s">
         <v>99</v>
       </c>
       <c r="K26" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2640,22 +2567,22 @@
         <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="D27" t="s">
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="I27" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="J27" t="s">
         <v>100</v>
       </c>
       <c r="K27" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2666,19 +2593,19 @@
         <v>138</v>
       </c>
       <c r="C28" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="D28" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="H28" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="I28" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="J28" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2689,19 +2616,19 @@
         <v>139</v>
       </c>
       <c r="C29" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="D29" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="H29" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="I29" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="J29" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2712,19 +2639,19 @@
         <v>140</v>
       </c>
       <c r="C30" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="D30" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
       <c r="H30" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="I30" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="J30" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2735,19 +2662,19 @@
         <v>141</v>
       </c>
       <c r="C31" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="D31" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="H31" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="I31" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="J31" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2758,19 +2685,19 @@
         <v>142</v>
       </c>
       <c r="C32" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="D32" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="H32" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="I32" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="J32" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2781,19 +2708,19 @@
         <v>143</v>
       </c>
       <c r="C33" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="D33" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
       <c r="H33" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="I33" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="J33" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2804,19 +2731,19 @@
         <v>144</v>
       </c>
       <c r="C34" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="D34" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="H34" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="I34" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="J34" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2827,19 +2754,19 @@
         <v>145</v>
       </c>
       <c r="C35" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="D35" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="H35" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="I35" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="J35" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2850,25 +2777,25 @@
         <v>146</v>
       </c>
       <c r="C36" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="D36" t="s">
         <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="H36" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="I36" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="J36" t="s">
         <v>101</v>
       </c>
       <c r="K36" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2879,22 +2806,22 @@
         <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="D37" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="H37" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="I37" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="J37" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="K37" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2905,25 +2832,25 @@
         <v>148</v>
       </c>
       <c r="C38" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="D38" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="E38" t="s">
         <v>192</v>
       </c>
       <c r="H38" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="I38" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="J38" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="K38" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2934,25 +2861,25 @@
         <v>149</v>
       </c>
       <c r="C39" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="D39" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="E39" t="s">
         <v>191</v>
       </c>
       <c r="H39" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="I39" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="J39" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="K39" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2963,25 +2890,25 @@
         <v>150</v>
       </c>
       <c r="C40" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="D40" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="E40" t="s">
         <v>190</v>
       </c>
       <c r="H40" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="I40" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="J40" t="s">
+        <v>367</v>
+      </c>
+      <c r="K40" t="s">
         <v>391</v>
-      </c>
-      <c r="K40" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2992,25 +2919,25 @@
         <v>151</v>
       </c>
       <c r="C41" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="D41" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="E41" t="s">
         <v>189</v>
       </c>
       <c r="H41" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="I41" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="J41" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="K41" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3021,10 +2948,10 @@
         <v>152</v>
       </c>
       <c r="C42" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="D42" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="E42" t="s">
         <v>188</v>
@@ -3038,10 +2965,10 @@
         <v>153</v>
       </c>
       <c r="C43" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="D43" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="E43" t="s">
         <v>187</v>
@@ -3055,10 +2982,10 @@
         <v>154</v>
       </c>
       <c r="C44" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="D44" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="E44" t="s">
         <v>186</v>
@@ -3072,10 +2999,10 @@
         <v>155</v>
       </c>
       <c r="C45" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="D45" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="E45" t="s">
         <v>185</v>
@@ -3190,7 +3117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -3246,7 +3173,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3254,7 +3181,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3332,7 +3259,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
@@ -3343,7 +3270,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="D17" t="s">
         <v>67</v>
@@ -3354,7 +3281,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3411,7 +3338,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3435,12 +3362,12 @@
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3465,10 +3392,10 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
       <c r="D33" t="s">
-        <v>453</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3598,10 +3525,10 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="D44" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3612,7 +3539,7 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -3793,10 +3720,10 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="E16" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3804,10 +3731,10 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
       <c r="E17" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3815,10 +3742,10 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="E18" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3829,7 +3756,7 @@
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3840,7 +3767,7 @@
         <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3848,10 +3775,10 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
       <c r="E21" t="s">
-        <v>459</v>
+        <v>435</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3859,10 +3786,10 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
       <c r="E22" t="s">
-        <v>460</v>
+        <v>436</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3870,7 +3797,7 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3878,7 +3805,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3886,7 +3813,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3894,7 +3821,7 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3902,7 +3829,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3910,7 +3837,7 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3918,7 +3845,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3926,7 +3853,7 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3934,7 +3861,7 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3942,7 +3869,7 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3950,10 +3877,10 @@
         <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="E33" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3961,10 +3888,10 @@
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="E34" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3972,7 +3899,7 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3980,7 +3907,7 @@
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3988,7 +3915,7 @@
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4008,7 +3935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -4058,638 +3985,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D65"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>181</v>
-      </c>
-      <c r="C8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>183</v>
-      </c>
-      <c r="C10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>128</v>
-      </c>
-      <c r="B14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>126</v>
-      </c>
-      <c r="B15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>118</v>
-      </c>
-      <c r="B16" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>115</v>
-      </c>
-      <c r="B17" t="s">
-        <v>194</v>
-      </c>
-      <c r="C17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>113</v>
-      </c>
-      <c r="B18" t="s">
-        <v>195</v>
-      </c>
-      <c r="C18" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>110</v>
-      </c>
-      <c r="B19" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>107</v>
-      </c>
-      <c r="B20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>106</v>
-      </c>
-      <c r="B21" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>96</v>
-      </c>
-      <c r="B22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>90</v>
-      </c>
-      <c r="B23" t="s">
-        <v>200</v>
-      </c>
-      <c r="C23" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>94</v>
-      </c>
-      <c r="B24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D24" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>89</v>
-      </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" t="s">
-        <v>244</v>
-      </c>
-      <c r="D25" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>87</v>
-      </c>
-      <c r="B26" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>86</v>
-      </c>
-      <c r="B27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>85</v>
-      </c>
-      <c r="B28" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>84</v>
-      </c>
-      <c r="C29" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>238</v>
-      </c>
-      <c r="C34" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>70</v>
-      </c>
-      <c r="B35" t="s">
-        <v>239</v>
-      </c>
-      <c r="C35" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>69</v>
-      </c>
-      <c r="B36" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>67</v>
-      </c>
-      <c r="B37" t="s">
-        <v>240</v>
-      </c>
-      <c r="C37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>82</v>
-      </c>
-      <c r="B38" t="s">
-        <v>229</v>
-      </c>
-      <c r="C38" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>21</v>
-      </c>
-      <c r="B39" t="s">
-        <v>230</v>
-      </c>
-      <c r="C39" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>76</v>
-      </c>
-      <c r="B40" t="s">
-        <v>231</v>
-      </c>
-      <c r="C40" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>75</v>
-      </c>
-      <c r="B41" t="s">
-        <v>232</v>
-      </c>
-      <c r="C41" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>100</v>
-      </c>
-      <c r="B42" t="s">
-        <v>233</v>
-      </c>
-      <c r="C42" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>98</v>
-      </c>
-      <c r="B43" t="s">
-        <v>234</v>
-      </c>
-      <c r="C43" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>97</v>
-      </c>
-      <c r="B44" t="s">
-        <v>235</v>
-      </c>
-      <c r="C44" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>95</v>
-      </c>
-      <c r="B45" t="s">
-        <v>236</v>
-      </c>
-      <c r="C45" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>4</v>
-      </c>
-      <c r="B46" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>8</v>
-      </c>
-      <c r="B48" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>9</v>
-      </c>
-      <c r="B49" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>11</v>
-      </c>
-      <c r="B50" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>13</v>
-      </c>
-      <c r="B51" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>31</v>
-      </c>
-      <c r="B52" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>33</v>
-      </c>
-      <c r="B53" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>35</v>
-      </c>
-      <c r="B54" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>38</v>
-      </c>
-      <c r="B55" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>3</v>
-      </c>
-      <c r="B56" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>127</v>
-      </c>
-      <c r="B57" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>125</v>
-      </c>
-      <c r="B58" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>124</v>
-      </c>
-      <c r="B59" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>122</v>
-      </c>
-      <c r="B60" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>121</v>
-      </c>
-      <c r="B61" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>119</v>
-      </c>
-      <c r="B62" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>117</v>
-      </c>
-      <c r="B63" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>114</v>
-      </c>
-      <c r="B64" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>112</v>
-      </c>
-      <c r="B65" t="s">
-        <v>220</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Moved the STM32 UART signals one IO pin to the right.
For layout reasons, it is more convenient to have the free IO pin run above the UART traces than below.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -1731,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,7 +2184,7 @@
         <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F14" t="s">
         <v>224</v>
@@ -2218,9 +2218,6 @@
       <c r="D15" t="s">
         <v>96</v>
       </c>
-      <c r="E15" t="s">
-        <v>420</v>
-      </c>
       <c r="H15" t="s">
         <v>254</v>
       </c>
@@ -2489,7 +2486,7 @@
         <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>220</v>
+        <v>420</v>
       </c>
       <c r="F24" t="s">
         <v>223</v>
@@ -2545,6 +2542,9 @@
       </c>
       <c r="D26" t="s">
         <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>221</v>
       </c>
       <c r="H26" t="s">
         <v>265</v>
@@ -3935,7 +3935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Defined TX/RX signals for XBee UART connection to U1.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="460">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1391,6 +1391,12 @@
   </si>
   <si>
     <t>3.3V</t>
+  </si>
+  <si>
+    <t>XBEE_DOUT</t>
+  </si>
+  <si>
+    <t>XBEE_DIN</t>
   </si>
 </sst>
 </file>
@@ -1732,7 +1738,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2193,7 @@
         <v>220</v>
       </c>
       <c r="F14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H14" t="s">
         <v>253</v>
@@ -2218,6 +2224,12 @@
       <c r="D15" t="s">
         <v>96</v>
       </c>
+      <c r="E15" t="s">
+        <v>458</v>
+      </c>
+      <c r="F15" t="s">
+        <v>223</v>
+      </c>
       <c r="H15" t="s">
         <v>254</v>
       </c>
@@ -2488,9 +2500,6 @@
       <c r="E24" t="s">
         <v>420</v>
       </c>
-      <c r="F24" t="s">
-        <v>223</v>
-      </c>
       <c r="H24" t="s">
         <v>263</v>
       </c>
@@ -2517,6 +2526,12 @@
       <c r="D25" t="s">
         <v>98</v>
       </c>
+      <c r="E25" t="s">
+        <v>459</v>
+      </c>
+      <c r="F25" t="s">
+        <v>224</v>
+      </c>
       <c r="H25" t="s">
         <v>264</v>
       </c>
@@ -2545,6 +2560,9 @@
       </c>
       <c r="E26" t="s">
         <v>221</v>
+      </c>
+      <c r="F26" t="s">
+        <v>224</v>
       </c>
       <c r="H26" t="s">
         <v>265</v>

</xml_diff>

<commit_message>
Created book in spreadsheet with fields for all signals.
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
     <sheet name="STM32 Connections" sheetId="2" r:id="rId2"/>
     <sheet name="Arduino Connections" sheetId="3" r:id="rId3"/>
     <sheet name="I2C" sheetId="4" r:id="rId4"/>
+    <sheet name="XMOS Multichip" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="579">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1397,6 +1398,363 @@
   </si>
   <si>
     <t>XBEE_DIN</t>
+  </si>
+  <si>
+    <t>Xcore Signal</t>
+  </si>
+  <si>
+    <t>D00</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>D03</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>D05</t>
+  </si>
+  <si>
+    <t>D06</t>
+  </si>
+  <si>
+    <t>D07</t>
+  </si>
+  <si>
+    <t>D08</t>
+  </si>
+  <si>
+    <t>D09</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>D20</t>
+  </si>
+  <si>
+    <t>D21</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t>D25</t>
+  </si>
+  <si>
+    <t>D26</t>
+  </si>
+  <si>
+    <t>D27</t>
+  </si>
+  <si>
+    <t>D28</t>
+  </si>
+  <si>
+    <t>D29</t>
+  </si>
+  <si>
+    <t>D30</t>
+  </si>
+  <si>
+    <t>D31</t>
+  </si>
+  <si>
+    <t>D32</t>
+  </si>
+  <si>
+    <t>D33</t>
+  </si>
+  <si>
+    <t>D34</t>
+  </si>
+  <si>
+    <t>D35</t>
+  </si>
+  <si>
+    <t>D36</t>
+  </si>
+  <si>
+    <t>D37</t>
+  </si>
+  <si>
+    <t>D38</t>
+  </si>
+  <si>
+    <t>D39</t>
+  </si>
+  <si>
+    <t>D40</t>
+  </si>
+  <si>
+    <t>D41</t>
+  </si>
+  <si>
+    <t>D42</t>
+  </si>
+  <si>
+    <t>D43</t>
+  </si>
+  <si>
+    <t>D49</t>
+  </si>
+  <si>
+    <t>D50</t>
+  </si>
+  <si>
+    <t>D51</t>
+  </si>
+  <si>
+    <t>D52</t>
+  </si>
+  <si>
+    <t>D53</t>
+  </si>
+  <si>
+    <t>D54</t>
+  </si>
+  <si>
+    <t>D55</t>
+  </si>
+  <si>
+    <t>D56</t>
+  </si>
+  <si>
+    <t>D57</t>
+  </si>
+  <si>
+    <t>D58</t>
+  </si>
+  <si>
+    <t>D61</t>
+  </si>
+  <si>
+    <t>D62</t>
+  </si>
+  <si>
+    <t>D63</t>
+  </si>
+  <si>
+    <t>D64</t>
+  </si>
+  <si>
+    <t>D65</t>
+  </si>
+  <si>
+    <t>D66</t>
+  </si>
+  <si>
+    <t>D67</t>
+  </si>
+  <si>
+    <t>D68</t>
+  </si>
+  <si>
+    <t>D69</t>
+  </si>
+  <si>
+    <t>D70</t>
+  </si>
+  <si>
+    <t>U1 Package Pin</t>
+  </si>
+  <si>
+    <t>U1 Port</t>
+  </si>
+  <si>
+    <t>U1 Signal</t>
+  </si>
+  <si>
+    <t>U2 Package Pin</t>
+  </si>
+  <si>
+    <t>U2 Port</t>
+  </si>
+  <si>
+    <t>U2 Signal</t>
+  </si>
+  <si>
+    <t>U3 Package Pin</t>
+  </si>
+  <si>
+    <t>U3 Port</t>
+  </si>
+  <si>
+    <t>U3 Signal</t>
+  </si>
+  <si>
+    <t>U4 Package Pin</t>
+  </si>
+  <si>
+    <t>U4 Port</t>
+  </si>
+  <si>
+    <t>U4 Signal</t>
+  </si>
+  <si>
+    <t>XLB0i</t>
+  </si>
+  <si>
+    <t>XLB1i</t>
+  </si>
+  <si>
+    <t>XLB0o</t>
+  </si>
+  <si>
+    <t>XLB1o</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>XLC1o</t>
+  </si>
+  <si>
+    <t>XLC0o</t>
+  </si>
+  <si>
+    <t>XLC0i</t>
+  </si>
+  <si>
+    <t>XLC1i</t>
+  </si>
+  <si>
+    <t>P4A0</t>
+  </si>
+  <si>
+    <t>P4A1</t>
+  </si>
+  <si>
+    <t>P4B0</t>
+  </si>
+  <si>
+    <t>P4B1</t>
+  </si>
+  <si>
+    <t>P4B2</t>
+  </si>
+  <si>
+    <t>P4B3</t>
+  </si>
+  <si>
+    <t>P4A2</t>
+  </si>
+  <si>
+    <t>P4A3</t>
+  </si>
+  <si>
+    <t>P4F0</t>
+  </si>
+  <si>
+    <t>P4F1</t>
+  </si>
+  <si>
+    <t>P4F2</t>
+  </si>
+  <si>
+    <t>P4F3</t>
+  </si>
+  <si>
+    <t>P4E2</t>
+  </si>
+  <si>
+    <t>P4E3</t>
+  </si>
+  <si>
+    <t>P4E0</t>
+  </si>
+  <si>
+    <t>P4E1</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>P32A0</t>
+  </si>
+  <si>
+    <t>P32A1</t>
+  </si>
+  <si>
+    <t>P32A2</t>
+  </si>
+  <si>
+    <t>XLD1o</t>
+  </si>
+  <si>
+    <t>XLD0o</t>
+  </si>
+  <si>
+    <t>XLD0i</t>
+  </si>
+  <si>
+    <t>XLD1i</t>
+  </si>
+  <si>
+    <t>P32A7</t>
+  </si>
+  <si>
+    <t>P32A8</t>
+  </si>
+  <si>
+    <t>P32A9</t>
+  </si>
+  <si>
+    <t>P32A10</t>
+  </si>
+  <si>
+    <t>P32A11</t>
+  </si>
+  <si>
+    <t>P32A12</t>
+  </si>
+  <si>
+    <t>P32A17</t>
+  </si>
+  <si>
+    <t>P32A18</t>
+  </si>
+  <si>
+    <t>P32A19</t>
   </si>
 </sst>
 </file>
@@ -1737,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4003,4 +4361,1362 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D1" t="s">
+        <v>527</v>
+      </c>
+      <c r="F1" t="s">
+        <v>528</v>
+      </c>
+      <c r="G1" t="s">
+        <v>529</v>
+      </c>
+      <c r="H1" t="s">
+        <v>530</v>
+      </c>
+      <c r="J1" t="s">
+        <v>531</v>
+      </c>
+      <c r="K1" t="s">
+        <v>532</v>
+      </c>
+      <c r="L1" t="s">
+        <v>533</v>
+      </c>
+      <c r="N1" t="s">
+        <v>534</v>
+      </c>
+      <c r="O1" t="s">
+        <v>535</v>
+      </c>
+      <c r="P1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B3">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>466</v>
+      </c>
+      <c r="B7">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>467</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>468</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>470</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>93</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>472</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>94</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>473</v>
+      </c>
+      <c r="B14">
+        <v>128</v>
+      </c>
+      <c r="C14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>95</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>95</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>474</v>
+      </c>
+      <c r="B15">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15">
+        <v>48</v>
+      </c>
+      <c r="G15" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15">
+        <v>48</v>
+      </c>
+      <c r="K15" t="s">
+        <v>96</v>
+      </c>
+      <c r="N15">
+        <v>48</v>
+      </c>
+      <c r="O15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>475</v>
+      </c>
+      <c r="B16">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>377</v>
+      </c>
+      <c r="F16">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>377</v>
+      </c>
+      <c r="J16">
+        <v>46</v>
+      </c>
+      <c r="K16" t="s">
+        <v>377</v>
+      </c>
+      <c r="N16">
+        <v>46</v>
+      </c>
+      <c r="O16" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>476</v>
+      </c>
+      <c r="B17">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>378</v>
+      </c>
+      <c r="F17">
+        <v>45</v>
+      </c>
+      <c r="G17" t="s">
+        <v>378</v>
+      </c>
+      <c r="J17">
+        <v>45</v>
+      </c>
+      <c r="K17" t="s">
+        <v>378</v>
+      </c>
+      <c r="N17">
+        <v>45</v>
+      </c>
+      <c r="O17" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>477</v>
+      </c>
+      <c r="B18">
+        <v>113</v>
+      </c>
+      <c r="C18" t="s">
+        <v>540</v>
+      </c>
+      <c r="F18">
+        <v>44</v>
+      </c>
+      <c r="G18" t="s">
+        <v>540</v>
+      </c>
+      <c r="J18">
+        <v>44</v>
+      </c>
+      <c r="K18" t="s">
+        <v>540</v>
+      </c>
+      <c r="N18">
+        <v>44</v>
+      </c>
+      <c r="O18" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>478</v>
+      </c>
+      <c r="B19">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>539</v>
+      </c>
+      <c r="F19">
+        <v>43</v>
+      </c>
+      <c r="G19" t="s">
+        <v>539</v>
+      </c>
+      <c r="J19">
+        <v>43</v>
+      </c>
+      <c r="K19" t="s">
+        <v>539</v>
+      </c>
+      <c r="N19">
+        <v>43</v>
+      </c>
+      <c r="O19" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>479</v>
+      </c>
+      <c r="B20">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>537</v>
+      </c>
+      <c r="F20">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>537</v>
+      </c>
+      <c r="J20">
+        <v>42</v>
+      </c>
+      <c r="K20" t="s">
+        <v>537</v>
+      </c>
+      <c r="N20">
+        <v>42</v>
+      </c>
+      <c r="O20" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>480</v>
+      </c>
+      <c r="B21">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>538</v>
+      </c>
+      <c r="F21">
+        <v>41</v>
+      </c>
+      <c r="G21" t="s">
+        <v>538</v>
+      </c>
+      <c r="J21">
+        <v>41</v>
+      </c>
+      <c r="K21" t="s">
+        <v>538</v>
+      </c>
+      <c r="N21">
+        <v>41</v>
+      </c>
+      <c r="O21" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>481</v>
+      </c>
+      <c r="B22">
+        <v>96</v>
+      </c>
+      <c r="C22" t="s">
+        <v>383</v>
+      </c>
+      <c r="F22">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>383</v>
+      </c>
+      <c r="J22">
+        <v>39</v>
+      </c>
+      <c r="K22" t="s">
+        <v>383</v>
+      </c>
+      <c r="N22">
+        <v>39</v>
+      </c>
+      <c r="O22" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>482</v>
+      </c>
+      <c r="B23">
+        <v>90</v>
+      </c>
+      <c r="C23" t="s">
+        <v>384</v>
+      </c>
+      <c r="F23">
+        <v>38</v>
+      </c>
+      <c r="G23" t="s">
+        <v>384</v>
+      </c>
+      <c r="J23">
+        <v>38</v>
+      </c>
+      <c r="K23" t="s">
+        <v>384</v>
+      </c>
+      <c r="N23">
+        <v>38</v>
+      </c>
+      <c r="O23" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>483</v>
+      </c>
+      <c r="B24">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24">
+        <v>37</v>
+      </c>
+      <c r="G24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24">
+        <v>37</v>
+      </c>
+      <c r="K24" t="s">
+        <v>97</v>
+      </c>
+      <c r="N24">
+        <v>37</v>
+      </c>
+      <c r="O24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>484</v>
+      </c>
+      <c r="B25">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25">
+        <v>36</v>
+      </c>
+      <c r="G25" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25">
+        <v>36</v>
+      </c>
+      <c r="K25" t="s">
+        <v>98</v>
+      </c>
+      <c r="N25">
+        <v>36</v>
+      </c>
+      <c r="O25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>485</v>
+      </c>
+      <c r="B26">
+        <v>87</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26">
+        <v>35</v>
+      </c>
+      <c r="G26" t="s">
+        <v>99</v>
+      </c>
+      <c r="J26">
+        <v>35</v>
+      </c>
+      <c r="K26" t="s">
+        <v>99</v>
+      </c>
+      <c r="N26">
+        <v>35</v>
+      </c>
+      <c r="O26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>486</v>
+      </c>
+      <c r="B27">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>34</v>
+      </c>
+      <c r="G27" t="s">
+        <v>100</v>
+      </c>
+      <c r="J27">
+        <v>34</v>
+      </c>
+      <c r="K27" t="s">
+        <v>100</v>
+      </c>
+      <c r="N27">
+        <v>34</v>
+      </c>
+      <c r="O27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>487</v>
+      </c>
+      <c r="B28">
+        <v>85</v>
+      </c>
+      <c r="C28" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>488</v>
+      </c>
+      <c r="B29">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>489</v>
+      </c>
+      <c r="B30">
+        <v>109</v>
+      </c>
+      <c r="C30" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>490</v>
+      </c>
+      <c r="B31">
+        <v>105</v>
+      </c>
+      <c r="C31" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>491</v>
+      </c>
+      <c r="B32">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>492</v>
+      </c>
+      <c r="B33">
+        <v>102</v>
+      </c>
+      <c r="C33" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>493</v>
+      </c>
+      <c r="B34">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>494</v>
+      </c>
+      <c r="B35">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>495</v>
+      </c>
+      <c r="B36">
+        <v>69</v>
+      </c>
+      <c r="C36" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36">
+        <v>27</v>
+      </c>
+      <c r="G36" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36">
+        <v>27</v>
+      </c>
+      <c r="K36" t="s">
+        <v>101</v>
+      </c>
+      <c r="N36">
+        <v>27</v>
+      </c>
+      <c r="O36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>496</v>
+      </c>
+      <c r="B37">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>217</v>
+      </c>
+      <c r="F37">
+        <v>26</v>
+      </c>
+      <c r="G37" t="s">
+        <v>217</v>
+      </c>
+      <c r="J37">
+        <v>26</v>
+      </c>
+      <c r="K37" t="s">
+        <v>217</v>
+      </c>
+      <c r="N37">
+        <v>26</v>
+      </c>
+      <c r="O37" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>497</v>
+      </c>
+      <c r="B38">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>365</v>
+      </c>
+      <c r="F38">
+        <v>32</v>
+      </c>
+      <c r="G38" t="s">
+        <v>365</v>
+      </c>
+      <c r="J38">
+        <v>32</v>
+      </c>
+      <c r="K38" t="s">
+        <v>365</v>
+      </c>
+      <c r="N38">
+        <v>32</v>
+      </c>
+      <c r="O38" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>498</v>
+      </c>
+      <c r="B39">
+        <v>81</v>
+      </c>
+      <c r="C39" t="s">
+        <v>366</v>
+      </c>
+      <c r="F39">
+        <v>31</v>
+      </c>
+      <c r="G39" t="s">
+        <v>366</v>
+      </c>
+      <c r="J39">
+        <v>31</v>
+      </c>
+      <c r="K39" t="s">
+        <v>366</v>
+      </c>
+      <c r="N39">
+        <v>31</v>
+      </c>
+      <c r="O39" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>499</v>
+      </c>
+      <c r="B40">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>541</v>
+      </c>
+      <c r="F40">
+        <v>29</v>
+      </c>
+      <c r="G40" t="s">
+        <v>541</v>
+      </c>
+      <c r="J40">
+        <v>29</v>
+      </c>
+      <c r="K40" t="s">
+        <v>541</v>
+      </c>
+      <c r="N40">
+        <v>29</v>
+      </c>
+      <c r="O40" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>500</v>
+      </c>
+      <c r="B41">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>368</v>
+      </c>
+      <c r="F41">
+        <v>28</v>
+      </c>
+      <c r="G41" t="s">
+        <v>368</v>
+      </c>
+      <c r="J41">
+        <v>28</v>
+      </c>
+      <c r="K41" t="s">
+        <v>368</v>
+      </c>
+      <c r="N41">
+        <v>28</v>
+      </c>
+      <c r="O41" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>501</v>
+      </c>
+      <c r="B42">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>213</v>
+      </c>
+      <c r="D42" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>502</v>
+      </c>
+      <c r="B43">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
+        <v>214</v>
+      </c>
+      <c r="D43" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>503</v>
+      </c>
+      <c r="B44">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s">
+        <v>215</v>
+      </c>
+      <c r="D44" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>504</v>
+      </c>
+      <c r="B45">
+        <v>95</v>
+      </c>
+      <c r="C45" t="s">
+        <v>216</v>
+      </c>
+      <c r="D45" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>505</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>563</v>
+      </c>
+      <c r="D46" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>506</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>564</v>
+      </c>
+      <c r="D47" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>507</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>565</v>
+      </c>
+      <c r="D48" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>508</v>
+      </c>
+      <c r="B49">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
+        <v>542</v>
+      </c>
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="G49" t="s">
+        <v>542</v>
+      </c>
+      <c r="H49" t="s">
+        <v>562</v>
+      </c>
+      <c r="J49">
+        <v>4</v>
+      </c>
+      <c r="K49" t="s">
+        <v>542</v>
+      </c>
+      <c r="L49" t="s">
+        <v>562</v>
+      </c>
+      <c r="N49">
+        <v>4</v>
+      </c>
+      <c r="O49" t="s">
+        <v>542</v>
+      </c>
+      <c r="P49" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>509</v>
+      </c>
+      <c r="B50">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>543</v>
+      </c>
+      <c r="F50">
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>543</v>
+      </c>
+      <c r="H50" t="s">
+        <v>562</v>
+      </c>
+      <c r="J50">
+        <v>5</v>
+      </c>
+      <c r="K50" t="s">
+        <v>543</v>
+      </c>
+      <c r="L50" t="s">
+        <v>562</v>
+      </c>
+      <c r="N50">
+        <v>5</v>
+      </c>
+      <c r="O50" t="s">
+        <v>543</v>
+      </c>
+      <c r="P50" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>510</v>
+      </c>
+      <c r="B51">
+        <v>13</v>
+      </c>
+      <c r="C51" t="s">
+        <v>544</v>
+      </c>
+      <c r="F51">
+        <v>6</v>
+      </c>
+      <c r="G51" t="s">
+        <v>544</v>
+      </c>
+      <c r="H51" t="s">
+        <v>562</v>
+      </c>
+      <c r="J51">
+        <v>6</v>
+      </c>
+      <c r="K51" t="s">
+        <v>544</v>
+      </c>
+      <c r="L51" t="s">
+        <v>562</v>
+      </c>
+      <c r="N51">
+        <v>6</v>
+      </c>
+      <c r="O51" t="s">
+        <v>544</v>
+      </c>
+      <c r="P51" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>511</v>
+      </c>
+      <c r="B52">
+        <v>31</v>
+      </c>
+      <c r="C52" t="s">
+        <v>545</v>
+      </c>
+      <c r="F52">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>545</v>
+      </c>
+      <c r="H52" t="s">
+        <v>562</v>
+      </c>
+      <c r="J52">
+        <v>11</v>
+      </c>
+      <c r="K52" t="s">
+        <v>545</v>
+      </c>
+      <c r="L52" t="s">
+        <v>562</v>
+      </c>
+      <c r="N52">
+        <v>11</v>
+      </c>
+      <c r="O52" t="s">
+        <v>545</v>
+      </c>
+      <c r="P52" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>512</v>
+      </c>
+      <c r="B53">
+        <v>33</v>
+      </c>
+      <c r="C53" t="s">
+        <v>570</v>
+      </c>
+      <c r="D53" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>513</v>
+      </c>
+      <c r="B54">
+        <v>35</v>
+      </c>
+      <c r="C54" t="s">
+        <v>571</v>
+      </c>
+      <c r="D54" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>514</v>
+      </c>
+      <c r="B55">
+        <v>38</v>
+      </c>
+      <c r="C55" t="s">
+        <v>572</v>
+      </c>
+      <c r="D55" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>515</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>573</v>
+      </c>
+      <c r="D56" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>516</v>
+      </c>
+      <c r="B57">
+        <v>127</v>
+      </c>
+      <c r="C57" t="s">
+        <v>574</v>
+      </c>
+      <c r="D57" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>517</v>
+      </c>
+      <c r="B58">
+        <v>125</v>
+      </c>
+      <c r="C58" t="s">
+        <v>575</v>
+      </c>
+      <c r="D58" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>518</v>
+      </c>
+      <c r="B59">
+        <v>124</v>
+      </c>
+      <c r="C59" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>519</v>
+      </c>
+      <c r="B60">
+        <v>122</v>
+      </c>
+      <c r="C60" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>520</v>
+      </c>
+      <c r="B61">
+        <v>121</v>
+      </c>
+      <c r="C61" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>521</v>
+      </c>
+      <c r="B62">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>522</v>
+      </c>
+      <c r="B63">
+        <v>117</v>
+      </c>
+      <c r="C63" t="s">
+        <v>576</v>
+      </c>
+      <c r="D63" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>523</v>
+      </c>
+      <c r="B64">
+        <v>114</v>
+      </c>
+      <c r="C64" t="s">
+        <v>577</v>
+      </c>
+      <c r="D64" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>524</v>
+      </c>
+      <c r="B65">
+        <v>112</v>
+      </c>
+      <c r="C65" t="s">
+        <v>578</v>
+      </c>
+      <c r="D65" t="s">
+        <v>562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
U1 signal names set.
In setting the signal names, the XMOS Link connections have been made.
Relative orientation of each processor IC has been set.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="591">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1755,6 +1755,42 @@
   </si>
   <si>
     <t>P32A19</t>
+  </si>
+  <si>
+    <t>U2_XLB1i</t>
+  </si>
+  <si>
+    <t>U2_XLB0i</t>
+  </si>
+  <si>
+    <t>U2_XLB0o</t>
+  </si>
+  <si>
+    <t>U2_XLB1o</t>
+  </si>
+  <si>
+    <t>U3_XLB1i</t>
+  </si>
+  <si>
+    <t>U3_XLB0i</t>
+  </si>
+  <si>
+    <t>U3_XLB0o</t>
+  </si>
+  <si>
+    <t>U3_XLB1o</t>
+  </si>
+  <si>
+    <t>U4_XLB1i</t>
+  </si>
+  <si>
+    <t>U4_XLB0i</t>
+  </si>
+  <si>
+    <t>U4_XLB0o</t>
+  </si>
+  <si>
+    <t>U4_XLB1o</t>
   </si>
 </sst>
 </file>
@@ -4367,8 +4403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4377,6 +4413,7 @@
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" customWidth="1"/>
@@ -4754,6 +4791,9 @@
       <c r="C18" t="s">
         <v>540</v>
       </c>
+      <c r="D18" t="s">
+        <v>579</v>
+      </c>
       <c r="F18">
         <v>44</v>
       </c>
@@ -4783,6 +4823,9 @@
       <c r="C19" t="s">
         <v>539</v>
       </c>
+      <c r="D19" t="s">
+        <v>580</v>
+      </c>
       <c r="F19">
         <v>43</v>
       </c>
@@ -4812,6 +4855,9 @@
       <c r="C20" t="s">
         <v>537</v>
       </c>
+      <c r="D20" t="s">
+        <v>581</v>
+      </c>
       <c r="F20">
         <v>42</v>
       </c>
@@ -4841,6 +4887,9 @@
       <c r="C21" t="s">
         <v>538</v>
       </c>
+      <c r="D21" t="s">
+        <v>582</v>
+      </c>
       <c r="F21">
         <v>41</v>
       </c>
@@ -5404,6 +5453,9 @@
       <c r="C49" t="s">
         <v>542</v>
       </c>
+      <c r="D49" t="s">
+        <v>583</v>
+      </c>
       <c r="F49">
         <v>4</v>
       </c>
@@ -5442,6 +5494,9 @@
       <c r="C50" t="s">
         <v>543</v>
       </c>
+      <c r="D50" t="s">
+        <v>584</v>
+      </c>
       <c r="F50">
         <v>5</v>
       </c>
@@ -5480,6 +5535,9 @@
       <c r="C51" t="s">
         <v>544</v>
       </c>
+      <c r="D51" t="s">
+        <v>585</v>
+      </c>
       <c r="F51">
         <v>6</v>
       </c>
@@ -5518,6 +5576,9 @@
       <c r="C52" t="s">
         <v>545</v>
       </c>
+      <c r="D52" t="s">
+        <v>586</v>
+      </c>
       <c r="F52">
         <v>11</v>
       </c>
@@ -5640,6 +5701,9 @@
       <c r="C59" t="s">
         <v>566</v>
       </c>
+      <c r="D59" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -5651,6 +5715,9 @@
       <c r="C60" t="s">
         <v>567</v>
       </c>
+      <c r="D60" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -5662,6 +5729,9 @@
       <c r="C61" t="s">
         <v>568</v>
       </c>
+      <c r="D61" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -5672,6 +5742,9 @@
       </c>
       <c r="C62" t="s">
         <v>569</v>
+      </c>
+      <c r="D62" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
SPI signals connected to U1.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="591">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -4403,8 +4403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4471,6 +4471,9 @@
       <c r="C2" t="s">
         <v>91</v>
       </c>
+      <c r="D2" t="s">
+        <v>412</v>
+      </c>
       <c r="F2">
         <v>13</v>
       </c>
@@ -4500,6 +4503,9 @@
       <c r="C3" t="s">
         <v>92</v>
       </c>
+      <c r="D3" t="s">
+        <v>225</v>
+      </c>
       <c r="F3">
         <v>12</v>
       </c>
@@ -4617,6 +4623,9 @@
       <c r="C12" t="s">
         <v>93</v>
       </c>
+      <c r="D12" t="s">
+        <v>414</v>
+      </c>
       <c r="F12">
         <v>3</v>
       </c>
@@ -4645,6 +4654,9 @@
       </c>
       <c r="C13" t="s">
         <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>413</v>
       </c>
       <c r="F13">
         <v>2</v>

</xml_diff>

<commit_message>
Added a tab to help plan XCore division of labor.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Arduino Connections" sheetId="3" r:id="rId3"/>
     <sheet name="I2C" sheetId="4" r:id="rId4"/>
     <sheet name="XMOS Multichip" sheetId="5" r:id="rId5"/>
+    <sheet name="XMOS Multichip Planning" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="609">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1791,6 +1792,60 @@
   </si>
   <si>
     <t>U4_XLB1o</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>1-bit ports</t>
+  </si>
+  <si>
+    <t>Xcore</t>
+  </si>
+  <si>
+    <t>Pmod 0</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Pmod 1</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Pmod 2</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>and a P4C</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>Enc</t>
+  </si>
+  <si>
+    <t>STM32 UART</t>
+  </si>
+  <si>
+    <t>Xbee UART</t>
+  </si>
+  <si>
+    <t>2 free for RTS/CTS</t>
   </si>
 </sst>
 </file>
@@ -4403,7 +4458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -5804,4 +5859,150 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>591</v>
+      </c>
+      <c r="B1" t="s">
+        <v>592</v>
+      </c>
+      <c r="D1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>596</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>601</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>602</v>
+      </c>
+      <c r="D7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>604</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>605</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>606</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>607</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>608</v>
+      </c>
+      <c r="D11" t="s">
+        <v>603</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
JP3 signals connected to U3.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="612">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1846,6 +1846,15 @@
   </si>
   <si>
     <t>2 free for RTS/CTS</t>
+  </si>
+  <si>
+    <t>JP3_9</t>
+  </si>
+  <si>
+    <t>JP3_10</t>
+  </si>
+  <si>
+    <t>JP3_8</t>
   </si>
 </sst>
 </file>
@@ -2186,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4458,8 +4467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26:M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5114,6 +5123,9 @@
       <c r="K26" t="s">
         <v>99</v>
       </c>
+      <c r="L26" t="s">
+        <v>186</v>
+      </c>
       <c r="N26">
         <v>35</v>
       </c>
@@ -5143,6 +5155,9 @@
       <c r="K27" t="s">
         <v>100</v>
       </c>
+      <c r="L27" t="s">
+        <v>187</v>
+      </c>
       <c r="N27">
         <v>34</v>
       </c>
@@ -5260,6 +5275,9 @@
       <c r="K36" t="s">
         <v>101</v>
       </c>
+      <c r="L36" t="s">
+        <v>609</v>
+      </c>
       <c r="N36">
         <v>27</v>
       </c>
@@ -5289,6 +5307,9 @@
       <c r="K37" t="s">
         <v>217</v>
       </c>
+      <c r="L37" t="s">
+        <v>610</v>
+      </c>
       <c r="N37">
         <v>26</v>
       </c>
@@ -5318,6 +5339,9 @@
       <c r="K38" t="s">
         <v>365</v>
       </c>
+      <c r="L38" t="s">
+        <v>188</v>
+      </c>
       <c r="N38">
         <v>32</v>
       </c>
@@ -5347,6 +5371,9 @@
       <c r="K39" t="s">
         <v>366</v>
       </c>
+      <c r="L39" t="s">
+        <v>189</v>
+      </c>
       <c r="N39">
         <v>31</v>
       </c>
@@ -5376,6 +5403,9 @@
       <c r="K40" t="s">
         <v>541</v>
       </c>
+      <c r="L40" t="s">
+        <v>192</v>
+      </c>
       <c r="N40">
         <v>29</v>
       </c>
@@ -5404,6 +5434,9 @@
       </c>
       <c r="K41" t="s">
         <v>368</v>
+      </c>
+      <c r="L41" t="s">
+        <v>611</v>
       </c>
       <c r="N41">
         <v>28</v>
@@ -5865,8 +5898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
JP13 signals connected to U3.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="612">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -4467,8 +4467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26:M41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4582,6 +4582,9 @@
       <c r="K3" t="s">
         <v>92</v>
       </c>
+      <c r="L3" t="s">
+        <v>405</v>
+      </c>
       <c r="N3">
         <v>12</v>
       </c>
@@ -4702,6 +4705,9 @@
       <c r="K12" t="s">
         <v>93</v>
       </c>
+      <c r="L12" t="s">
+        <v>407</v>
+      </c>
       <c r="N12">
         <v>3</v>
       </c>
@@ -4734,6 +4740,9 @@
       <c r="K13" t="s">
         <v>94</v>
       </c>
+      <c r="L13" t="s">
+        <v>409</v>
+      </c>
       <c r="N13">
         <v>2</v>
       </c>
@@ -4763,6 +4772,9 @@
       <c r="K14" t="s">
         <v>95</v>
       </c>
+      <c r="L14" t="s">
+        <v>410</v>
+      </c>
       <c r="N14">
         <v>1</v>
       </c>
@@ -4792,6 +4804,9 @@
       <c r="K15" t="s">
         <v>96</v>
       </c>
+      <c r="L15" t="s">
+        <v>408</v>
+      </c>
       <c r="N15">
         <v>48</v>
       </c>
@@ -5065,6 +5080,9 @@
       <c r="K24" t="s">
         <v>97</v>
       </c>
+      <c r="L24" t="s">
+        <v>406</v>
+      </c>
       <c r="N24">
         <v>37</v>
       </c>
@@ -5093,6 +5111,9 @@
       </c>
       <c r="K25" t="s">
         <v>98</v>
+      </c>
+      <c r="L25" t="s">
+        <v>404</v>
       </c>
       <c r="N25">
         <v>36</v>

</xml_diff>

<commit_message>
U4 Pmod signals defined.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="626">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1879,6 +1879,24 @@
   </si>
   <si>
     <t>IC7_X</t>
+  </si>
+  <si>
+    <t>JP4_8</t>
+  </si>
+  <si>
+    <t>JP4_9</t>
+  </si>
+  <si>
+    <t>JP4_10</t>
+  </si>
+  <si>
+    <t>JP5_8</t>
+  </si>
+  <si>
+    <t>JP5_9</t>
+  </si>
+  <si>
+    <t>JP5_10</t>
   </si>
 </sst>
 </file>
@@ -4491,8 +4509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4583,6 +4601,9 @@
       <c r="O2" t="s">
         <v>91</v>
       </c>
+      <c r="P2" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4618,6 +4639,9 @@
       <c r="O3" t="s">
         <v>92</v>
       </c>
+      <c r="P3" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4741,6 +4765,9 @@
       <c r="O12" t="s">
         <v>93</v>
       </c>
+      <c r="P12" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -4776,6 +4803,9 @@
       <c r="O13" t="s">
         <v>94</v>
       </c>
+      <c r="P13" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4808,6 +4838,9 @@
       <c r="O14" t="s">
         <v>95</v>
       </c>
+      <c r="P14" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -4840,6 +4873,9 @@
       <c r="O15" t="s">
         <v>96</v>
       </c>
+      <c r="P15" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -4870,7 +4906,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>476</v>
       </c>
@@ -4899,7 +4935,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>477</v>
       </c>
@@ -4931,7 +4967,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>478</v>
       </c>
@@ -4963,7 +4999,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>479</v>
       </c>
@@ -4995,7 +5031,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>480</v>
       </c>
@@ -5027,7 +5063,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>481</v>
       </c>
@@ -5056,7 +5092,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>482</v>
       </c>
@@ -5085,7 +5121,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>483</v>
       </c>
@@ -5116,8 +5152,11 @@
       <c r="O24" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>484</v>
       </c>
@@ -5148,8 +5187,11 @@
       <c r="O25" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>485</v>
       </c>
@@ -5180,8 +5222,11 @@
       <c r="O26" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>486</v>
       </c>
@@ -5212,8 +5257,11 @@
       <c r="O27" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>487</v>
       </c>
@@ -5224,7 +5272,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>488</v>
       </c>
@@ -5235,7 +5283,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>489</v>
       </c>
@@ -5246,7 +5294,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>490</v>
       </c>
@@ -5257,7 +5305,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>491</v>
       </c>
@@ -5268,7 +5316,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>492</v>
       </c>
@@ -5279,7 +5327,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>493</v>
       </c>
@@ -5290,7 +5338,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>494</v>
       </c>
@@ -5301,7 +5349,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>495</v>
       </c>
@@ -5332,8 +5380,11 @@
       <c r="O36" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>496</v>
       </c>
@@ -5364,8 +5415,11 @@
       <c r="O37" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>497</v>
       </c>
@@ -5396,8 +5450,11 @@
       <c r="O38" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>498</v>
       </c>
@@ -5428,8 +5485,11 @@
       <c r="O39" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>499</v>
       </c>
@@ -5460,8 +5520,11 @@
       <c r="O40" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>500</v>
       </c>
@@ -5492,8 +5555,11 @@
       <c r="O41" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>501</v>
       </c>
@@ -5507,7 +5573,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>502</v>
       </c>
@@ -5521,7 +5587,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>503</v>
       </c>
@@ -5535,7 +5601,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>504</v>
       </c>
@@ -5549,7 +5615,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>505</v>
       </c>
@@ -5563,7 +5629,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>506</v>
       </c>
@@ -5577,7 +5643,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>507</v>
       </c>

</xml_diff>

<commit_message>
Servo PWM and microSD slave select signals assigned.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="626">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -2237,7 +2237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -4509,8 +4509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5236,6 +5236,9 @@
       <c r="C27" t="s">
         <v>100</v>
       </c>
+      <c r="D27" t="s">
+        <v>403</v>
+      </c>
       <c r="F27">
         <v>34</v>
       </c>
@@ -5359,6 +5362,9 @@
       <c r="C36" t="s">
         <v>101</v>
       </c>
+      <c r="D36" t="s">
+        <v>398</v>
+      </c>
       <c r="F36">
         <v>27</v>
       </c>
@@ -5394,6 +5400,9 @@
       <c r="C37" t="s">
         <v>217</v>
       </c>
+      <c r="D37" t="s">
+        <v>421</v>
+      </c>
       <c r="F37">
         <v>26</v>
       </c>
@@ -5429,6 +5438,9 @@
       <c r="C38" t="s">
         <v>365</v>
       </c>
+      <c r="D38" t="s">
+        <v>402</v>
+      </c>
       <c r="F38">
         <v>32</v>
       </c>
@@ -5464,6 +5476,9 @@
       <c r="C39" t="s">
         <v>366</v>
       </c>
+      <c r="D39" t="s">
+        <v>401</v>
+      </c>
       <c r="F39">
         <v>31</v>
       </c>
@@ -5499,6 +5514,9 @@
       <c r="C40" t="s">
         <v>541</v>
       </c>
+      <c r="D40" t="s">
+        <v>400</v>
+      </c>
       <c r="F40">
         <v>29</v>
       </c>
@@ -5533,6 +5551,9 @@
       </c>
       <c r="C41" t="s">
         <v>368</v>
+      </c>
+      <c r="D41" t="s">
+        <v>399</v>
       </c>
       <c r="F41">
         <v>28</v>
@@ -6010,10 +6031,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6149,6 +6170,12 @@
         <v>603</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>SUM(B2:B11)</f>
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
U19 and U20 B-side signals assigned.
Net names in the H-bridge circuits have been altered.
Nets named ICx_INy, ICx_DIAGy, etc  which connect to U1
are now the externally-facing nets. The nets connected to
the driver directly are now named based on the name of the
resistor on that pin.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="641">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1897,6 +1897,51 @@
   </si>
   <si>
     <t>JP5_10</t>
+  </si>
+  <si>
+    <t>IC1_DIAGA</t>
+  </si>
+  <si>
+    <t>IC2_DIAGA</t>
+  </si>
+  <si>
+    <t>IC3_DIAGB</t>
+  </si>
+  <si>
+    <t>IC3_DIAGA</t>
+  </si>
+  <si>
+    <t>IC1_INB</t>
+  </si>
+  <si>
+    <t>IC1_INA</t>
+  </si>
+  <si>
+    <t>IC3_INB</t>
+  </si>
+  <si>
+    <t>IC3_INA</t>
+  </si>
+  <si>
+    <t>IC2_INB</t>
+  </si>
+  <si>
+    <t>IC2_INA</t>
+  </si>
+  <si>
+    <t>IC1_PWM</t>
+  </si>
+  <si>
+    <t>IC2_PWM</t>
+  </si>
+  <si>
+    <t>IC3_PWM</t>
+  </si>
+  <si>
+    <t>IC1_DIAGB</t>
+  </si>
+  <si>
+    <t>IC2_DIAGB</t>
   </si>
 </sst>
 </file>
@@ -4509,8 +4554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5073,6 +5118,9 @@
       <c r="C22" t="s">
         <v>383</v>
       </c>
+      <c r="D22" t="s">
+        <v>640</v>
+      </c>
       <c r="F22">
         <v>39</v>
       </c>
@@ -5102,6 +5150,9 @@
       <c r="C23" t="s">
         <v>384</v>
       </c>
+      <c r="D23" t="s">
+        <v>639</v>
+      </c>
       <c r="F23">
         <v>38</v>
       </c>
@@ -5131,6 +5182,9 @@
       <c r="C24" t="s">
         <v>97</v>
       </c>
+      <c r="D24" t="s">
+        <v>638</v>
+      </c>
       <c r="F24">
         <v>37</v>
       </c>
@@ -5166,6 +5220,9 @@
       <c r="C25" t="s">
         <v>98</v>
       </c>
+      <c r="D25" t="s">
+        <v>637</v>
+      </c>
       <c r="F25">
         <v>36</v>
       </c>
@@ -5201,6 +5258,9 @@
       <c r="C26" t="s">
         <v>99</v>
       </c>
+      <c r="D26" t="s">
+        <v>636</v>
+      </c>
       <c r="F26">
         <v>35</v>
       </c>
@@ -5274,6 +5334,9 @@
       <c r="C28" t="s">
         <v>560</v>
       </c>
+      <c r="D28" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -5285,6 +5348,9 @@
       <c r="C29" t="s">
         <v>561</v>
       </c>
+      <c r="D29" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -5318,6 +5384,9 @@
       <c r="C32" t="s">
         <v>556</v>
       </c>
+      <c r="D32" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -5329,6 +5398,9 @@
       <c r="C33" t="s">
         <v>557</v>
       </c>
+      <c r="D33" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -5340,6 +5412,9 @@
       <c r="C34" t="s">
         <v>558</v>
       </c>
+      <c r="D34" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -5351,6 +5426,9 @@
       <c r="C35" t="s">
         <v>559</v>
       </c>
+      <c r="D35" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -5591,7 +5669,7 @@
         <v>213</v>
       </c>
       <c r="D42" t="s">
-        <v>562</v>
+        <v>629</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -5605,7 +5683,7 @@
         <v>214</v>
       </c>
       <c r="D43" t="s">
-        <v>562</v>
+        <v>628</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -5619,7 +5697,7 @@
         <v>215</v>
       </c>
       <c r="D44" t="s">
-        <v>562</v>
+        <v>627</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -5633,7 +5711,7 @@
         <v>216</v>
       </c>
       <c r="D45" t="s">
-        <v>562</v>
+        <v>626</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -6034,7 +6112,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Converted XMOS Multichip workbooks for dual chip.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -11,15 +11,15 @@
     <sheet name="STM32 Connections" sheetId="2" r:id="rId2"/>
     <sheet name="Arduino Connections" sheetId="3" r:id="rId3"/>
     <sheet name="I2C" sheetId="4" r:id="rId4"/>
-    <sheet name="XMOS Multichip" sheetId="5" r:id="rId5"/>
-    <sheet name="XMOS Multichip Planning" sheetId="6" r:id="rId6"/>
+    <sheet name="XMOS Dualchip" sheetId="5" r:id="rId5"/>
+    <sheet name="XMOS Dualchip Planning" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="594">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1536,102 +1536,12 @@
     <t>D43</t>
   </si>
   <si>
-    <t>D49</t>
-  </si>
-  <si>
-    <t>D50</t>
-  </si>
-  <si>
-    <t>D51</t>
-  </si>
-  <si>
-    <t>D52</t>
-  </si>
-  <si>
-    <t>D53</t>
-  </si>
-  <si>
-    <t>D54</t>
-  </si>
-  <si>
-    <t>D55</t>
-  </si>
-  <si>
-    <t>D56</t>
-  </si>
-  <si>
-    <t>D57</t>
-  </si>
-  <si>
-    <t>D58</t>
-  </si>
-  <si>
-    <t>D61</t>
-  </si>
-  <si>
-    <t>D62</t>
-  </si>
-  <si>
-    <t>D63</t>
-  </si>
-  <si>
-    <t>D64</t>
-  </si>
-  <si>
-    <t>D65</t>
-  </si>
-  <si>
-    <t>D66</t>
-  </si>
-  <si>
-    <t>D67</t>
-  </si>
-  <si>
-    <t>D68</t>
-  </si>
-  <si>
-    <t>D69</t>
-  </si>
-  <si>
-    <t>D70</t>
-  </si>
-  <si>
     <t>U1 Package Pin</t>
   </si>
   <si>
-    <t>U1 Port</t>
-  </si>
-  <si>
-    <t>U1 Signal</t>
-  </si>
-  <si>
     <t>U2 Package Pin</t>
   </si>
   <si>
-    <t>U2 Port</t>
-  </si>
-  <si>
-    <t>U2 Signal</t>
-  </si>
-  <si>
-    <t>U3 Package Pin</t>
-  </si>
-  <si>
-    <t>U3 Port</t>
-  </si>
-  <si>
-    <t>U3 Signal</t>
-  </si>
-  <si>
-    <t>U4 Package Pin</t>
-  </si>
-  <si>
-    <t>U4 Port</t>
-  </si>
-  <si>
-    <t>U4 Signal</t>
-  </si>
-  <si>
     <t>XLB0i</t>
   </si>
   <si>
@@ -1647,18 +1557,6 @@
     <t>P10</t>
   </si>
   <si>
-    <t>XLC1o</t>
-  </si>
-  <si>
-    <t>XLC0o</t>
-  </si>
-  <si>
-    <t>XLC0i</t>
-  </si>
-  <si>
-    <t>XLC1i</t>
-  </si>
-  <si>
     <t>P4A0</t>
   </si>
   <si>
@@ -1707,57 +1605,6 @@
     <t>P4E1</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>P32A0</t>
-  </si>
-  <si>
-    <t>P32A1</t>
-  </si>
-  <si>
-    <t>P32A2</t>
-  </si>
-  <si>
-    <t>XLD1o</t>
-  </si>
-  <si>
-    <t>XLD0o</t>
-  </si>
-  <si>
-    <t>XLD0i</t>
-  </si>
-  <si>
-    <t>XLD1i</t>
-  </si>
-  <si>
-    <t>P32A7</t>
-  </si>
-  <si>
-    <t>P32A8</t>
-  </si>
-  <si>
-    <t>P32A9</t>
-  </si>
-  <si>
-    <t>P32A10</t>
-  </si>
-  <si>
-    <t>P32A11</t>
-  </si>
-  <si>
-    <t>P32A12</t>
-  </si>
-  <si>
-    <t>P32A17</t>
-  </si>
-  <si>
-    <t>P32A18</t>
-  </si>
-  <si>
-    <t>P32A19</t>
-  </si>
-  <si>
     <t>U2_XLB1i</t>
   </si>
   <si>
@@ -1770,30 +1617,6 @@
     <t>U2_XLB1o</t>
   </si>
   <si>
-    <t>U3_XLB1i</t>
-  </si>
-  <si>
-    <t>U3_XLB0i</t>
-  </si>
-  <si>
-    <t>U3_XLB0o</t>
-  </si>
-  <si>
-    <t>U3_XLB1o</t>
-  </si>
-  <si>
-    <t>U4_XLB1i</t>
-  </si>
-  <si>
-    <t>U4_XLB0i</t>
-  </si>
-  <si>
-    <t>U4_XLB0o</t>
-  </si>
-  <si>
-    <t>U4_XLB1o</t>
-  </si>
-  <si>
     <t>Block</t>
   </si>
   <si>
@@ -1942,6 +1765,42 @@
   </si>
   <si>
     <t>IC2_DIAGB</t>
+  </si>
+  <si>
+    <t>X1 Port</t>
+  </si>
+  <si>
+    <t>X2 Port</t>
+  </si>
+  <si>
+    <t>X3 Port</t>
+  </si>
+  <si>
+    <t>X2 Signal</t>
+  </si>
+  <si>
+    <t>X3 Signal</t>
+  </si>
+  <si>
+    <t>X0 Signal</t>
+  </si>
+  <si>
+    <t>X1 Signal</t>
+  </si>
+  <si>
+    <t>X0 Port</t>
+  </si>
+  <si>
+    <t>XLA1o</t>
+  </si>
+  <si>
+    <t>XLA0o</t>
+  </si>
+  <si>
+    <t>XLA0i</t>
+  </si>
+  <si>
+    <t>XLA1i</t>
   </si>
 </sst>
 </file>
@@ -4552,10 +4411,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4571,895 +4430,667 @@
     <col min="16" max="16" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>460</v>
       </c>
       <c r="B1" t="s">
-        <v>525</v>
+        <v>505</v>
       </c>
       <c r="C1" t="s">
-        <v>526</v>
+        <v>589</v>
       </c>
       <c r="D1" t="s">
-        <v>527</v>
+        <v>587</v>
       </c>
       <c r="F1" t="s">
-        <v>528</v>
+        <v>505</v>
       </c>
       <c r="G1" t="s">
-        <v>529</v>
+        <v>582</v>
       </c>
       <c r="H1" t="s">
-        <v>530</v>
+        <v>588</v>
       </c>
       <c r="J1" t="s">
-        <v>531</v>
+        <v>506</v>
       </c>
       <c r="K1" t="s">
-        <v>532</v>
+        <v>583</v>
       </c>
       <c r="L1" t="s">
-        <v>533</v>
+        <v>585</v>
       </c>
       <c r="N1" t="s">
-        <v>534</v>
+        <v>506</v>
       </c>
       <c r="O1" t="s">
-        <v>535</v>
+        <v>584</v>
       </c>
       <c r="P1" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>461</v>
       </c>
-      <c r="B2">
-        <v>37</v>
-      </c>
       <c r="C2" t="s">
         <v>91</v>
       </c>
       <c r="D2" t="s">
         <v>412</v>
       </c>
-      <c r="F2">
-        <v>13</v>
-      </c>
       <c r="G2" t="s">
         <v>91</v>
       </c>
-      <c r="J2">
-        <v>13</v>
-      </c>
       <c r="K2" t="s">
         <v>91</v>
       </c>
-      <c r="L2" t="s">
-        <v>613</v>
-      </c>
-      <c r="N2">
-        <v>13</v>
+      <c r="M2" t="s">
+        <v>554</v>
       </c>
       <c r="O2" t="s">
         <v>91</v>
       </c>
-      <c r="P2" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>462</v>
       </c>
-      <c r="B3">
-        <v>36</v>
-      </c>
       <c r="C3" t="s">
         <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>225</v>
       </c>
-      <c r="F3">
-        <v>12</v>
-      </c>
       <c r="G3" t="s">
         <v>92</v>
       </c>
-      <c r="J3">
-        <v>12</v>
-      </c>
       <c r="K3" t="s">
         <v>92</v>
       </c>
-      <c r="L3" t="s">
-        <v>614</v>
-      </c>
-      <c r="N3">
-        <v>12</v>
+      <c r="M3" t="s">
+        <v>555</v>
       </c>
       <c r="O3" t="s">
         <v>92</v>
       </c>
-      <c r="P3" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>463</v>
       </c>
-      <c r="B4">
-        <v>34</v>
-      </c>
       <c r="C4" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>464</v>
       </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
       <c r="C5" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>465</v>
       </c>
-      <c r="B6">
-        <v>28</v>
-      </c>
       <c r="C6" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+      <c r="D6" t="s">
+        <v>590</v>
+      </c>
+      <c r="G6" t="s">
+        <v>590</v>
+      </c>
+      <c r="K6" t="s">
+        <v>590</v>
+      </c>
+      <c r="O6" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>466</v>
       </c>
-      <c r="B7">
-        <v>27</v>
-      </c>
       <c r="C7" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+      <c r="D7" t="s">
+        <v>591</v>
+      </c>
+      <c r="G7" t="s">
+        <v>591</v>
+      </c>
+      <c r="K7" t="s">
+        <v>591</v>
+      </c>
+      <c r="O7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>467</v>
       </c>
-      <c r="B8">
-        <v>16</v>
-      </c>
       <c r="C8" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+      <c r="D8" t="s">
+        <v>592</v>
+      </c>
+      <c r="G8" t="s">
+        <v>592</v>
+      </c>
+      <c r="K8" t="s">
+        <v>592</v>
+      </c>
+      <c r="O8" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>468</v>
       </c>
-      <c r="B9">
-        <v>14</v>
-      </c>
       <c r="C9" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+      <c r="D9" t="s">
+        <v>593</v>
+      </c>
+      <c r="G9" t="s">
+        <v>593</v>
+      </c>
+      <c r="K9" t="s">
+        <v>593</v>
+      </c>
+      <c r="O9" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>469</v>
       </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
       <c r="C10" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>470</v>
       </c>
-      <c r="B11">
-        <v>7</v>
-      </c>
       <c r="C11" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>471</v>
       </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
       <c r="C12" t="s">
         <v>93</v>
       </c>
       <c r="D12" t="s">
         <v>414</v>
       </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
       <c r="G12" t="s">
         <v>93</v>
       </c>
-      <c r="J12">
-        <v>3</v>
-      </c>
       <c r="K12" t="s">
         <v>93</v>
       </c>
-      <c r="L12" t="s">
-        <v>615</v>
-      </c>
-      <c r="N12">
-        <v>3</v>
+      <c r="M12" t="s">
+        <v>556</v>
       </c>
       <c r="O12" t="s">
         <v>93</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>472</v>
       </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
       <c r="C13" t="s">
         <v>94</v>
       </c>
       <c r="D13" t="s">
         <v>413</v>
       </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
       <c r="G13" t="s">
         <v>94</v>
       </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
       <c r="K13" t="s">
         <v>94</v>
       </c>
-      <c r="L13" t="s">
-        <v>617</v>
-      </c>
-      <c r="N13">
-        <v>2</v>
+      <c r="M13" t="s">
+        <v>558</v>
       </c>
       <c r="O13" t="s">
         <v>94</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>473</v>
       </c>
-      <c r="B14">
-        <v>128</v>
-      </c>
       <c r="C14" t="s">
         <v>95</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
       <c r="G14" t="s">
         <v>95</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
       <c r="K14" t="s">
         <v>95</v>
       </c>
-      <c r="L14" t="s">
-        <v>616</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
+      <c r="M14" t="s">
+        <v>557</v>
       </c>
       <c r="O14" t="s">
         <v>95</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>474</v>
       </c>
-      <c r="B15">
-        <v>126</v>
-      </c>
       <c r="C15" t="s">
         <v>96</v>
       </c>
-      <c r="F15">
-        <v>48</v>
-      </c>
       <c r="G15" t="s">
         <v>96</v>
       </c>
-      <c r="J15">
-        <v>48</v>
-      </c>
       <c r="K15" t="s">
         <v>96</v>
       </c>
-      <c r="L15" t="s">
-        <v>618</v>
-      </c>
-      <c r="N15">
-        <v>48</v>
+      <c r="M15" t="s">
+        <v>559</v>
       </c>
       <c r="O15" t="s">
         <v>96</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>475</v>
       </c>
-      <c r="B16">
-        <v>118</v>
-      </c>
       <c r="C16" t="s">
         <v>377</v>
       </c>
-      <c r="F16">
-        <v>46</v>
-      </c>
       <c r="G16" t="s">
         <v>377</v>
       </c>
-      <c r="J16">
-        <v>46</v>
-      </c>
       <c r="K16" t="s">
         <v>377</v>
       </c>
-      <c r="N16">
-        <v>46</v>
-      </c>
       <c r="O16" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>476</v>
       </c>
-      <c r="B17">
-        <v>115</v>
-      </c>
       <c r="C17" t="s">
         <v>378</v>
       </c>
-      <c r="F17">
-        <v>45</v>
-      </c>
       <c r="G17" t="s">
         <v>378</v>
       </c>
-      <c r="J17">
-        <v>45</v>
-      </c>
       <c r="K17" t="s">
         <v>378</v>
       </c>
-      <c r="N17">
-        <v>45</v>
-      </c>
       <c r="O17" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>477</v>
       </c>
-      <c r="B18">
-        <v>113</v>
-      </c>
       <c r="C18" t="s">
-        <v>540</v>
-      </c>
-      <c r="D18" t="s">
-        <v>579</v>
-      </c>
-      <c r="F18">
-        <v>44</v>
+        <v>510</v>
+      </c>
+      <c r="E18" t="s">
+        <v>528</v>
       </c>
       <c r="G18" t="s">
-        <v>540</v>
-      </c>
-      <c r="J18">
-        <v>44</v>
+        <v>510</v>
       </c>
       <c r="K18" t="s">
-        <v>540</v>
-      </c>
-      <c r="N18">
-        <v>44</v>
+        <v>510</v>
       </c>
       <c r="O18" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>478</v>
       </c>
-      <c r="B19">
-        <v>110</v>
-      </c>
       <c r="C19" t="s">
-        <v>539</v>
-      </c>
-      <c r="D19" t="s">
-        <v>580</v>
-      </c>
-      <c r="F19">
-        <v>43</v>
+        <v>509</v>
+      </c>
+      <c r="E19" t="s">
+        <v>529</v>
       </c>
       <c r="G19" t="s">
-        <v>539</v>
-      </c>
-      <c r="J19">
-        <v>43</v>
+        <v>509</v>
       </c>
       <c r="K19" t="s">
-        <v>539</v>
-      </c>
-      <c r="N19">
-        <v>43</v>
+        <v>509</v>
       </c>
       <c r="O19" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>479</v>
       </c>
-      <c r="B20">
-        <v>107</v>
-      </c>
       <c r="C20" t="s">
-        <v>537</v>
-      </c>
-      <c r="D20" t="s">
-        <v>581</v>
-      </c>
-      <c r="F20">
-        <v>42</v>
+        <v>507</v>
+      </c>
+      <c r="E20" t="s">
+        <v>530</v>
       </c>
       <c r="G20" t="s">
-        <v>537</v>
-      </c>
-      <c r="J20">
-        <v>42</v>
+        <v>507</v>
       </c>
       <c r="K20" t="s">
-        <v>537</v>
-      </c>
-      <c r="N20">
-        <v>42</v>
+        <v>507</v>
       </c>
       <c r="O20" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>480</v>
       </c>
-      <c r="B21">
-        <v>106</v>
-      </c>
       <c r="C21" t="s">
-        <v>538</v>
-      </c>
-      <c r="D21" t="s">
-        <v>582</v>
-      </c>
-      <c r="F21">
-        <v>41</v>
+        <v>508</v>
+      </c>
+      <c r="E21" t="s">
+        <v>531</v>
       </c>
       <c r="G21" t="s">
-        <v>538</v>
-      </c>
-      <c r="J21">
-        <v>41</v>
+        <v>508</v>
       </c>
       <c r="K21" t="s">
-        <v>538</v>
-      </c>
-      <c r="N21">
-        <v>41</v>
+        <v>508</v>
       </c>
       <c r="O21" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>481</v>
       </c>
-      <c r="B22">
-        <v>96</v>
-      </c>
       <c r="C22" t="s">
         <v>383</v>
       </c>
-      <c r="D22" t="s">
-        <v>640</v>
-      </c>
-      <c r="F22">
-        <v>39</v>
+      <c r="E22" t="s">
+        <v>581</v>
       </c>
       <c r="G22" t="s">
         <v>383</v>
       </c>
-      <c r="J22">
-        <v>39</v>
-      </c>
       <c r="K22" t="s">
         <v>383</v>
       </c>
-      <c r="N22">
-        <v>39</v>
-      </c>
       <c r="O22" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>482</v>
       </c>
-      <c r="B23">
-        <v>90</v>
-      </c>
       <c r="C23" t="s">
         <v>384</v>
       </c>
-      <c r="D23" t="s">
-        <v>639</v>
-      </c>
-      <c r="F23">
-        <v>38</v>
+      <c r="E23" t="s">
+        <v>580</v>
       </c>
       <c r="G23" t="s">
         <v>384</v>
       </c>
-      <c r="J23">
-        <v>38</v>
-      </c>
       <c r="K23" t="s">
         <v>384</v>
       </c>
-      <c r="N23">
-        <v>38</v>
-      </c>
       <c r="O23" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>483</v>
       </c>
-      <c r="B24">
-        <v>94</v>
-      </c>
       <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="D24" t="s">
-        <v>638</v>
-      </c>
-      <c r="F24">
-        <v>37</v>
+      <c r="E24" t="s">
+        <v>579</v>
       </c>
       <c r="G24" t="s">
         <v>97</v>
       </c>
-      <c r="J24">
-        <v>37</v>
-      </c>
       <c r="K24" t="s">
         <v>97</v>
       </c>
-      <c r="L24" t="s">
-        <v>619</v>
-      </c>
-      <c r="N24">
-        <v>37</v>
+      <c r="M24" t="s">
+        <v>560</v>
       </c>
       <c r="O24" t="s">
         <v>97</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>484</v>
       </c>
-      <c r="B25">
-        <v>89</v>
-      </c>
       <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="D25" t="s">
-        <v>637</v>
-      </c>
-      <c r="F25">
-        <v>36</v>
+      <c r="E25" t="s">
+        <v>578</v>
       </c>
       <c r="G25" t="s">
         <v>98</v>
       </c>
-      <c r="J25">
-        <v>36</v>
-      </c>
       <c r="K25" t="s">
         <v>98</v>
       </c>
-      <c r="L25" t="s">
-        <v>612</v>
-      </c>
-      <c r="N25">
-        <v>36</v>
+      <c r="M25" t="s">
+        <v>553</v>
       </c>
       <c r="O25" t="s">
         <v>98</v>
       </c>
-      <c r="P25" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>485</v>
       </c>
-      <c r="B26">
-        <v>87</v>
-      </c>
       <c r="C26" t="s">
         <v>99</v>
       </c>
-      <c r="D26" t="s">
-        <v>636</v>
-      </c>
-      <c r="F26">
-        <v>35</v>
+      <c r="E26" t="s">
+        <v>577</v>
       </c>
       <c r="G26" t="s">
         <v>99</v>
       </c>
-      <c r="J26">
-        <v>35</v>
-      </c>
       <c r="K26" t="s">
         <v>99</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>186</v>
-      </c>
-      <c r="N26">
-        <v>35</v>
       </c>
       <c r="O26" t="s">
         <v>99</v>
       </c>
-      <c r="P26" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>486</v>
       </c>
-      <c r="B27">
-        <v>86</v>
-      </c>
       <c r="C27" t="s">
         <v>100</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>403</v>
-      </c>
-      <c r="F27">
-        <v>34</v>
       </c>
       <c r="G27" t="s">
         <v>100</v>
       </c>
-      <c r="J27">
-        <v>34</v>
-      </c>
       <c r="K27" t="s">
         <v>100</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>187</v>
-      </c>
-      <c r="N27">
-        <v>34</v>
       </c>
       <c r="O27" t="s">
         <v>100</v>
       </c>
-      <c r="P27" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>487</v>
       </c>
-      <c r="B28">
-        <v>85</v>
-      </c>
       <c r="C28" t="s">
-        <v>560</v>
-      </c>
-      <c r="D28" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+      <c r="E28" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>488</v>
       </c>
-      <c r="B29">
-        <v>84</v>
-      </c>
       <c r="C29" t="s">
-        <v>561</v>
-      </c>
-      <c r="D29" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+      <c r="E29" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>489</v>
       </c>
-      <c r="B30">
-        <v>109</v>
-      </c>
       <c r="C30" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>490</v>
       </c>
-      <c r="B31">
-        <v>105</v>
-      </c>
       <c r="C31" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>491</v>
       </c>
-      <c r="B32">
-        <v>104</v>
-      </c>
       <c r="C32" t="s">
-        <v>556</v>
-      </c>
-      <c r="D32" t="s">
-        <v>633</v>
+        <v>522</v>
+      </c>
+      <c r="E32" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>492</v>
       </c>
-      <c r="B33">
-        <v>102</v>
-      </c>
       <c r="C33" t="s">
-        <v>557</v>
-      </c>
-      <c r="D33" t="s">
-        <v>632</v>
+        <v>523</v>
+      </c>
+      <c r="E33" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>493</v>
       </c>
-      <c r="B34">
-        <v>72</v>
-      </c>
       <c r="C34" t="s">
-        <v>558</v>
-      </c>
-      <c r="D34" t="s">
-        <v>631</v>
+        <v>524</v>
+      </c>
+      <c r="E34" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>494</v>
       </c>
-      <c r="B35">
-        <v>70</v>
-      </c>
       <c r="C35" t="s">
-        <v>559</v>
-      </c>
-      <c r="D35" t="s">
-        <v>630</v>
+        <v>525</v>
+      </c>
+      <c r="E35" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>495</v>
       </c>
-      <c r="B36">
-        <v>69</v>
-      </c>
       <c r="C36" t="s">
         <v>101</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>398</v>
-      </c>
-      <c r="F36">
-        <v>27</v>
       </c>
       <c r="G36" t="s">
         <v>101</v>
       </c>
-      <c r="J36">
-        <v>27</v>
-      </c>
       <c r="K36" t="s">
         <v>101</v>
       </c>
       <c r="L36" t="s">
-        <v>609</v>
-      </c>
-      <c r="N36">
-        <v>27</v>
+        <v>550</v>
       </c>
       <c r="O36" t="s">
         <v>101</v>
@@ -5472,70 +5103,46 @@
       <c r="A37" t="s">
         <v>496</v>
       </c>
-      <c r="B37">
-        <v>67</v>
-      </c>
       <c r="C37" t="s">
         <v>217</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>421</v>
-      </c>
-      <c r="F37">
-        <v>26</v>
       </c>
       <c r="G37" t="s">
         <v>217</v>
       </c>
-      <c r="J37">
-        <v>26</v>
-      </c>
       <c r="K37" t="s">
         <v>217</v>
       </c>
       <c r="L37" t="s">
-        <v>610</v>
-      </c>
-      <c r="N37">
-        <v>26</v>
+        <v>551</v>
       </c>
       <c r="O37" t="s">
         <v>217</v>
       </c>
       <c r="P37" t="s">
-        <v>623</v>
+        <v>564</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>497</v>
       </c>
-      <c r="B38">
-        <v>82</v>
-      </c>
       <c r="C38" t="s">
         <v>365</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>402</v>
-      </c>
-      <c r="F38">
-        <v>32</v>
       </c>
       <c r="G38" t="s">
         <v>365</v>
       </c>
-      <c r="J38">
-        <v>32</v>
-      </c>
       <c r="K38" t="s">
         <v>365</v>
       </c>
       <c r="L38" t="s">
         <v>188</v>
-      </c>
-      <c r="N38">
-        <v>32</v>
       </c>
       <c r="O38" t="s">
         <v>365</v>
@@ -5548,32 +5155,20 @@
       <c r="A39" t="s">
         <v>498</v>
       </c>
-      <c r="B39">
-        <v>81</v>
-      </c>
       <c r="C39" t="s">
         <v>366</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>401</v>
-      </c>
-      <c r="F39">
-        <v>31</v>
       </c>
       <c r="G39" t="s">
         <v>366</v>
       </c>
-      <c r="J39">
-        <v>31</v>
-      </c>
       <c r="K39" t="s">
         <v>366</v>
       </c>
       <c r="L39" t="s">
         <v>189</v>
-      </c>
-      <c r="N39">
-        <v>31</v>
       </c>
       <c r="O39" t="s">
         <v>366</v>
@@ -5586,35 +5181,23 @@
       <c r="A40" t="s">
         <v>499</v>
       </c>
-      <c r="B40">
-        <v>76</v>
-      </c>
       <c r="C40" t="s">
-        <v>541</v>
-      </c>
-      <c r="D40" t="s">
+        <v>511</v>
+      </c>
+      <c r="E40" t="s">
         <v>400</v>
       </c>
-      <c r="F40">
-        <v>29</v>
-      </c>
       <c r="G40" t="s">
-        <v>541</v>
-      </c>
-      <c r="J40">
-        <v>29</v>
+        <v>511</v>
       </c>
       <c r="K40" t="s">
-        <v>541</v>
+        <v>511</v>
       </c>
       <c r="L40" t="s">
         <v>192</v>
       </c>
-      <c r="N40">
-        <v>29</v>
-      </c>
       <c r="O40" t="s">
-        <v>541</v>
+        <v>511</v>
       </c>
       <c r="P40" t="s">
         <v>204</v>
@@ -5624,32 +5207,20 @@
       <c r="A41" t="s">
         <v>500</v>
       </c>
-      <c r="B41">
-        <v>75</v>
-      </c>
       <c r="C41" t="s">
         <v>368</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>399</v>
-      </c>
-      <c r="F41">
-        <v>28</v>
       </c>
       <c r="G41" t="s">
         <v>368</v>
       </c>
-      <c r="J41">
-        <v>28</v>
-      </c>
       <c r="K41" t="s">
         <v>368</v>
       </c>
       <c r="L41" t="s">
-        <v>611</v>
-      </c>
-      <c r="N41">
-        <v>28</v>
+        <v>552</v>
       </c>
       <c r="O41" t="s">
         <v>368</v>
@@ -5662,444 +5233,44 @@
       <c r="A42" t="s">
         <v>501</v>
       </c>
-      <c r="B42">
-        <v>100</v>
-      </c>
       <c r="C42" t="s">
         <v>213</v>
       </c>
-      <c r="D42" t="s">
-        <v>629</v>
+      <c r="E42" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>502</v>
       </c>
-      <c r="B43">
-        <v>98</v>
-      </c>
       <c r="C43" t="s">
         <v>214</v>
       </c>
-      <c r="D43" t="s">
-        <v>628</v>
+      <c r="E43" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>503</v>
       </c>
-      <c r="B44">
-        <v>97</v>
-      </c>
       <c r="C44" t="s">
         <v>215</v>
       </c>
-      <c r="D44" t="s">
-        <v>627</v>
+      <c r="E44" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>504</v>
       </c>
-      <c r="B45">
-        <v>95</v>
-      </c>
       <c r="C45" t="s">
         <v>216</v>
       </c>
-      <c r="D45" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>505</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46" t="s">
-        <v>563</v>
-      </c>
-      <c r="D46" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>506</v>
-      </c>
-      <c r="B47">
-        <v>6</v>
-      </c>
-      <c r="C47" t="s">
-        <v>564</v>
-      </c>
-      <c r="D47" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>507</v>
-      </c>
-      <c r="B48">
-        <v>8</v>
-      </c>
-      <c r="C48" t="s">
-        <v>565</v>
-      </c>
-      <c r="D48" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>508</v>
-      </c>
-      <c r="B49">
-        <v>9</v>
-      </c>
-      <c r="C49" t="s">
-        <v>542</v>
-      </c>
-      <c r="D49" t="s">
-        <v>583</v>
-      </c>
-      <c r="F49">
-        <v>4</v>
-      </c>
-      <c r="G49" t="s">
-        <v>542</v>
-      </c>
-      <c r="H49" t="s">
-        <v>562</v>
-      </c>
-      <c r="J49">
-        <v>4</v>
-      </c>
-      <c r="K49" t="s">
-        <v>542</v>
-      </c>
-      <c r="L49" t="s">
-        <v>562</v>
-      </c>
-      <c r="N49">
-        <v>4</v>
-      </c>
-      <c r="O49" t="s">
-        <v>542</v>
-      </c>
-      <c r="P49" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>509</v>
-      </c>
-      <c r="B50">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
-        <v>543</v>
-      </c>
-      <c r="D50" t="s">
-        <v>584</v>
-      </c>
-      <c r="F50">
-        <v>5</v>
-      </c>
-      <c r="G50" t="s">
-        <v>543</v>
-      </c>
-      <c r="H50" t="s">
-        <v>562</v>
-      </c>
-      <c r="J50">
-        <v>5</v>
-      </c>
-      <c r="K50" t="s">
-        <v>543</v>
-      </c>
-      <c r="L50" t="s">
-        <v>562</v>
-      </c>
-      <c r="N50">
-        <v>5</v>
-      </c>
-      <c r="O50" t="s">
-        <v>543</v>
-      </c>
-      <c r="P50" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>510</v>
-      </c>
-      <c r="B51">
-        <v>13</v>
-      </c>
-      <c r="C51" t="s">
-        <v>544</v>
-      </c>
-      <c r="D51" t="s">
-        <v>585</v>
-      </c>
-      <c r="F51">
-        <v>6</v>
-      </c>
-      <c r="G51" t="s">
-        <v>544</v>
-      </c>
-      <c r="H51" t="s">
-        <v>562</v>
-      </c>
-      <c r="J51">
-        <v>6</v>
-      </c>
-      <c r="K51" t="s">
-        <v>544</v>
-      </c>
-      <c r="L51" t="s">
-        <v>562</v>
-      </c>
-      <c r="N51">
-        <v>6</v>
-      </c>
-      <c r="O51" t="s">
-        <v>544</v>
-      </c>
-      <c r="P51" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>511</v>
-      </c>
-      <c r="B52">
-        <v>31</v>
-      </c>
-      <c r="C52" t="s">
-        <v>545</v>
-      </c>
-      <c r="D52" t="s">
-        <v>586</v>
-      </c>
-      <c r="F52">
-        <v>11</v>
-      </c>
-      <c r="G52" t="s">
-        <v>545</v>
-      </c>
-      <c r="H52" t="s">
-        <v>562</v>
-      </c>
-      <c r="J52">
-        <v>11</v>
-      </c>
-      <c r="K52" t="s">
-        <v>545</v>
-      </c>
-      <c r="L52" t="s">
-        <v>562</v>
-      </c>
-      <c r="N52">
-        <v>11</v>
-      </c>
-      <c r="O52" t="s">
-        <v>545</v>
-      </c>
-      <c r="P52" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>512</v>
-      </c>
-      <c r="B53">
-        <v>33</v>
-      </c>
-      <c r="C53" t="s">
-        <v>570</v>
-      </c>
-      <c r="D53" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>513</v>
-      </c>
-      <c r="B54">
-        <v>35</v>
-      </c>
-      <c r="C54" t="s">
-        <v>571</v>
-      </c>
-      <c r="D54" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>514</v>
-      </c>
-      <c r="B55">
-        <v>38</v>
-      </c>
-      <c r="C55" t="s">
-        <v>572</v>
-      </c>
-      <c r="D55" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>515</v>
-      </c>
-      <c r="B56">
-        <v>3</v>
-      </c>
-      <c r="C56" t="s">
-        <v>573</v>
-      </c>
-      <c r="D56" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>516</v>
-      </c>
-      <c r="B57">
-        <v>127</v>
-      </c>
-      <c r="C57" t="s">
-        <v>574</v>
-      </c>
-      <c r="D57" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>517</v>
-      </c>
-      <c r="B58">
-        <v>125</v>
-      </c>
-      <c r="C58" t="s">
-        <v>575</v>
-      </c>
-      <c r="D58" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>518</v>
-      </c>
-      <c r="B59">
-        <v>124</v>
-      </c>
-      <c r="C59" t="s">
-        <v>566</v>
-      </c>
-      <c r="D59" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>519</v>
-      </c>
-      <c r="B60">
-        <v>122</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="E45" t="s">
         <v>567</v>
-      </c>
-      <c r="D60" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>520</v>
-      </c>
-      <c r="B61">
-        <v>121</v>
-      </c>
-      <c r="C61" t="s">
-        <v>568</v>
-      </c>
-      <c r="D61" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>521</v>
-      </c>
-      <c r="B62">
-        <v>119</v>
-      </c>
-      <c r="C62" t="s">
-        <v>569</v>
-      </c>
-      <c r="D62" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>522</v>
-      </c>
-      <c r="B63">
-        <v>117</v>
-      </c>
-      <c r="C63" t="s">
-        <v>576</v>
-      </c>
-      <c r="D63" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>523</v>
-      </c>
-      <c r="B64">
-        <v>114</v>
-      </c>
-      <c r="C64" t="s">
-        <v>577</v>
-      </c>
-      <c r="D64" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>524</v>
-      </c>
-      <c r="B65">
-        <v>112</v>
-      </c>
-      <c r="C65" t="s">
-        <v>578</v>
-      </c>
-      <c r="D65" t="s">
-        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -6123,46 +5294,46 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>591</v>
+        <v>532</v>
       </c>
       <c r="B1" t="s">
-        <v>592</v>
+        <v>533</v>
       </c>
       <c r="D1" t="s">
-        <v>593</v>
+        <v>534</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>594</v>
+        <v>535</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>595</v>
+        <v>536</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>596</v>
+        <v>537</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>597</v>
+        <v>538</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>598</v>
+        <v>539</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>597</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6173,79 +5344,79 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>595</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>599</v>
+        <v>540</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>600</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>601</v>
+        <v>542</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>602</v>
+        <v>543</v>
       </c>
       <c r="D7" t="s">
-        <v>603</v>
+        <v>544</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>604</v>
+        <v>545</v>
       </c>
       <c r="B8">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>600</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>605</v>
+        <v>546</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>603</v>
+        <v>544</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>606</v>
+        <v>547</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>603</v>
+        <v>544</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>607</v>
+        <v>548</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>608</v>
+        <v>549</v>
       </c>
       <c r="D11" t="s">
-        <v>603</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
XMOS chips assigned in planning workbook.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="593">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1623,21 +1623,12 @@
     <t>1-bit ports</t>
   </si>
   <si>
-    <t>Xcore</t>
-  </si>
-  <si>
     <t>Pmod 0</t>
   </si>
   <si>
-    <t>U3</t>
-  </si>
-  <si>
     <t>Pmod 1</t>
   </si>
   <si>
-    <t>U4</t>
-  </si>
-  <si>
     <t>Pmod 2</t>
   </si>
   <si>
@@ -1801,6 +1792,12 @@
   </si>
   <si>
     <t>XLA1i</t>
+  </si>
+  <si>
+    <t>Chip</t>
+  </si>
+  <si>
+    <t>Core</t>
   </si>
 </sst>
 </file>
@@ -4414,7 +4411,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6:O9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4438,37 +4435,37 @@
         <v>505</v>
       </c>
       <c r="C1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="F1" t="s">
         <v>505</v>
       </c>
       <c r="G1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="H1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="J1" t="s">
         <v>506</v>
       </c>
       <c r="K1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="L1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="N1" t="s">
         <v>506</v>
       </c>
       <c r="O1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="P1" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -4488,13 +4485,13 @@
         <v>91</v>
       </c>
       <c r="M2" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="O2" t="s">
         <v>91</v>
       </c>
       <c r="Q2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -4514,13 +4511,13 @@
         <v>92</v>
       </c>
       <c r="M3" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="O3" t="s">
         <v>92</v>
       </c>
       <c r="Q3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4547,16 +4544,16 @@
         <v>514</v>
       </c>
       <c r="D6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="G6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="K6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="O6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4567,16 +4564,16 @@
         <v>515</v>
       </c>
       <c r="D7" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="G7" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="K7" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="O7" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4587,16 +4584,16 @@
         <v>516</v>
       </c>
       <c r="D8" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="G8" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="K8" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="O8" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -4607,16 +4604,16 @@
         <v>517</v>
       </c>
       <c r="D9" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="G9" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="K9" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="O9" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -4652,7 +4649,7 @@
         <v>93</v>
       </c>
       <c r="M12" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="O12" t="s">
         <v>93</v>
@@ -4678,7 +4675,7 @@
         <v>94</v>
       </c>
       <c r="M13" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="O13" t="s">
         <v>94</v>
@@ -4701,7 +4698,7 @@
         <v>95</v>
       </c>
       <c r="M14" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="O14" t="s">
         <v>95</v>
@@ -4724,7 +4721,7 @@
         <v>96</v>
       </c>
       <c r="M15" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="O15" t="s">
         <v>96</v>
@@ -4855,7 +4852,7 @@
         <v>383</v>
       </c>
       <c r="E22" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="G22" t="s">
         <v>383</v>
@@ -4875,7 +4872,7 @@
         <v>384</v>
       </c>
       <c r="E23" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="G23" t="s">
         <v>384</v>
@@ -4895,7 +4892,7 @@
         <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="G24" t="s">
         <v>97</v>
@@ -4904,7 +4901,7 @@
         <v>97</v>
       </c>
       <c r="M24" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="O24" t="s">
         <v>97</v>
@@ -4921,7 +4918,7 @@
         <v>98</v>
       </c>
       <c r="E25" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="G25" t="s">
         <v>98</v>
@@ -4930,13 +4927,13 @@
         <v>98</v>
       </c>
       <c r="M25" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="O25" t="s">
         <v>98</v>
       </c>
       <c r="Q25" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -4947,7 +4944,7 @@
         <v>99</v>
       </c>
       <c r="E26" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="G26" t="s">
         <v>99</v>
@@ -4962,7 +4959,7 @@
         <v>99</v>
       </c>
       <c r="Q26" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -4988,7 +4985,7 @@
         <v>100</v>
       </c>
       <c r="Q27" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -4999,7 +4996,7 @@
         <v>526</v>
       </c>
       <c r="E28" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -5010,7 +5007,7 @@
         <v>527</v>
       </c>
       <c r="E29" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -5037,7 +5034,7 @@
         <v>522</v>
       </c>
       <c r="E32" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -5048,7 +5045,7 @@
         <v>523</v>
       </c>
       <c r="E33" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -5059,7 +5056,7 @@
         <v>524</v>
       </c>
       <c r="E34" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -5070,7 +5067,7 @@
         <v>525</v>
       </c>
       <c r="E35" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -5090,7 +5087,7 @@
         <v>101</v>
       </c>
       <c r="L36" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="O36" t="s">
         <v>101</v>
@@ -5116,13 +5113,13 @@
         <v>217</v>
       </c>
       <c r="L37" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="O37" t="s">
         <v>217</v>
       </c>
       <c r="P37" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -5220,7 +5217,7 @@
         <v>368</v>
       </c>
       <c r="L41" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="O41" t="s">
         <v>368</v>
@@ -5237,7 +5234,7 @@
         <v>213</v>
       </c>
       <c r="E42" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -5248,7 +5245,7 @@
         <v>214</v>
       </c>
       <c r="E43" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -5259,7 +5256,7 @@
         <v>215</v>
       </c>
       <c r="E44" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -5270,7 +5267,7 @@
         <v>216</v>
       </c>
       <c r="E45" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -5280,10 +5277,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5292,7 +5289,7 @@
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>532</v>
       </c>
@@ -5300,43 +5297,46 @@
         <v>533</v>
       </c>
       <c r="D1" t="s">
+        <v>591</v>
+      </c>
+      <c r="E1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>534</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>535</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -5344,82 +5344,82 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D7" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B8">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>544</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>547</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D11" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(B2:B11)</f>
         <v>59</v>

</xml_diff>

<commit_message>
Connecting XBee UART RTS/CTS to XMOS.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -1659,9 +1659,6 @@
     <t>Xbee UART</t>
   </si>
   <si>
-    <t>2 free for RTS/CTS</t>
-  </si>
-  <si>
     <t>JP3_9</t>
   </si>
   <si>
@@ -1798,6 +1795,9 @@
   </si>
   <si>
     <t>Core</t>
+  </si>
+  <si>
+    <t>Include RTS/CTS</t>
   </si>
 </sst>
 </file>
@@ -4410,7 +4410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -4435,37 +4435,37 @@
         <v>505</v>
       </c>
       <c r="C1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F1" t="s">
         <v>505</v>
       </c>
       <c r="G1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J1" t="s">
         <v>506</v>
       </c>
       <c r="K1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="L1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="N1" t="s">
         <v>506</v>
       </c>
       <c r="O1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="P1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -4485,13 +4485,13 @@
         <v>91</v>
       </c>
       <c r="M2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="O2" t="s">
         <v>91</v>
       </c>
       <c r="Q2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -4511,13 +4511,13 @@
         <v>92</v>
       </c>
       <c r="M3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="O3" t="s">
         <v>92</v>
       </c>
       <c r="Q3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4544,16 +4544,16 @@
         <v>514</v>
       </c>
       <c r="D6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="K6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="O6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4564,16 +4564,16 @@
         <v>515</v>
       </c>
       <c r="D7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="K7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="O7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4584,16 +4584,16 @@
         <v>516</v>
       </c>
       <c r="D8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="O8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -4604,16 +4604,16 @@
         <v>517</v>
       </c>
       <c r="D9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="O9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -4649,7 +4649,7 @@
         <v>93</v>
       </c>
       <c r="M12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="O12" t="s">
         <v>93</v>
@@ -4675,7 +4675,7 @@
         <v>94</v>
       </c>
       <c r="M13" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="O13" t="s">
         <v>94</v>
@@ -4698,7 +4698,7 @@
         <v>95</v>
       </c>
       <c r="M14" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="O14" t="s">
         <v>95</v>
@@ -4721,7 +4721,7 @@
         <v>96</v>
       </c>
       <c r="M15" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="O15" t="s">
         <v>96</v>
@@ -4852,7 +4852,7 @@
         <v>383</v>
       </c>
       <c r="E22" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G22" t="s">
         <v>383</v>
@@ -4872,7 +4872,7 @@
         <v>384</v>
       </c>
       <c r="E23" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G23" t="s">
         <v>384</v>
@@ -4892,7 +4892,7 @@
         <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G24" t="s">
         <v>97</v>
@@ -4901,7 +4901,7 @@
         <v>97</v>
       </c>
       <c r="M24" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="O24" t="s">
         <v>97</v>
@@ -4918,7 +4918,7 @@
         <v>98</v>
       </c>
       <c r="E25" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G25" t="s">
         <v>98</v>
@@ -4927,13 +4927,13 @@
         <v>98</v>
       </c>
       <c r="M25" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="O25" t="s">
         <v>98</v>
       </c>
       <c r="Q25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -4944,7 +4944,7 @@
         <v>99</v>
       </c>
       <c r="E26" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G26" t="s">
         <v>99</v>
@@ -4959,7 +4959,7 @@
         <v>99</v>
       </c>
       <c r="Q26" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -4985,7 +4985,7 @@
         <v>100</v>
       </c>
       <c r="Q27" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -4996,7 +4996,7 @@
         <v>526</v>
       </c>
       <c r="E28" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -5007,7 +5007,7 @@
         <v>527</v>
       </c>
       <c r="E29" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -5034,7 +5034,7 @@
         <v>522</v>
       </c>
       <c r="E32" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -5045,7 +5045,7 @@
         <v>523</v>
       </c>
       <c r="E33" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -5056,7 +5056,7 @@
         <v>524</v>
       </c>
       <c r="E34" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -5067,7 +5067,7 @@
         <v>525</v>
       </c>
       <c r="E35" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -5087,7 +5087,7 @@
         <v>101</v>
       </c>
       <c r="L36" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="O36" t="s">
         <v>101</v>
@@ -5113,13 +5113,13 @@
         <v>217</v>
       </c>
       <c r="L37" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="O37" t="s">
         <v>217</v>
       </c>
       <c r="P37" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -5217,7 +5217,7 @@
         <v>368</v>
       </c>
       <c r="L41" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="O41" t="s">
         <v>368</v>
@@ -5234,7 +5234,7 @@
         <v>213</v>
       </c>
       <c r="E42" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -5245,7 +5245,7 @@
         <v>214</v>
       </c>
       <c r="E43" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -5256,7 +5256,7 @@
         <v>215</v>
       </c>
       <c r="E44" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -5267,7 +5267,7 @@
         <v>216</v>
       </c>
       <c r="E45" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
   </sheetData>
@@ -5279,8 +5279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5297,10 +5297,10 @@
         <v>533</v>
       </c>
       <c r="D1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E1" t="s">
         <v>591</v>
-      </c>
-      <c r="E1" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5410,10 +5410,10 @@
         <v>545</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>546</v>
+        <v>592</v>
       </c>
       <c r="D11" t="s">
         <v>538</v>
@@ -5422,7 +5422,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(B2:B11)</f>
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XMOS package pins marked.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="593">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -4410,8 +4410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4472,20 +4472,32 @@
       <c r="A2" t="s">
         <v>461</v>
       </c>
+      <c r="B2" t="s">
+        <v>281</v>
+      </c>
       <c r="C2" t="s">
         <v>91</v>
       </c>
       <c r="D2" t="s">
         <v>412</v>
       </c>
+      <c r="F2" t="s">
+        <v>325</v>
+      </c>
       <c r="G2" t="s">
         <v>91</v>
       </c>
+      <c r="J2" t="s">
+        <v>281</v>
+      </c>
       <c r="K2" t="s">
         <v>91</v>
       </c>
       <c r="M2" t="s">
         <v>550</v>
+      </c>
+      <c r="N2" t="s">
+        <v>325</v>
       </c>
       <c r="O2" t="s">
         <v>91</v>
@@ -4498,20 +4510,32 @@
       <c r="A3" t="s">
         <v>462</v>
       </c>
+      <c r="B3" t="s">
+        <v>282</v>
+      </c>
       <c r="C3" t="s">
         <v>92</v>
       </c>
       <c r="D3" t="s">
         <v>225</v>
       </c>
+      <c r="F3" t="s">
+        <v>326</v>
+      </c>
       <c r="G3" t="s">
         <v>92</v>
       </c>
+      <c r="J3" t="s">
+        <v>282</v>
+      </c>
       <c r="K3" t="s">
         <v>92</v>
       </c>
       <c r="M3" t="s">
         <v>551</v>
+      </c>
+      <c r="N3" t="s">
+        <v>326</v>
       </c>
       <c r="O3" t="s">
         <v>92</v>
@@ -4524,33 +4548,69 @@
       <c r="A4" t="s">
         <v>463</v>
       </c>
+      <c r="B4" t="s">
+        <v>285</v>
+      </c>
       <c r="C4" t="s">
         <v>512</v>
+      </c>
+      <c r="F4" t="s">
+        <v>327</v>
+      </c>
+      <c r="J4" t="s">
+        <v>285</v>
+      </c>
+      <c r="N4" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>464</v>
       </c>
+      <c r="B5" t="s">
+        <v>286</v>
+      </c>
       <c r="C5" t="s">
         <v>513</v>
+      </c>
+      <c r="F5" t="s">
+        <v>328</v>
+      </c>
+      <c r="J5" t="s">
+        <v>286</v>
+      </c>
+      <c r="N5" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>465</v>
       </c>
+      <c r="B6" t="s">
+        <v>287</v>
+      </c>
       <c r="C6" t="s">
         <v>514</v>
       </c>
       <c r="D6" t="s">
         <v>586</v>
       </c>
+      <c r="F6" t="s">
+        <v>329</v>
+      </c>
       <c r="G6" t="s">
         <v>586</v>
       </c>
+      <c r="J6" t="s">
+        <v>287</v>
+      </c>
       <c r="K6" t="s">
         <v>586</v>
+      </c>
+      <c r="N6" t="s">
+        <v>329</v>
       </c>
       <c r="O6" t="s">
         <v>586</v>
@@ -4560,17 +4620,29 @@
       <c r="A7" t="s">
         <v>466</v>
       </c>
+      <c r="B7" t="s">
+        <v>288</v>
+      </c>
       <c r="C7" t="s">
         <v>515</v>
       </c>
       <c r="D7" t="s">
         <v>587</v>
       </c>
+      <c r="F7" t="s">
+        <v>330</v>
+      </c>
       <c r="G7" t="s">
         <v>587</v>
       </c>
+      <c r="J7" t="s">
+        <v>288</v>
+      </c>
       <c r="K7" t="s">
         <v>587</v>
+      </c>
+      <c r="N7" t="s">
+        <v>330</v>
       </c>
       <c r="O7" t="s">
         <v>587</v>
@@ -4580,17 +4652,29 @@
       <c r="A8" t="s">
         <v>467</v>
       </c>
+      <c r="B8" t="s">
+        <v>289</v>
+      </c>
       <c r="C8" t="s">
         <v>516</v>
       </c>
       <c r="D8" t="s">
         <v>588</v>
       </c>
+      <c r="F8" t="s">
+        <v>331</v>
+      </c>
       <c r="G8" t="s">
         <v>588</v>
       </c>
+      <c r="J8" t="s">
+        <v>289</v>
+      </c>
       <c r="K8" t="s">
         <v>588</v>
+      </c>
+      <c r="N8" t="s">
+        <v>331</v>
       </c>
       <c r="O8" t="s">
         <v>588</v>
@@ -4600,17 +4684,29 @@
       <c r="A9" t="s">
         <v>468</v>
       </c>
+      <c r="B9" t="s">
+        <v>290</v>
+      </c>
       <c r="C9" t="s">
         <v>517</v>
       </c>
       <c r="D9" t="s">
         <v>589</v>
       </c>
+      <c r="F9" t="s">
+        <v>332</v>
+      </c>
       <c r="G9" t="s">
         <v>589</v>
       </c>
+      <c r="J9" t="s">
+        <v>290</v>
+      </c>
       <c r="K9" t="s">
         <v>589</v>
+      </c>
+      <c r="N9" t="s">
+        <v>332</v>
       </c>
       <c r="O9" t="s">
         <v>589</v>
@@ -4620,36 +4716,72 @@
       <c r="A10" t="s">
         <v>469</v>
       </c>
+      <c r="B10" t="s">
+        <v>291</v>
+      </c>
       <c r="C10" t="s">
         <v>518</v>
+      </c>
+      <c r="F10" t="s">
+        <v>333</v>
+      </c>
+      <c r="J10" t="s">
+        <v>291</v>
+      </c>
+      <c r="N10" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>470</v>
       </c>
+      <c r="B11" t="s">
+        <v>292</v>
+      </c>
       <c r="C11" t="s">
         <v>519</v>
+      </c>
+      <c r="F11" t="s">
+        <v>334</v>
+      </c>
+      <c r="J11" t="s">
+        <v>292</v>
+      </c>
+      <c r="N11" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>471</v>
       </c>
+      <c r="B12" t="s">
+        <v>283</v>
+      </c>
       <c r="C12" t="s">
         <v>93</v>
       </c>
       <c r="D12" t="s">
         <v>414</v>
       </c>
+      <c r="F12" t="s">
+        <v>335</v>
+      </c>
       <c r="G12" t="s">
         <v>93</v>
       </c>
+      <c r="J12" t="s">
+        <v>283</v>
+      </c>
       <c r="K12" t="s">
         <v>93</v>
       </c>
       <c r="M12" t="s">
         <v>552</v>
+      </c>
+      <c r="N12" t="s">
+        <v>335</v>
       </c>
       <c r="O12" t="s">
         <v>93</v>
@@ -4662,20 +4794,32 @@
       <c r="A13" t="s">
         <v>472</v>
       </c>
+      <c r="B13" t="s">
+        <v>284</v>
+      </c>
       <c r="C13" t="s">
         <v>94</v>
       </c>
       <c r="D13" t="s">
         <v>413</v>
       </c>
+      <c r="F13" t="s">
+        <v>336</v>
+      </c>
       <c r="G13" t="s">
         <v>94</v>
       </c>
+      <c r="J13" t="s">
+        <v>284</v>
+      </c>
       <c r="K13" t="s">
         <v>94</v>
       </c>
       <c r="M13" t="s">
         <v>554</v>
+      </c>
+      <c r="N13" t="s">
+        <v>336</v>
       </c>
       <c r="O13" t="s">
         <v>94</v>
@@ -4688,17 +4832,29 @@
       <c r="A14" t="s">
         <v>473</v>
       </c>
+      <c r="B14" t="s">
+        <v>293</v>
+      </c>
       <c r="C14" t="s">
         <v>95</v>
       </c>
+      <c r="F14" t="s">
+        <v>337</v>
+      </c>
       <c r="G14" t="s">
         <v>95</v>
       </c>
+      <c r="J14" t="s">
+        <v>293</v>
+      </c>
       <c r="K14" t="s">
         <v>95</v>
       </c>
       <c r="M14" t="s">
         <v>553</v>
+      </c>
+      <c r="N14" t="s">
+        <v>337</v>
       </c>
       <c r="O14" t="s">
         <v>95</v>
@@ -4711,17 +4867,29 @@
       <c r="A15" t="s">
         <v>474</v>
       </c>
+      <c r="B15" t="s">
+        <v>294</v>
+      </c>
       <c r="C15" t="s">
         <v>96</v>
       </c>
+      <c r="F15" t="s">
+        <v>341</v>
+      </c>
       <c r="G15" t="s">
         <v>96</v>
       </c>
+      <c r="J15" t="s">
+        <v>294</v>
+      </c>
       <c r="K15" t="s">
         <v>96</v>
       </c>
       <c r="M15" t="s">
         <v>555</v>
+      </c>
+      <c r="N15" t="s">
+        <v>341</v>
       </c>
       <c r="O15" t="s">
         <v>96</v>
@@ -4734,14 +4902,26 @@
       <c r="A16" t="s">
         <v>475</v>
       </c>
+      <c r="B16" t="s">
+        <v>295</v>
+      </c>
       <c r="C16" t="s">
         <v>377</v>
       </c>
+      <c r="F16" t="s">
+        <v>342</v>
+      </c>
       <c r="G16" t="s">
         <v>377</v>
       </c>
+      <c r="J16" t="s">
+        <v>295</v>
+      </c>
       <c r="K16" t="s">
         <v>377</v>
+      </c>
+      <c r="N16" t="s">
+        <v>342</v>
       </c>
       <c r="O16" t="s">
         <v>377</v>
@@ -4751,14 +4931,26 @@
       <c r="A17" t="s">
         <v>476</v>
       </c>
+      <c r="B17" t="s">
+        <v>296</v>
+      </c>
       <c r="C17" t="s">
         <v>378</v>
       </c>
+      <c r="F17" t="s">
+        <v>343</v>
+      </c>
       <c r="G17" t="s">
         <v>378</v>
       </c>
+      <c r="J17" t="s">
+        <v>296</v>
+      </c>
       <c r="K17" t="s">
         <v>378</v>
+      </c>
+      <c r="N17" t="s">
+        <v>343</v>
       </c>
       <c r="O17" t="s">
         <v>378</v>
@@ -4768,17 +4960,29 @@
       <c r="A18" t="s">
         <v>477</v>
       </c>
+      <c r="B18" t="s">
+        <v>297</v>
+      </c>
       <c r="C18" t="s">
         <v>510</v>
       </c>
       <c r="E18" t="s">
         <v>528</v>
       </c>
+      <c r="F18" t="s">
+        <v>344</v>
+      </c>
       <c r="G18" t="s">
         <v>510</v>
       </c>
+      <c r="J18" t="s">
+        <v>297</v>
+      </c>
       <c r="K18" t="s">
         <v>510</v>
+      </c>
+      <c r="N18" t="s">
+        <v>344</v>
       </c>
       <c r="O18" t="s">
         <v>510</v>
@@ -4788,17 +4992,29 @@
       <c r="A19" t="s">
         <v>478</v>
       </c>
+      <c r="B19" t="s">
+        <v>298</v>
+      </c>
       <c r="C19" t="s">
         <v>509</v>
       </c>
       <c r="E19" t="s">
         <v>529</v>
       </c>
+      <c r="F19" t="s">
+        <v>345</v>
+      </c>
       <c r="G19" t="s">
         <v>509</v>
       </c>
+      <c r="J19" t="s">
+        <v>298</v>
+      </c>
       <c r="K19" t="s">
         <v>509</v>
+      </c>
+      <c r="N19" t="s">
+        <v>345</v>
       </c>
       <c r="O19" t="s">
         <v>509</v>
@@ -4808,17 +5024,29 @@
       <c r="A20" t="s">
         <v>479</v>
       </c>
+      <c r="B20" t="s">
+        <v>302</v>
+      </c>
       <c r="C20" t="s">
         <v>507</v>
       </c>
       <c r="E20" t="s">
         <v>530</v>
       </c>
+      <c r="F20" t="s">
+        <v>346</v>
+      </c>
       <c r="G20" t="s">
         <v>507</v>
       </c>
+      <c r="J20" t="s">
+        <v>302</v>
+      </c>
       <c r="K20" t="s">
         <v>507</v>
+      </c>
+      <c r="N20" t="s">
+        <v>346</v>
       </c>
       <c r="O20" t="s">
         <v>507</v>
@@ -4828,17 +5056,29 @@
       <c r="A21" t="s">
         <v>480</v>
       </c>
+      <c r="B21" t="s">
+        <v>303</v>
+      </c>
       <c r="C21" t="s">
         <v>508</v>
       </c>
       <c r="E21" t="s">
         <v>531</v>
       </c>
+      <c r="F21" t="s">
+        <v>347</v>
+      </c>
       <c r="G21" t="s">
         <v>508</v>
       </c>
+      <c r="J21" t="s">
+        <v>303</v>
+      </c>
       <c r="K21" t="s">
         <v>508</v>
+      </c>
+      <c r="N21" t="s">
+        <v>347</v>
       </c>
       <c r="O21" t="s">
         <v>508</v>
@@ -4848,17 +5088,29 @@
       <c r="A22" t="s">
         <v>481</v>
       </c>
+      <c r="B22" t="s">
+        <v>304</v>
+      </c>
       <c r="C22" t="s">
         <v>383</v>
       </c>
       <c r="E22" t="s">
         <v>577</v>
       </c>
+      <c r="F22" t="s">
+        <v>348</v>
+      </c>
       <c r="G22" t="s">
         <v>383</v>
       </c>
+      <c r="J22" t="s">
+        <v>304</v>
+      </c>
       <c r="K22" t="s">
         <v>383</v>
+      </c>
+      <c r="N22" t="s">
+        <v>348</v>
       </c>
       <c r="O22" t="s">
         <v>383</v>
@@ -4868,17 +5120,29 @@
       <c r="A23" t="s">
         <v>482</v>
       </c>
+      <c r="B23" t="s">
+        <v>305</v>
+      </c>
       <c r="C23" t="s">
         <v>384</v>
       </c>
       <c r="E23" t="s">
         <v>576</v>
       </c>
+      <c r="F23" t="s">
+        <v>349</v>
+      </c>
       <c r="G23" t="s">
         <v>384</v>
       </c>
+      <c r="J23" t="s">
+        <v>305</v>
+      </c>
       <c r="K23" t="s">
         <v>384</v>
+      </c>
+      <c r="N23" t="s">
+        <v>349</v>
       </c>
       <c r="O23" t="s">
         <v>384</v>
@@ -4888,20 +5152,32 @@
       <c r="A24" t="s">
         <v>483</v>
       </c>
+      <c r="B24" t="s">
+        <v>301</v>
+      </c>
       <c r="C24" t="s">
         <v>97</v>
       </c>
       <c r="E24" t="s">
         <v>575</v>
       </c>
+      <c r="F24" t="s">
+        <v>339</v>
+      </c>
       <c r="G24" t="s">
         <v>97</v>
       </c>
+      <c r="J24" t="s">
+        <v>301</v>
+      </c>
       <c r="K24" t="s">
         <v>97</v>
       </c>
       <c r="M24" t="s">
         <v>556</v>
+      </c>
+      <c r="N24" t="s">
+        <v>339</v>
       </c>
       <c r="O24" t="s">
         <v>97</v>
@@ -4914,20 +5190,32 @@
       <c r="A25" t="s">
         <v>484</v>
       </c>
+      <c r="B25" t="s">
+        <v>299</v>
+      </c>
       <c r="C25" t="s">
         <v>98</v>
       </c>
       <c r="E25" t="s">
         <v>574</v>
       </c>
+      <c r="F25" t="s">
+        <v>340</v>
+      </c>
       <c r="G25" t="s">
         <v>98</v>
       </c>
+      <c r="J25" t="s">
+        <v>299</v>
+      </c>
       <c r="K25" t="s">
         <v>98</v>
       </c>
       <c r="M25" t="s">
         <v>549</v>
+      </c>
+      <c r="N25" t="s">
+        <v>340</v>
       </c>
       <c r="O25" t="s">
         <v>98</v>
@@ -4940,20 +5228,32 @@
       <c r="A26" t="s">
         <v>485</v>
       </c>
+      <c r="B26" t="s">
+        <v>300</v>
+      </c>
       <c r="C26" t="s">
         <v>99</v>
       </c>
       <c r="E26" t="s">
         <v>573</v>
       </c>
+      <c r="F26" t="s">
+        <v>338</v>
+      </c>
       <c r="G26" t="s">
         <v>99</v>
       </c>
+      <c r="J26" t="s">
+        <v>300</v>
+      </c>
       <c r="K26" t="s">
         <v>99</v>
       </c>
       <c r="M26" t="s">
         <v>186</v>
+      </c>
+      <c r="N26" t="s">
+        <v>338</v>
       </c>
       <c r="O26" t="s">
         <v>99</v>
@@ -4966,20 +5266,32 @@
       <c r="A27" t="s">
         <v>486</v>
       </c>
+      <c r="B27" t="s">
+        <v>306</v>
+      </c>
       <c r="C27" t="s">
         <v>100</v>
       </c>
       <c r="E27" t="s">
         <v>403</v>
       </c>
+      <c r="F27" t="s">
+        <v>350</v>
+      </c>
       <c r="G27" t="s">
         <v>100</v>
       </c>
+      <c r="J27" t="s">
+        <v>306</v>
+      </c>
       <c r="K27" t="s">
         <v>100</v>
       </c>
       <c r="M27" t="s">
         <v>187</v>
+      </c>
+      <c r="N27" t="s">
+        <v>350</v>
       </c>
       <c r="O27" t="s">
         <v>100</v>
@@ -4992,102 +5304,210 @@
       <c r="A28" t="s">
         <v>487</v>
       </c>
+      <c r="B28" t="s">
+        <v>307</v>
+      </c>
       <c r="C28" t="s">
         <v>526</v>
       </c>
       <c r="E28" t="s">
         <v>572</v>
+      </c>
+      <c r="F28" t="s">
+        <v>351</v>
+      </c>
+      <c r="J28" t="s">
+        <v>307</v>
+      </c>
+      <c r="N28" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>488</v>
       </c>
+      <c r="B29" t="s">
+        <v>308</v>
+      </c>
       <c r="C29" t="s">
         <v>527</v>
       </c>
       <c r="E29" t="s">
         <v>571</v>
+      </c>
+      <c r="F29" t="s">
+        <v>352</v>
+      </c>
+      <c r="J29" t="s">
+        <v>308</v>
+      </c>
+      <c r="N29" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>489</v>
       </c>
+      <c r="B30" t="s">
+        <v>309</v>
+      </c>
       <c r="C30" t="s">
         <v>520</v>
+      </c>
+      <c r="F30" t="s">
+        <v>353</v>
+      </c>
+      <c r="J30" t="s">
+        <v>309</v>
+      </c>
+      <c r="N30" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>490</v>
       </c>
+      <c r="B31" t="s">
+        <v>310</v>
+      </c>
       <c r="C31" t="s">
         <v>521</v>
+      </c>
+      <c r="F31" t="s">
+        <v>354</v>
+      </c>
+      <c r="J31" t="s">
+        <v>310</v>
+      </c>
+      <c r="N31" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>491</v>
       </c>
+      <c r="B32" t="s">
+        <v>311</v>
+      </c>
       <c r="C32" t="s">
         <v>522</v>
       </c>
       <c r="E32" t="s">
         <v>570</v>
+      </c>
+      <c r="F32" t="s">
+        <v>355</v>
+      </c>
+      <c r="J32" t="s">
+        <v>311</v>
+      </c>
+      <c r="N32" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>492</v>
       </c>
+      <c r="B33" t="s">
+        <v>312</v>
+      </c>
       <c r="C33" t="s">
         <v>523</v>
       </c>
       <c r="E33" t="s">
         <v>569</v>
+      </c>
+      <c r="F33" t="s">
+        <v>356</v>
+      </c>
+      <c r="J33" t="s">
+        <v>312</v>
+      </c>
+      <c r="N33" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>493</v>
       </c>
+      <c r="B34" t="s">
+        <v>313</v>
+      </c>
       <c r="C34" t="s">
         <v>524</v>
       </c>
       <c r="E34" t="s">
         <v>568</v>
+      </c>
+      <c r="F34" t="s">
+        <v>357</v>
+      </c>
+      <c r="J34" t="s">
+        <v>313</v>
+      </c>
+      <c r="N34" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>494</v>
       </c>
+      <c r="B35" t="s">
+        <v>314</v>
+      </c>
       <c r="C35" t="s">
         <v>525</v>
       </c>
       <c r="E35" t="s">
         <v>567</v>
+      </c>
+      <c r="F35" t="s">
+        <v>358</v>
+      </c>
+      <c r="J35" t="s">
+        <v>314</v>
+      </c>
+      <c r="N35" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>495</v>
       </c>
+      <c r="B36" t="s">
+        <v>317</v>
+      </c>
       <c r="C36" t="s">
         <v>101</v>
       </c>
       <c r="E36" t="s">
         <v>398</v>
       </c>
+      <c r="F36" t="s">
+        <v>359</v>
+      </c>
       <c r="G36" t="s">
         <v>101</v>
       </c>
+      <c r="J36" t="s">
+        <v>317</v>
+      </c>
       <c r="K36" t="s">
         <v>101</v>
       </c>
       <c r="L36" t="s">
         <v>546</v>
+      </c>
+      <c r="N36" t="s">
+        <v>359</v>
       </c>
       <c r="O36" t="s">
         <v>101</v>
@@ -5100,20 +5520,32 @@
       <c r="A37" t="s">
         <v>496</v>
       </c>
+      <c r="B37" t="s">
+        <v>318</v>
+      </c>
       <c r="C37" t="s">
         <v>217</v>
       </c>
       <c r="E37" t="s">
         <v>421</v>
       </c>
+      <c r="F37" t="s">
+        <v>360</v>
+      </c>
       <c r="G37" t="s">
         <v>217</v>
       </c>
+      <c r="J37" t="s">
+        <v>318</v>
+      </c>
       <c r="K37" t="s">
         <v>217</v>
       </c>
       <c r="L37" t="s">
         <v>547</v>
+      </c>
+      <c r="N37" t="s">
+        <v>360</v>
       </c>
       <c r="O37" t="s">
         <v>217</v>
@@ -5126,20 +5558,32 @@
       <c r="A38" t="s">
         <v>497</v>
       </c>
+      <c r="B38" t="s">
+        <v>315</v>
+      </c>
       <c r="C38" t="s">
         <v>365</v>
       </c>
       <c r="E38" t="s">
         <v>402</v>
       </c>
+      <c r="F38" t="s">
+        <v>361</v>
+      </c>
       <c r="G38" t="s">
         <v>365</v>
       </c>
+      <c r="J38" t="s">
+        <v>315</v>
+      </c>
       <c r="K38" t="s">
         <v>365</v>
       </c>
       <c r="L38" t="s">
         <v>188</v>
+      </c>
+      <c r="N38" t="s">
+        <v>361</v>
       </c>
       <c r="O38" t="s">
         <v>365</v>
@@ -5152,20 +5596,32 @@
       <c r="A39" t="s">
         <v>498</v>
       </c>
+      <c r="B39" t="s">
+        <v>316</v>
+      </c>
       <c r="C39" t="s">
         <v>366</v>
       </c>
       <c r="E39" t="s">
         <v>401</v>
       </c>
+      <c r="F39" t="s">
+        <v>362</v>
+      </c>
       <c r="G39" t="s">
         <v>366</v>
       </c>
+      <c r="J39" t="s">
+        <v>316</v>
+      </c>
       <c r="K39" t="s">
         <v>366</v>
       </c>
       <c r="L39" t="s">
         <v>189</v>
+      </c>
+      <c r="N39" t="s">
+        <v>362</v>
       </c>
       <c r="O39" t="s">
         <v>366</v>
@@ -5178,20 +5634,32 @@
       <c r="A40" t="s">
         <v>499</v>
       </c>
+      <c r="B40" t="s">
+        <v>319</v>
+      </c>
       <c r="C40" t="s">
         <v>511</v>
       </c>
       <c r="E40" t="s">
         <v>400</v>
       </c>
+      <c r="F40" t="s">
+        <v>363</v>
+      </c>
       <c r="G40" t="s">
         <v>511</v>
       </c>
+      <c r="J40" t="s">
+        <v>319</v>
+      </c>
       <c r="K40" t="s">
         <v>511</v>
       </c>
       <c r="L40" t="s">
         <v>192</v>
+      </c>
+      <c r="N40" t="s">
+        <v>363</v>
       </c>
       <c r="O40" t="s">
         <v>511</v>
@@ -5204,20 +5672,32 @@
       <c r="A41" t="s">
         <v>500</v>
       </c>
+      <c r="B41" t="s">
+        <v>320</v>
+      </c>
       <c r="C41" t="s">
         <v>368</v>
       </c>
       <c r="E41" t="s">
         <v>399</v>
       </c>
+      <c r="F41" t="s">
+        <v>364</v>
+      </c>
       <c r="G41" t="s">
         <v>368</v>
       </c>
+      <c r="J41" t="s">
+        <v>320</v>
+      </c>
       <c r="K41" t="s">
         <v>368</v>
       </c>
       <c r="L41" t="s">
         <v>548</v>
+      </c>
+      <c r="N41" t="s">
+        <v>364</v>
       </c>
       <c r="O41" t="s">
         <v>368</v>
@@ -5230,44 +5710,68 @@
       <c r="A42" t="s">
         <v>501</v>
       </c>
+      <c r="B42" t="s">
+        <v>321</v>
+      </c>
       <c r="C42" t="s">
         <v>213</v>
       </c>
       <c r="E42" t="s">
         <v>566</v>
+      </c>
+      <c r="J42" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>502</v>
       </c>
+      <c r="B43" t="s">
+        <v>322</v>
+      </c>
       <c r="C43" t="s">
         <v>214</v>
       </c>
       <c r="E43" t="s">
         <v>565</v>
+      </c>
+      <c r="J43" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>503</v>
       </c>
+      <c r="B44" t="s">
+        <v>323</v>
+      </c>
       <c r="C44" t="s">
         <v>215</v>
       </c>
       <c r="E44" t="s">
         <v>564</v>
+      </c>
+      <c r="J44" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>504</v>
       </c>
+      <c r="B45" t="s">
+        <v>324</v>
+      </c>
       <c r="C45" t="s">
         <v>216</v>
       </c>
       <c r="E45" t="s">
         <v>563</v>
+      </c>
+      <c r="J45" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5279,7 +5783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PWM signals assidned to XCore 2, P16A.
The PWM multi-bit port module will be used.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="603">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1638,9 +1638,6 @@
     <t>I2C</t>
   </si>
   <si>
-    <t>and a P4C</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -1798,6 +1795,39 @@
   </si>
   <si>
     <t>PB0/PC4</t>
+  </si>
+  <si>
+    <t>2?</t>
+  </si>
+  <si>
+    <t>and a P4</t>
+  </si>
+  <si>
+    <t>P16A0</t>
+  </si>
+  <si>
+    <t>P16A1</t>
+  </si>
+  <si>
+    <t>P16A2</t>
+  </si>
+  <si>
+    <t>P16A3</t>
+  </si>
+  <si>
+    <t>P16A4</t>
+  </si>
+  <si>
+    <t>P16A5</t>
+  </si>
+  <si>
+    <t>P16A6</t>
+  </si>
+  <si>
+    <t>P16A7</t>
+  </si>
+  <si>
+    <t>P16A15</t>
   </si>
 </sst>
 </file>
@@ -3970,7 +4000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -4194,7 +4224,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E21" t="s">
         <v>435</v>
@@ -4410,8 +4440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4419,6 +4449,7 @@
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
@@ -4435,37 +4466,37 @@
         <v>504</v>
       </c>
       <c r="C1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F1" t="s">
         <v>504</v>
       </c>
       <c r="G1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J1" t="s">
         <v>505</v>
       </c>
       <c r="K1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="L1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="N1" t="s">
         <v>505</v>
       </c>
       <c r="O1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="P1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -4494,7 +4525,7 @@
         <v>91</v>
       </c>
       <c r="M2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="N2" t="s">
         <v>325</v>
@@ -4503,7 +4534,7 @@
         <v>91</v>
       </c>
       <c r="Q2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -4532,7 +4563,7 @@
         <v>92</v>
       </c>
       <c r="M3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N3" t="s">
         <v>326</v>
@@ -4541,7 +4572,7 @@
         <v>92</v>
       </c>
       <c r="Q3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -4560,6 +4591,12 @@
       <c r="J4" t="s">
         <v>285</v>
       </c>
+      <c r="K4" t="s">
+        <v>594</v>
+      </c>
+      <c r="L4" t="s">
+        <v>399</v>
+      </c>
       <c r="N4" t="s">
         <v>327</v>
       </c>
@@ -4580,6 +4617,12 @@
       <c r="J5" t="s">
         <v>286</v>
       </c>
+      <c r="K5" t="s">
+        <v>595</v>
+      </c>
+      <c r="L5" t="s">
+        <v>400</v>
+      </c>
       <c r="N5" t="s">
         <v>328</v>
       </c>
@@ -4595,25 +4638,28 @@
         <v>513</v>
       </c>
       <c r="D6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F6" t="s">
         <v>329</v>
       </c>
       <c r="G6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="J6" t="s">
         <v>287</v>
       </c>
       <c r="K6" t="s">
-        <v>585</v>
+        <v>596</v>
+      </c>
+      <c r="L6" t="s">
+        <v>401</v>
       </c>
       <c r="N6" t="s">
         <v>329</v>
       </c>
       <c r="O6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4627,25 +4673,28 @@
         <v>514</v>
       </c>
       <c r="D7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F7" t="s">
         <v>330</v>
       </c>
       <c r="G7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="J7" t="s">
         <v>288</v>
       </c>
       <c r="K7" t="s">
-        <v>586</v>
+        <v>597</v>
+      </c>
+      <c r="L7" t="s">
+        <v>402</v>
       </c>
       <c r="N7" t="s">
         <v>330</v>
       </c>
       <c r="O7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4659,25 +4708,28 @@
         <v>515</v>
       </c>
       <c r="D8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F8" t="s">
         <v>331</v>
       </c>
       <c r="G8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="J8" t="s">
         <v>289</v>
       </c>
       <c r="K8" t="s">
-        <v>587</v>
+        <v>598</v>
+      </c>
+      <c r="L8" t="s">
+        <v>403</v>
       </c>
       <c r="N8" t="s">
         <v>331</v>
       </c>
       <c r="O8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -4691,25 +4743,28 @@
         <v>516</v>
       </c>
       <c r="D9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F9" t="s">
         <v>332</v>
       </c>
       <c r="G9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J9" t="s">
         <v>290</v>
       </c>
       <c r="K9" t="s">
-        <v>588</v>
+        <v>599</v>
+      </c>
+      <c r="L9" t="s">
+        <v>571</v>
       </c>
       <c r="N9" t="s">
         <v>332</v>
       </c>
       <c r="O9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -4728,6 +4783,12 @@
       <c r="J10" t="s">
         <v>291</v>
       </c>
+      <c r="K10" t="s">
+        <v>600</v>
+      </c>
+      <c r="L10" t="s">
+        <v>572</v>
+      </c>
       <c r="N10" t="s">
         <v>333</v>
       </c>
@@ -4748,6 +4809,12 @@
       <c r="J11" t="s">
         <v>292</v>
       </c>
+      <c r="K11" t="s">
+        <v>601</v>
+      </c>
+      <c r="L11" t="s">
+        <v>573</v>
+      </c>
       <c r="N11" t="s">
         <v>334</v>
       </c>
@@ -4778,7 +4845,7 @@
         <v>93</v>
       </c>
       <c r="M12" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="N12" t="s">
         <v>335</v>
@@ -4816,7 +4883,7 @@
         <v>94</v>
       </c>
       <c r="M13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="N13" t="s">
         <v>336</v>
@@ -4851,7 +4918,7 @@
         <v>95</v>
       </c>
       <c r="M14" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="N14" t="s">
         <v>337</v>
@@ -4886,7 +4953,7 @@
         <v>96</v>
       </c>
       <c r="M15" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="N15" t="s">
         <v>341</v>
@@ -5095,7 +5162,7 @@
         <v>383</v>
       </c>
       <c r="E22" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F22" t="s">
         <v>348</v>
@@ -5127,7 +5194,7 @@
         <v>384</v>
       </c>
       <c r="E23" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F23" t="s">
         <v>349</v>
@@ -5139,7 +5206,10 @@
         <v>305</v>
       </c>
       <c r="K23" t="s">
-        <v>384</v>
+        <v>602</v>
+      </c>
+      <c r="L23" t="s">
+        <v>398</v>
       </c>
       <c r="N23" t="s">
         <v>349</v>
@@ -5158,9 +5228,6 @@
       <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="E24" t="s">
-        <v>574</v>
-      </c>
       <c r="F24" t="s">
         <v>339</v>
       </c>
@@ -5174,7 +5241,7 @@
         <v>97</v>
       </c>
       <c r="M24" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="N24" t="s">
         <v>339</v>
@@ -5196,9 +5263,6 @@
       <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="E25" t="s">
-        <v>573</v>
-      </c>
       <c r="F25" t="s">
         <v>340</v>
       </c>
@@ -5212,7 +5276,7 @@
         <v>98</v>
       </c>
       <c r="M25" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="N25" t="s">
         <v>340</v>
@@ -5221,7 +5285,7 @@
         <v>98</v>
       </c>
       <c r="Q25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -5234,9 +5298,6 @@
       <c r="C26" t="s">
         <v>99</v>
       </c>
-      <c r="E26" t="s">
-        <v>572</v>
-      </c>
       <c r="F26" t="s">
         <v>338</v>
       </c>
@@ -5259,7 +5320,7 @@
         <v>99</v>
       </c>
       <c r="Q26" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -5272,9 +5333,6 @@
       <c r="C27" t="s">
         <v>100</v>
       </c>
-      <c r="E27" t="s">
-        <v>403</v>
-      </c>
       <c r="F27" t="s">
         <v>350</v>
       </c>
@@ -5297,7 +5355,7 @@
         <v>100</v>
       </c>
       <c r="Q27" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -5311,7 +5369,7 @@
         <v>525</v>
       </c>
       <c r="E28" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F28" t="s">
         <v>351</v>
@@ -5334,7 +5392,7 @@
         <v>526</v>
       </c>
       <c r="E29" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F29" t="s">
         <v>352</v>
@@ -5397,7 +5455,7 @@
         <v>521</v>
       </c>
       <c r="E32" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F32" t="s">
         <v>355</v>
@@ -5420,7 +5478,7 @@
         <v>522</v>
       </c>
       <c r="E33" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F33" t="s">
         <v>356</v>
@@ -5443,7 +5501,7 @@
         <v>523</v>
       </c>
       <c r="E34" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F34" t="s">
         <v>357</v>
@@ -5466,7 +5524,7 @@
         <v>524</v>
       </c>
       <c r="E35" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F35" t="s">
         <v>358</v>
@@ -5488,9 +5546,6 @@
       <c r="C36" t="s">
         <v>101</v>
       </c>
-      <c r="E36" t="s">
-        <v>398</v>
-      </c>
       <c r="F36" t="s">
         <v>359</v>
       </c>
@@ -5504,7 +5559,7 @@
         <v>101</v>
       </c>
       <c r="L36" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="N36" t="s">
         <v>359</v>
@@ -5542,7 +5597,7 @@
         <v>217</v>
       </c>
       <c r="L37" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N37" t="s">
         <v>360</v>
@@ -5551,7 +5606,7 @@
         <v>217</v>
       </c>
       <c r="P37" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -5564,9 +5619,6 @@
       <c r="C38" t="s">
         <v>365</v>
       </c>
-      <c r="E38" t="s">
-        <v>402</v>
-      </c>
       <c r="F38" t="s">
         <v>361</v>
       </c>
@@ -5602,9 +5654,6 @@
       <c r="C39" t="s">
         <v>366</v>
       </c>
-      <c r="E39" t="s">
-        <v>401</v>
-      </c>
       <c r="F39" t="s">
         <v>362</v>
       </c>
@@ -5640,9 +5689,6 @@
       <c r="C40" t="s">
         <v>510</v>
       </c>
-      <c r="E40" t="s">
-        <v>400</v>
-      </c>
       <c r="F40" t="s">
         <v>363</v>
       </c>
@@ -5678,9 +5724,6 @@
       <c r="C41" t="s">
         <v>368</v>
       </c>
-      <c r="E41" t="s">
-        <v>399</v>
-      </c>
       <c r="F41" t="s">
         <v>364</v>
       </c>
@@ -5694,7 +5737,7 @@
         <v>368</v>
       </c>
       <c r="L41" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="N41" t="s">
         <v>364</v>
@@ -5717,7 +5760,7 @@
         <v>213</v>
       </c>
       <c r="E42" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="J42" t="s">
         <v>321</v>
@@ -5734,7 +5777,7 @@
         <v>214</v>
       </c>
       <c r="E43" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J43" t="s">
         <v>322</v>
@@ -5751,7 +5794,7 @@
         <v>215</v>
       </c>
       <c r="E44" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J44" t="s">
         <v>323</v>
@@ -5768,7 +5811,7 @@
         <v>216</v>
       </c>
       <c r="E45" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="J45" t="s">
         <v>324</v>
@@ -5781,10 +5824,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5793,7 +5836,7 @@
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>531</v>
       </c>
@@ -5801,13 +5844,13 @@
         <v>532</v>
       </c>
       <c r="D1" t="s">
+        <v>588</v>
+      </c>
+      <c r="E1" t="s">
         <v>589</v>
       </c>
-      <c r="E1" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>533</v>
       </c>
@@ -5815,10 +5858,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>534</v>
       </c>
@@ -5826,10 +5869,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>535</v>
       </c>
@@ -5837,10 +5880,10 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -5848,10 +5891,10 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>536</v>
       </c>
@@ -5862,7 +5905,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>538</v>
       </c>
@@ -5870,15 +5913,15 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>539</v>
+        <v>593</v>
       </c>
       <c r="D7" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B8">
         <v>9</v>
@@ -5886,10 +5929,13 @@
       <c r="D8" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -5898,9 +5944,9 @@
         <v>537</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -5909,21 +5955,21 @@
         <v>537</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D11" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(B2:B11)</f>
         <v>61</v>

</xml_diff>

<commit_message>
U12 and U19 A-side connections to U2 defined.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="615">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1828,6 +1828,42 @@
   </si>
   <si>
     <t>P16A15</t>
+  </si>
+  <si>
+    <t>U12_A5</t>
+  </si>
+  <si>
+    <t>U12_A4</t>
+  </si>
+  <si>
+    <t>U12_A3</t>
+  </si>
+  <si>
+    <t>U12_A2</t>
+  </si>
+  <si>
+    <t>U12_A1</t>
+  </si>
+  <si>
+    <t>U19_A7</t>
+  </si>
+  <si>
+    <t>U19_A6</t>
+  </si>
+  <si>
+    <t>U19_A5</t>
+  </si>
+  <si>
+    <t>U19_A4</t>
+  </si>
+  <si>
+    <t>U19_A3</t>
+  </si>
+  <si>
+    <t>U19_A2</t>
+  </si>
+  <si>
+    <t>U19_A8</t>
   </si>
 </sst>
 </file>
@@ -4440,8 +4476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4993,6 +5029,9 @@
       <c r="O16" t="s">
         <v>377</v>
       </c>
+      <c r="P16" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -5022,6 +5061,9 @@
       <c r="O17" t="s">
         <v>378</v>
       </c>
+      <c r="P17" t="s">
+        <v>609</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5054,6 +5096,9 @@
       <c r="O18" t="s">
         <v>509</v>
       </c>
+      <c r="P18" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -5086,6 +5131,9 @@
       <c r="O19" t="s">
         <v>508</v>
       </c>
+      <c r="P19" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -5118,6 +5166,9 @@
       <c r="O20" t="s">
         <v>506</v>
       </c>
+      <c r="P20" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -5150,6 +5201,9 @@
       <c r="O21" t="s">
         <v>507</v>
       </c>
+      <c r="P21" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -5380,6 +5434,9 @@
       <c r="N28" t="s">
         <v>351</v>
       </c>
+      <c r="P28" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -5403,6 +5460,9 @@
       <c r="N29" t="s">
         <v>352</v>
       </c>
+      <c r="P29" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -5423,6 +5483,9 @@
       <c r="N30" t="s">
         <v>353</v>
       </c>
+      <c r="P30" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -5443,6 +5506,9 @@
       <c r="N31" t="s">
         <v>354</v>
       </c>
+      <c r="P31" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -5466,6 +5532,9 @@
       <c r="N32" t="s">
         <v>355</v>
       </c>
+      <c r="P32" t="s">
+        <v>607</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -5488,6 +5557,9 @@
       </c>
       <c r="N33" t="s">
         <v>356</v>
+      </c>
+      <c r="P33" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -5827,7 +5899,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
U12 and U19 B-side connections to H-bridges defined.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="603">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1828,42 +1828,6 @@
   </si>
   <si>
     <t>P16A15</t>
-  </si>
-  <si>
-    <t>U12_A5</t>
-  </si>
-  <si>
-    <t>U12_A4</t>
-  </si>
-  <si>
-    <t>U12_A3</t>
-  </si>
-  <si>
-    <t>U12_A2</t>
-  </si>
-  <si>
-    <t>U12_A1</t>
-  </si>
-  <si>
-    <t>U19_A7</t>
-  </si>
-  <si>
-    <t>U19_A6</t>
-  </si>
-  <si>
-    <t>U19_A5</t>
-  </si>
-  <si>
-    <t>U19_A4</t>
-  </si>
-  <si>
-    <t>U19_A3</t>
-  </si>
-  <si>
-    <t>U19_A2</t>
-  </si>
-  <si>
-    <t>U19_A8</t>
   </si>
 </sst>
 </file>
@@ -4476,8 +4440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5030,7 +4994,7 @@
         <v>377</v>
       </c>
       <c r="P16" t="s">
-        <v>608</v>
+        <v>574</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -5062,7 +5026,7 @@
         <v>378</v>
       </c>
       <c r="P17" t="s">
-        <v>609</v>
+        <v>561</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -5097,7 +5061,7 @@
         <v>509</v>
       </c>
       <c r="P18" t="s">
-        <v>610</v>
+        <v>575</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -5132,7 +5096,7 @@
         <v>508</v>
       </c>
       <c r="P19" t="s">
-        <v>611</v>
+        <v>562</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -5167,7 +5131,7 @@
         <v>506</v>
       </c>
       <c r="P20" t="s">
-        <v>612</v>
+        <v>563</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -5202,7 +5166,7 @@
         <v>507</v>
       </c>
       <c r="P21" t="s">
-        <v>613</v>
+        <v>564</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -5215,9 +5179,6 @@
       <c r="C22" t="s">
         <v>383</v>
       </c>
-      <c r="E22" t="s">
-        <v>575</v>
-      </c>
       <c r="F22" t="s">
         <v>348</v>
       </c>
@@ -5247,9 +5208,6 @@
       <c r="C23" t="s">
         <v>384</v>
       </c>
-      <c r="E23" t="s">
-        <v>574</v>
-      </c>
       <c r="F23" t="s">
         <v>349</v>
       </c>
@@ -5422,9 +5380,6 @@
       <c r="C28" t="s">
         <v>525</v>
       </c>
-      <c r="E28" t="s">
-        <v>570</v>
-      </c>
       <c r="F28" t="s">
         <v>351</v>
       </c>
@@ -5435,7 +5390,7 @@
         <v>351</v>
       </c>
       <c r="P28" t="s">
-        <v>603</v>
+        <v>565</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -5448,9 +5403,6 @@
       <c r="C29" t="s">
         <v>526</v>
       </c>
-      <c r="E29" t="s">
-        <v>569</v>
-      </c>
       <c r="F29" t="s">
         <v>352</v>
       </c>
@@ -5461,7 +5413,7 @@
         <v>352</v>
       </c>
       <c r="P29" t="s">
-        <v>604</v>
+        <v>566</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -5484,7 +5436,7 @@
         <v>353</v>
       </c>
       <c r="P30" t="s">
-        <v>605</v>
+        <v>569</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -5507,7 +5459,7 @@
         <v>354</v>
       </c>
       <c r="P31" t="s">
-        <v>606</v>
+        <v>570</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -5520,9 +5472,6 @@
       <c r="C32" t="s">
         <v>521</v>
       </c>
-      <c r="E32" t="s">
-        <v>568</v>
-      </c>
       <c r="F32" t="s">
         <v>355</v>
       </c>
@@ -5533,7 +5482,7 @@
         <v>355</v>
       </c>
       <c r="P32" t="s">
-        <v>607</v>
+        <v>567</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -5546,9 +5495,6 @@
       <c r="C33" t="s">
         <v>522</v>
       </c>
-      <c r="E33" t="s">
-        <v>567</v>
-      </c>
       <c r="F33" t="s">
         <v>356</v>
       </c>
@@ -5559,7 +5505,7 @@
         <v>356</v>
       </c>
       <c r="P33" t="s">
-        <v>614</v>
+        <v>568</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -5572,9 +5518,6 @@
       <c r="C34" t="s">
         <v>523</v>
       </c>
-      <c r="E34" t="s">
-        <v>566</v>
-      </c>
       <c r="F34" t="s">
         <v>357</v>
       </c>
@@ -5595,9 +5538,6 @@
       <c r="C35" t="s">
         <v>524</v>
       </c>
-      <c r="E35" t="s">
-        <v>565</v>
-      </c>
       <c r="F35" t="s">
         <v>358</v>
       </c>
@@ -5831,9 +5771,6 @@
       <c r="C42" t="s">
         <v>213</v>
       </c>
-      <c r="E42" t="s">
-        <v>564</v>
-      </c>
       <c r="J42" t="s">
         <v>321</v>
       </c>
@@ -5848,9 +5785,6 @@
       <c r="C43" t="s">
         <v>214</v>
       </c>
-      <c r="E43" t="s">
-        <v>563</v>
-      </c>
       <c r="J43" t="s">
         <v>322</v>
       </c>
@@ -5865,9 +5799,6 @@
       <c r="C44" t="s">
         <v>215</v>
       </c>
-      <c r="E44" t="s">
-        <v>562</v>
-      </c>
       <c r="J44" t="s">
         <v>323</v>
       </c>
@@ -5881,9 +5812,6 @@
       </c>
       <c r="C45" t="s">
         <v>216</v>
-      </c>
-      <c r="E45" t="s">
-        <v>561</v>
       </c>
       <c r="J45" t="s">
         <v>324</v>

</xml_diff>

<commit_message>
Assigned the microSD SS line to X0P1K.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="609">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1797,9 +1797,6 @@
     <t>PB0/PC4</t>
   </si>
   <si>
-    <t>2?</t>
-  </si>
-  <si>
     <t>and a P4</t>
   </si>
   <si>
@@ -1828,6 +1825,27 @@
   </si>
   <si>
     <t>P16A15</t>
+  </si>
+  <si>
+    <t>By Block ^</t>
+  </si>
+  <si>
+    <t>By Core^</t>
+  </si>
+  <si>
+    <t>X0 1-bit</t>
+  </si>
+  <si>
+    <t>X1 1-bit</t>
+  </si>
+  <si>
+    <t>X2 1-bit</t>
+  </si>
+  <si>
+    <t>X3 1-bit</t>
+  </si>
+  <si>
+    <t>Total 1-bits</t>
   </si>
 </sst>
 </file>
@@ -4440,8 +4458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4592,7 +4610,7 @@
         <v>285</v>
       </c>
       <c r="K4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="L4" t="s">
         <v>399</v>
@@ -4618,7 +4636,7 @@
         <v>286</v>
       </c>
       <c r="K5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L5" t="s">
         <v>400</v>
@@ -4650,7 +4668,7 @@
         <v>287</v>
       </c>
       <c r="K6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L6" t="s">
         <v>401</v>
@@ -4685,7 +4703,7 @@
         <v>288</v>
       </c>
       <c r="K7" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L7" t="s">
         <v>402</v>
@@ -4720,7 +4738,7 @@
         <v>289</v>
       </c>
       <c r="K8" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L8" t="s">
         <v>403</v>
@@ -4755,7 +4773,7 @@
         <v>290</v>
       </c>
       <c r="K9" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L9" t="s">
         <v>571</v>
@@ -4784,7 +4802,7 @@
         <v>291</v>
       </c>
       <c r="K10" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="L10" t="s">
         <v>572</v>
@@ -4810,7 +4828,7 @@
         <v>292</v>
       </c>
       <c r="K11" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L11" t="s">
         <v>573</v>
@@ -5218,7 +5236,7 @@
         <v>305</v>
       </c>
       <c r="K23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L23" t="s">
         <v>398</v>
@@ -5558,6 +5576,9 @@
       <c r="C36" t="s">
         <v>101</v>
       </c>
+      <c r="D36" t="s">
+        <v>421</v>
+      </c>
       <c r="F36" t="s">
         <v>359</v>
       </c>
@@ -5592,9 +5613,6 @@
       </c>
       <c r="C37" t="s">
         <v>217</v>
-      </c>
-      <c r="E37" t="s">
-        <v>421</v>
       </c>
       <c r="F37" t="s">
         <v>360</v>
@@ -5824,19 +5842,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>531</v>
       </c>
@@ -5849,8 +5868,23 @@
       <c r="E1" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>531</v>
+      </c>
+      <c r="H1" t="s">
+        <v>604</v>
+      </c>
+      <c r="I1" t="s">
+        <v>605</v>
+      </c>
+      <c r="J1" t="s">
+        <v>606</v>
+      </c>
+      <c r="K1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>533</v>
       </c>
@@ -5860,8 +5894,11 @@
       <c r="D2" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>534</v>
       </c>
@@ -5871,8 +5908,11 @@
       <c r="D3" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>535</v>
       </c>
@@ -5882,8 +5922,11 @@
       <c r="D4" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -5893,8 +5936,11 @@
       <c r="D5" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>536</v>
       </c>
@@ -5904,8 +5950,14 @@
       <c r="D6" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>536</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>538</v>
       </c>
@@ -5913,13 +5965,16 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D7" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>540</v>
       </c>
@@ -5927,13 +5982,16 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>537</v>
-      </c>
-      <c r="F8" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+      <c r="G8" t="s">
+        <v>540</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>541</v>
       </c>
@@ -5943,8 +6001,11 @@
       <c r="D9" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>542</v>
       </c>
@@ -5954,8 +6015,11 @@
       <c r="D10" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>543</v>
       </c>
@@ -5968,11 +6032,41 @@
       <c r="D11" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(B2:B11)</f>
         <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>608</v>
+      </c>
+      <c r="H13">
+        <f>SUM(H3:H11)</f>
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:K13" si="0">SUM(I2:I11)</f>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>602</v>
+      </c>
+      <c r="G16" t="s">
+        <v>603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assigned Pmod 0 to X0.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -4458,8 +4458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4958,6 +4958,9 @@
       <c r="C15" t="s">
         <v>96</v>
       </c>
+      <c r="D15" t="s">
+        <v>545</v>
+      </c>
       <c r="F15" t="s">
         <v>341</v>
       </c>
@@ -5293,6 +5296,9 @@
       <c r="C25" t="s">
         <v>98</v>
       </c>
+      <c r="D25" t="s">
+        <v>188</v>
+      </c>
       <c r="F25" t="s">
         <v>340</v>
       </c>
@@ -5340,9 +5346,6 @@
       <c r="K26" t="s">
         <v>99</v>
       </c>
-      <c r="M26" t="s">
-        <v>186</v>
-      </c>
       <c r="N26" t="s">
         <v>338</v>
       </c>
@@ -5363,6 +5366,9 @@
       <c r="C27" t="s">
         <v>100</v>
       </c>
+      <c r="D27" t="s">
+        <v>187</v>
+      </c>
       <c r="F27" t="s">
         <v>350</v>
       </c>
@@ -5374,9 +5380,6 @@
       </c>
       <c r="K27" t="s">
         <v>100</v>
-      </c>
-      <c r="M27" t="s">
-        <v>187</v>
       </c>
       <c r="N27" t="s">
         <v>350</v>
@@ -5591,9 +5594,6 @@
       <c r="K36" t="s">
         <v>101</v>
       </c>
-      <c r="L36" t="s">
-        <v>544</v>
-      </c>
       <c r="N36" t="s">
         <v>359</v>
       </c>
@@ -5614,6 +5614,9 @@
       <c r="C37" t="s">
         <v>217</v>
       </c>
+      <c r="D37" t="s">
+        <v>186</v>
+      </c>
       <c r="F37" t="s">
         <v>360</v>
       </c>
@@ -5625,9 +5628,6 @@
       </c>
       <c r="K37" t="s">
         <v>217</v>
-      </c>
-      <c r="L37" t="s">
-        <v>545</v>
       </c>
       <c r="N37" t="s">
         <v>360</v>
@@ -5649,6 +5649,9 @@
       <c r="C38" t="s">
         <v>365</v>
       </c>
+      <c r="D38" t="s">
+        <v>544</v>
+      </c>
       <c r="F38" t="s">
         <v>361</v>
       </c>
@@ -5660,9 +5663,6 @@
       </c>
       <c r="K38" t="s">
         <v>365</v>
-      </c>
-      <c r="L38" t="s">
-        <v>188</v>
       </c>
       <c r="N38" t="s">
         <v>361</v>
@@ -5684,6 +5684,9 @@
       <c r="C39" t="s">
         <v>366</v>
       </c>
+      <c r="D39" t="s">
+        <v>546</v>
+      </c>
       <c r="F39" t="s">
         <v>362</v>
       </c>
@@ -5695,9 +5698,6 @@
       </c>
       <c r="K39" t="s">
         <v>366</v>
-      </c>
-      <c r="L39" t="s">
-        <v>189</v>
       </c>
       <c r="N39" t="s">
         <v>362</v>
@@ -5719,6 +5719,9 @@
       <c r="C40" t="s">
         <v>510</v>
       </c>
+      <c r="D40" t="s">
+        <v>192</v>
+      </c>
       <c r="F40" t="s">
         <v>363</v>
       </c>
@@ -5730,9 +5733,6 @@
       </c>
       <c r="K40" t="s">
         <v>510</v>
-      </c>
-      <c r="L40" t="s">
-        <v>192</v>
       </c>
       <c r="N40" t="s">
         <v>363</v>
@@ -5754,6 +5754,9 @@
       <c r="C41" t="s">
         <v>368</v>
       </c>
+      <c r="D41" t="s">
+        <v>189</v>
+      </c>
       <c r="F41" t="s">
         <v>364</v>
       </c>
@@ -5765,9 +5768,6 @@
       </c>
       <c r="K41" t="s">
         <v>368</v>
-      </c>
-      <c r="L41" t="s">
-        <v>546</v>
       </c>
       <c r="N41" t="s">
         <v>364</v>
@@ -5844,8 +5844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5897,6 +5897,9 @@
       <c r="G2" t="s">
         <v>533</v>
       </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -6045,8 +6048,8 @@
         <v>608</v>
       </c>
       <c r="H13">
-        <f>SUM(H3:H11)</f>
-        <v>5</v>
+        <f>SUM(H2:H11)</f>
+        <v>13</v>
       </c>
       <c r="I13">
         <f t="shared" ref="I13:K13" si="0">SUM(I2:I11)</f>

</xml_diff>

<commit_message>
Assigning encoders to XCore 3 (no pins yet).
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4458,8 +4458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5845,7 +5845,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5982,7 +5982,7 @@
         <v>540</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>539</v>
@@ -5999,13 +5999,16 @@
         <v>541</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>537</v>
       </c>
       <c r="G9" t="s">
         <v>541</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -6042,7 +6045,7 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(B2:B11)</f>
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
         <v>608</v>
@@ -6061,7 +6064,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Encoder ports assigned on X3.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="618">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1846,6 +1846,33 @@
   </si>
   <si>
     <t>Total 1-bits</t>
+  </si>
+  <si>
+    <t>ENC0_B</t>
+  </si>
+  <si>
+    <t>ENC0_A</t>
+  </si>
+  <si>
+    <t>ENC0_Z</t>
+  </si>
+  <si>
+    <t>ENC1_B</t>
+  </si>
+  <si>
+    <t>ENC1_Z</t>
+  </si>
+  <si>
+    <t>ENC1_A</t>
+  </si>
+  <si>
+    <t>ENC2_Z</t>
+  </si>
+  <si>
+    <t>ENC2_A</t>
+  </si>
+  <si>
+    <t>ENC2_B</t>
   </si>
 </sst>
 </file>
@@ -4456,10 +4483,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4476,7 +4503,7 @@
     <col min="16" max="16" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>459</v>
       </c>
@@ -4517,7 +4544,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>460</v>
       </c>
@@ -4551,11 +4578,11 @@
       <c r="O2" t="s">
         <v>91</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>461</v>
       </c>
@@ -4589,11 +4616,11 @@
       <c r="O3" t="s">
         <v>92</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>462</v>
       </c>
@@ -4619,7 +4646,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>463</v>
       </c>
@@ -4645,7 +4672,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>464</v>
       </c>
@@ -4680,7 +4707,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -4715,7 +4742,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>466</v>
       </c>
@@ -4750,7 +4777,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>467</v>
       </c>
@@ -4785,7 +4812,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>468</v>
       </c>
@@ -4811,7 +4838,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>469</v>
       </c>
@@ -4837,7 +4864,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>470</v>
       </c>
@@ -4871,11 +4898,11 @@
       <c r="O12" t="s">
         <v>93</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>471</v>
       </c>
@@ -4909,11 +4936,11 @@
       <c r="O13" t="s">
         <v>94</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>472</v>
       </c>
@@ -4944,11 +4971,14 @@
       <c r="O14" t="s">
         <v>95</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="P14" t="s">
+        <v>610</v>
+      </c>
+      <c r="R14" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>473</v>
       </c>
@@ -4982,11 +5012,14 @@
       <c r="O15" t="s">
         <v>96</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="P15" t="s">
+        <v>612</v>
+      </c>
+      <c r="R15" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>474</v>
       </c>
@@ -5018,7 +5051,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>475</v>
       </c>
@@ -5050,7 +5083,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>476</v>
       </c>
@@ -5085,7 +5118,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>477</v>
       </c>
@@ -5120,7 +5153,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>478</v>
       </c>
@@ -5155,7 +5188,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>479</v>
       </c>
@@ -5190,7 +5223,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>480</v>
       </c>
@@ -5219,7 +5252,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>481</v>
       </c>
@@ -5251,7 +5284,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>482</v>
       </c>
@@ -5282,11 +5315,14 @@
       <c r="O24" t="s">
         <v>97</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="P24" t="s">
+        <v>611</v>
+      </c>
+      <c r="R24" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>483</v>
       </c>
@@ -5320,11 +5356,14 @@
       <c r="O25" t="s">
         <v>98</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="P25" t="s">
+        <v>613</v>
+      </c>
+      <c r="R25" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>484</v>
       </c>
@@ -5352,11 +5391,14 @@
       <c r="O26" t="s">
         <v>99</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="P26" t="s">
+        <v>609</v>
+      </c>
+      <c r="R26" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>485</v>
       </c>
@@ -5387,11 +5429,11 @@
       <c r="O27" t="s">
         <v>100</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>486</v>
       </c>
@@ -5414,7 +5456,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>487</v>
       </c>
@@ -5437,7 +5479,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>488</v>
       </c>
@@ -5460,7 +5502,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>489</v>
       </c>
@@ -5483,7 +5525,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>490</v>
       </c>
@@ -5506,7 +5548,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>491</v>
       </c>
@@ -5529,7 +5571,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>492</v>
       </c>
@@ -5549,7 +5591,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>493</v>
       </c>
@@ -5569,7 +5611,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>494</v>
       </c>
@@ -5601,10 +5643,13 @@
         <v>101</v>
       </c>
       <c r="P36" t="s">
+        <v>614</v>
+      </c>
+      <c r="R36" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>495</v>
       </c>
@@ -5636,10 +5681,13 @@
         <v>217</v>
       </c>
       <c r="P37" t="s">
+        <v>615</v>
+      </c>
+      <c r="R37" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>496</v>
       </c>
@@ -5671,10 +5719,13 @@
         <v>365</v>
       </c>
       <c r="P38" t="s">
+        <v>616</v>
+      </c>
+      <c r="R38" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>497</v>
       </c>
@@ -5706,10 +5757,13 @@
         <v>366</v>
       </c>
       <c r="P39" t="s">
+        <v>617</v>
+      </c>
+      <c r="R39" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>498</v>
       </c>
@@ -5740,11 +5794,11 @@
       <c r="O40" t="s">
         <v>510</v>
       </c>
-      <c r="P40" t="s">
+      <c r="R40" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>499</v>
       </c>
@@ -5775,11 +5829,11 @@
       <c r="O41" t="s">
         <v>368</v>
       </c>
-      <c r="P41" t="s">
+      <c r="R41" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>500</v>
       </c>
@@ -5793,7 +5847,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>501</v>
       </c>
@@ -5807,7 +5861,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>502</v>
       </c>
@@ -5821,7 +5875,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>503</v>
       </c>
@@ -5844,7 +5898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed references to old chip assignments in XMOS Dualchip Planning.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="618">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -4485,8 +4485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5898,8 +5898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5946,7 +5946,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="G2" t="s">
         <v>533</v>
@@ -5962,9 +5962,6 @@
       <c r="B3">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>539</v>
-      </c>
       <c r="G3" t="s">
         <v>534</v>
       </c>
@@ -5976,9 +5973,6 @@
       <c r="B4">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>539</v>
-      </c>
       <c r="G4" t="s">
         <v>535</v>
       </c>
@@ -5990,9 +5984,6 @@
       <c r="B5">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>539</v>
-      </c>
       <c r="G5" t="s">
         <v>389</v>
       </c>
@@ -6024,9 +6015,6 @@
       <c r="C7" t="s">
         <v>592</v>
       </c>
-      <c r="D7" t="s">
-        <v>537</v>
-      </c>
       <c r="G7" t="s">
         <v>538</v>
       </c>
@@ -6056,7 +6044,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="G9" t="s">
         <v>541</v>
@@ -6072,9 +6060,6 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>537</v>
-      </c>
       <c r="G10" t="s">
         <v>542</v>
       </c>
@@ -6088,9 +6073,6 @@
       </c>
       <c r="C11" t="s">
         <v>590</v>
-      </c>
-      <c r="D11" t="s">
-        <v>537</v>
       </c>
       <c r="G11" t="s">
         <v>543</v>

</xml_diff>

<commit_message>
Gadgeteer requires 8 ports, not 7.
The 8th port is the I2C mode switch.
If need be, this IO line could be replaced with a jumper.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -5899,7 +5899,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5982,7 +5982,7 @@
         <v>389</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
         <v>389</v>
@@ -6081,7 +6081,7 @@
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(B2:B11)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
         <v>608</v>

</xml_diff>

<commit_message>
IMU and XBee blocks assigned to XCore 3.
-Signals set.
-Initial off-board trace routing.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="625">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1873,6 +1873,27 @@
   </si>
   <si>
     <t>ENC2_B</t>
+  </si>
+  <si>
+    <t>1-bit ports remaining</t>
+  </si>
+  <si>
+    <t>Unallocated</t>
+  </si>
+  <si>
+    <t>U13_DRDY</t>
+  </si>
+  <si>
+    <t>XBEE_CTS</t>
+  </si>
+  <si>
+    <t>XBEE_RTS</t>
+  </si>
+  <si>
+    <t>U15_INT1</t>
+  </si>
+  <si>
+    <t>U15_INT2</t>
   </si>
 </sst>
 </file>
@@ -4485,8 +4506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4578,6 +4599,9 @@
       <c r="O2" t="s">
         <v>91</v>
       </c>
+      <c r="P2" t="s">
+        <v>218</v>
+      </c>
       <c r="R2" t="s">
         <v>559</v>
       </c>
@@ -4616,6 +4640,9 @@
       <c r="O3" t="s">
         <v>92</v>
       </c>
+      <c r="P3" t="s">
+        <v>219</v>
+      </c>
       <c r="R3" t="s">
         <v>560</v>
       </c>
@@ -4645,6 +4672,12 @@
       <c r="N4" t="s">
         <v>327</v>
       </c>
+      <c r="O4" t="s">
+        <v>511</v>
+      </c>
+      <c r="P4" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4671,6 +4704,12 @@
       <c r="N5" t="s">
         <v>328</v>
       </c>
+      <c r="O5" t="s">
+        <v>512</v>
+      </c>
+      <c r="P5" t="s">
+        <v>624</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -4704,7 +4743,10 @@
         <v>329</v>
       </c>
       <c r="O6" t="s">
-        <v>584</v>
+        <v>513</v>
+      </c>
+      <c r="P6" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -4739,7 +4781,10 @@
         <v>330</v>
       </c>
       <c r="O7" t="s">
-        <v>585</v>
+        <v>514</v>
+      </c>
+      <c r="P7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -4774,7 +4819,7 @@
         <v>331</v>
       </c>
       <c r="O8" t="s">
-        <v>586</v>
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -4809,7 +4854,7 @@
         <v>332</v>
       </c>
       <c r="O9" t="s">
-        <v>587</v>
+        <v>516</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -4837,6 +4882,9 @@
       <c r="N10" t="s">
         <v>333</v>
       </c>
+      <c r="O10" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -4863,6 +4911,9 @@
       <c r="N11" t="s">
         <v>334</v>
       </c>
+      <c r="O11" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -4898,6 +4949,9 @@
       <c r="O12" t="s">
         <v>93</v>
       </c>
+      <c r="P12" t="s">
+        <v>457</v>
+      </c>
       <c r="R12" t="s">
         <v>233</v>
       </c>
@@ -4936,6 +4990,9 @@
       <c r="O13" t="s">
         <v>94</v>
       </c>
+      <c r="P13" t="s">
+        <v>458</v>
+      </c>
       <c r="R13" t="s">
         <v>234</v>
       </c>
@@ -5429,6 +5486,9 @@
       <c r="O27" t="s">
         <v>100</v>
       </c>
+      <c r="P27" t="s">
+        <v>620</v>
+      </c>
       <c r="R27" t="s">
         <v>557</v>
       </c>
@@ -5794,6 +5854,9 @@
       <c r="O40" t="s">
         <v>510</v>
       </c>
+      <c r="P40" t="s">
+        <v>621</v>
+      </c>
       <c r="R40" t="s">
         <v>204</v>
       </c>
@@ -5828,6 +5891,9 @@
       </c>
       <c r="O41" t="s">
         <v>368</v>
+      </c>
+      <c r="P41" t="s">
+        <v>622</v>
       </c>
       <c r="R41" t="s">
         <v>205</v>
@@ -5896,20 +5962,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>531</v>
       </c>
@@ -5937,8 +6004,11 @@
       <c r="K1" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>533</v>
       </c>
@@ -5955,7 +6025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>534</v>
       </c>
@@ -5965,8 +6035,11 @@
       <c r="G3" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>535</v>
       </c>
@@ -5976,8 +6049,11 @@
       <c r="G4" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -5987,8 +6063,11 @@
       <c r="G5" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>536</v>
       </c>
@@ -6005,7 +6084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>538</v>
       </c>
@@ -6018,8 +6097,11 @@
       <c r="G7" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>540</v>
       </c>
@@ -6036,7 +6118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>541</v>
       </c>
@@ -6053,7 +6135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>542</v>
       </c>
@@ -6063,8 +6145,11 @@
       <c r="G10" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>543</v>
       </c>
@@ -6077,8 +6162,11 @@
       <c r="G11" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>SUM(B2:B11)</f>
         <v>56</v>
@@ -6091,7 +6179,7 @@
         <v>13</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:K13" si="0">SUM(I2:I11)</f>
+        <f t="shared" ref="I13:L13" si="0">SUM(I2:I11)</f>
         <v>0</v>
       </c>
       <c r="J13">
@@ -6099,11 +6187,36 @@
         <v>0</v>
       </c>
       <c r="K13">
+        <f>SUM(K2:K11)</f>
+        <v>16</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>618</v>
+      </c>
+      <c r="H14">
+        <f>16-H13</f>
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <f>16-I13</f>
+        <v>16</v>
+      </c>
+      <c r="J14">
+        <f>16-J13</f>
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <f>16-K13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>602</v>
       </c>

</xml_diff>

<commit_message>
Shifted Pmod 0 signals over by one port to allow for UEXT_SS on X0_P1L.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="629">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1903,6 +1903,9 @@
   </si>
   <si>
     <t>IMU I2C</t>
+  </si>
+  <si>
+    <t>UEXT_SS</t>
   </si>
 </sst>
 </file>
@@ -4515,8 +4518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5055,7 +5058,7 @@
         <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F15" t="s">
         <v>341</v>
@@ -5360,6 +5363,9 @@
       <c r="C24" t="s">
         <v>97</v>
       </c>
+      <c r="D24" t="s">
+        <v>545</v>
+      </c>
       <c r="F24" t="s">
         <v>339</v>
       </c>
@@ -5399,7 +5405,7 @@
         <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F25" t="s">
         <v>340</v>
@@ -5475,7 +5481,7 @@
         <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F27" t="s">
         <v>350</v>
@@ -5729,7 +5735,7 @@
         <v>217</v>
       </c>
       <c r="D37" t="s">
-        <v>186</v>
+        <v>628</v>
       </c>
       <c r="F37" t="s">
         <v>360</v>
@@ -5767,7 +5773,7 @@
         <v>365</v>
       </c>
       <c r="D38" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="F38" t="s">
         <v>361</v>
@@ -5805,7 +5811,7 @@
         <v>366</v>
       </c>
       <c r="D39" t="s">
-        <v>546</v>
+        <v>192</v>
       </c>
       <c r="F39" t="s">
         <v>362</v>
@@ -5843,7 +5849,7 @@
         <v>510</v>
       </c>
       <c r="D40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F40" t="s">
         <v>363</v>
@@ -5881,7 +5887,7 @@
         <v>368</v>
       </c>
       <c r="D41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F41" t="s">
         <v>364</v>
@@ -5974,7 +5980,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6214,7 +6220,7 @@
         <v>16</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
+        <f>SUM(L2:L11)</f>
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Assigning (in planning only) UEXT I2C and UART to XCore 1.
Looking at probably X1_P1I, X1_P1E, X1_P1G, and X1_P1F for these.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -5980,7 +5980,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6112,7 +6112,7 @@
       <c r="G7" t="s">
         <v>625</v>
       </c>
-      <c r="L7">
+      <c r="I7">
         <v>2</v>
       </c>
     </row>
@@ -6191,7 +6191,7 @@
       <c r="G12" t="s">
         <v>626</v>
       </c>
-      <c r="L12">
+      <c r="I12">
         <v>2</v>
       </c>
     </row>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="I14">
         <f t="shared" ref="I14:L14" si="0">SUM(I2:I11)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
@@ -6221,7 +6221,7 @@
       </c>
       <c r="L14">
         <f>SUM(L2:L11)</f>
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -6234,7 +6234,7 @@
       </c>
       <c r="I15">
         <f>16-I14</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J15">
         <f>16-J14</f>

</xml_diff>

<commit_message>
All UEXT signals set.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="633">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1906,6 +1906,18 @@
   </si>
   <si>
     <t>UEXT_SS</t>
+  </si>
+  <si>
+    <t>UEXT_SCL</t>
+  </si>
+  <si>
+    <t>UEXT_SDA</t>
+  </si>
+  <si>
+    <t>UEXT_RXD</t>
+  </si>
+  <si>
+    <t>UEXT_TXD</t>
   </si>
 </sst>
 </file>
@@ -4518,8 +4530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5025,6 +5037,9 @@
       <c r="G14" t="s">
         <v>95</v>
       </c>
+      <c r="H14" t="s">
+        <v>630</v>
+      </c>
       <c r="J14" t="s">
         <v>293</v>
       </c>
@@ -5066,6 +5081,9 @@
       <c r="G15" t="s">
         <v>96</v>
       </c>
+      <c r="H15" t="s">
+        <v>631</v>
+      </c>
       <c r="J15" t="s">
         <v>294</v>
       </c>
@@ -5372,6 +5390,9 @@
       <c r="G24" t="s">
         <v>97</v>
       </c>
+      <c r="H24" t="s">
+        <v>632</v>
+      </c>
       <c r="J24" t="s">
         <v>301</v>
       </c>
@@ -5450,6 +5471,9 @@
       </c>
       <c r="G26" t="s">
         <v>99</v>
+      </c>
+      <c r="H26" t="s">
+        <v>629</v>
       </c>
       <c r="J26" t="s">
         <v>300</v>
@@ -5979,7 +6003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Eliminated references to JP13 Gadgeteer I2C signals.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="630">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1662,9 +1662,6 @@
     <t>JP3_8</t>
   </si>
   <si>
-    <t>JP13_I2C_MODE</t>
-  </si>
-  <si>
     <t>U17_A1</t>
   </si>
   <si>
@@ -1678,12 +1675,6 @@
   </si>
   <si>
     <t>U17_A4</t>
-  </si>
-  <si>
-    <t>IC6_X</t>
-  </si>
-  <si>
-    <t>IC7_X</t>
   </si>
   <si>
     <t>JP4_8</t>
@@ -4314,7 +4305,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E21" t="s">
         <v>435</v>
@@ -4531,7 +4522,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4556,37 +4547,37 @@
         <v>504</v>
       </c>
       <c r="C1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="F1" t="s">
         <v>504</v>
       </c>
       <c r="G1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="H1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="J1" t="s">
         <v>505</v>
       </c>
       <c r="K1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="L1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="N1" t="s">
         <v>505</v>
       </c>
       <c r="O1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="P1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -4615,7 +4606,7 @@
         <v>91</v>
       </c>
       <c r="M2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="N2" t="s">
         <v>325</v>
@@ -4627,7 +4618,7 @@
         <v>218</v>
       </c>
       <c r="R2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -4656,7 +4647,7 @@
         <v>92</v>
       </c>
       <c r="M3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="N3" t="s">
         <v>326</v>
@@ -4668,7 +4659,7 @@
         <v>219</v>
       </c>
       <c r="R3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -4688,7 +4679,7 @@
         <v>285</v>
       </c>
       <c r="K4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="L4" t="s">
         <v>399</v>
@@ -4700,7 +4691,7 @@
         <v>511</v>
       </c>
       <c r="P4" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -4720,7 +4711,7 @@
         <v>286</v>
       </c>
       <c r="K5" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="L5" t="s">
         <v>400</v>
@@ -4732,7 +4723,7 @@
         <v>512</v>
       </c>
       <c r="P5" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -4746,19 +4737,19 @@
         <v>513</v>
       </c>
       <c r="D6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F6" t="s">
         <v>329</v>
       </c>
       <c r="G6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="J6" t="s">
         <v>287</v>
       </c>
       <c r="K6" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="L6" t="s">
         <v>401</v>
@@ -4784,19 +4775,19 @@
         <v>514</v>
       </c>
       <c r="D7" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F7" t="s">
         <v>330</v>
       </c>
       <c r="G7" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="J7" t="s">
         <v>288</v>
       </c>
       <c r="K7" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="L7" t="s">
         <v>402</v>
@@ -4822,19 +4813,19 @@
         <v>515</v>
       </c>
       <c r="D8" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F8" t="s">
         <v>331</v>
       </c>
       <c r="G8" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="J8" t="s">
         <v>289</v>
       </c>
       <c r="K8" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="L8" t="s">
         <v>403</v>
@@ -4857,22 +4848,22 @@
         <v>516</v>
       </c>
       <c r="D9" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="F9" t="s">
         <v>332</v>
       </c>
       <c r="G9" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="J9" t="s">
         <v>290</v>
       </c>
       <c r="K9" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="L9" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="N9" t="s">
         <v>332</v>
@@ -4898,10 +4889,10 @@
         <v>291</v>
       </c>
       <c r="K10" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="L10" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="N10" t="s">
         <v>333</v>
@@ -4927,10 +4918,10 @@
         <v>292</v>
       </c>
       <c r="K11" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="L11" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="N11" t="s">
         <v>334</v>
@@ -4965,7 +4956,7 @@
         <v>93</v>
       </c>
       <c r="M12" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N12" t="s">
         <v>335</v>
@@ -5006,7 +4997,7 @@
         <v>94</v>
       </c>
       <c r="M13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="N13" t="s">
         <v>336</v>
@@ -5038,7 +5029,7 @@
         <v>95</v>
       </c>
       <c r="H14" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="J14" t="s">
         <v>293</v>
@@ -5047,7 +5038,7 @@
         <v>95</v>
       </c>
       <c r="M14" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="N14" t="s">
         <v>337</v>
@@ -5056,7 +5047,7 @@
         <v>95</v>
       </c>
       <c r="P14" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="R14" t="s">
         <v>235</v>
@@ -5082,7 +5073,7 @@
         <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="J15" t="s">
         <v>294</v>
@@ -5090,9 +5081,6 @@
       <c r="K15" t="s">
         <v>96</v>
       </c>
-      <c r="M15" t="s">
-        <v>553</v>
-      </c>
       <c r="N15" t="s">
         <v>341</v>
       </c>
@@ -5100,7 +5088,7 @@
         <v>96</v>
       </c>
       <c r="P15" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="R15" t="s">
         <v>236</v>
@@ -5135,7 +5123,7 @@
         <v>377</v>
       </c>
       <c r="P16" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -5167,7 +5155,7 @@
         <v>378</v>
       </c>
       <c r="P17" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -5202,7 +5190,7 @@
         <v>509</v>
       </c>
       <c r="P18" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -5237,7 +5225,7 @@
         <v>508</v>
       </c>
       <c r="P19" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -5272,7 +5260,7 @@
         <v>506</v>
       </c>
       <c r="P20" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -5307,7 +5295,7 @@
         <v>507</v>
       </c>
       <c r="P21" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -5359,7 +5347,7 @@
         <v>305</v>
       </c>
       <c r="K23" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="L23" t="s">
         <v>398</v>
@@ -5391,7 +5379,7 @@
         <v>97</v>
       </c>
       <c r="H24" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="J24" t="s">
         <v>301</v>
@@ -5399,9 +5387,6 @@
       <c r="K24" t="s">
         <v>97</v>
       </c>
-      <c r="M24" t="s">
-        <v>554</v>
-      </c>
       <c r="N24" t="s">
         <v>339</v>
       </c>
@@ -5409,7 +5394,7 @@
         <v>97</v>
       </c>
       <c r="P24" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="R24" t="s">
         <v>239</v>
@@ -5440,9 +5425,6 @@
       <c r="K25" t="s">
         <v>98</v>
       </c>
-      <c r="M25" t="s">
-        <v>547</v>
-      </c>
       <c r="N25" t="s">
         <v>340</v>
       </c>
@@ -5450,10 +5432,10 @@
         <v>98</v>
       </c>
       <c r="P25" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="R25" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -5473,7 +5455,7 @@
         <v>99</v>
       </c>
       <c r="H26" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="J26" t="s">
         <v>300</v>
@@ -5488,10 +5470,10 @@
         <v>99</v>
       </c>
       <c r="P26" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="R26" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -5526,10 +5508,10 @@
         <v>100</v>
       </c>
       <c r="P27" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="R27" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -5552,7 +5534,7 @@
         <v>351</v>
       </c>
       <c r="P28" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -5575,7 +5557,7 @@
         <v>352</v>
       </c>
       <c r="P29" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -5598,7 +5580,7 @@
         <v>353</v>
       </c>
       <c r="P30" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -5621,7 +5603,7 @@
         <v>354</v>
       </c>
       <c r="P31" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -5644,7 +5626,7 @@
         <v>355</v>
       </c>
       <c r="P32" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -5667,7 +5649,7 @@
         <v>356</v>
       </c>
       <c r="P33" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -5742,7 +5724,7 @@
         <v>101</v>
       </c>
       <c r="P36" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="R36" t="s">
         <v>208</v>
@@ -5759,7 +5741,7 @@
         <v>217</v>
       </c>
       <c r="D37" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F37" t="s">
         <v>360</v>
@@ -5780,10 +5762,10 @@
         <v>217</v>
       </c>
       <c r="P37" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="R37" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -5818,7 +5800,7 @@
         <v>365</v>
       </c>
       <c r="P38" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="R38" t="s">
         <v>202</v>
@@ -5856,7 +5838,7 @@
         <v>366</v>
       </c>
       <c r="P39" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="R39" t="s">
         <v>203</v>
@@ -5894,7 +5876,7 @@
         <v>510</v>
       </c>
       <c r="P40" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="R40" t="s">
         <v>204</v>
@@ -5932,7 +5914,7 @@
         <v>368</v>
       </c>
       <c r="P41" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="R41" t="s">
         <v>205</v>
@@ -6023,28 +6005,28 @@
         <v>532</v>
       </c>
       <c r="D1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="G1" t="s">
         <v>531</v>
       </c>
       <c r="H1" t="s">
+        <v>601</v>
+      </c>
+      <c r="I1" t="s">
+        <v>602</v>
+      </c>
+      <c r="J1" t="s">
+        <v>603</v>
+      </c>
+      <c r="K1" t="s">
         <v>604</v>
       </c>
-      <c r="I1" t="s">
-        <v>605</v>
-      </c>
-      <c r="J1" t="s">
-        <v>606</v>
-      </c>
-      <c r="K1" t="s">
-        <v>607</v>
-      </c>
       <c r="L1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -6117,10 +6099,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="G6" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -6128,13 +6110,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -6196,7 +6178,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="G11" t="s">
         <v>543</v>
@@ -6207,13 +6189,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -6225,14 +6207,14 @@
         <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H14">
         <f>SUM(H2:H11)</f>
         <v>14</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:L14" si="0">SUM(I2:I11)</f>
+        <f t="shared" ref="I14:J14" si="0">SUM(I2:I11)</f>
         <v>2</v>
       </c>
       <c r="J14">
@@ -6250,7 +6232,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="H15">
         <f>16-H14</f>
@@ -6271,10 +6253,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G17" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assigned STM32 UART to XCore 2.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="625">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1660,21 +1660,6 @@
   </si>
   <si>
     <t>JP3_8</t>
-  </si>
-  <si>
-    <t>U17_A1</t>
-  </si>
-  <si>
-    <t>U17_A2</t>
-  </si>
-  <si>
-    <t>U17_A3</t>
-  </si>
-  <si>
-    <t>U17_A5</t>
-  </si>
-  <si>
-    <t>U17_A4</t>
   </si>
   <si>
     <t>JP4_8</t>
@@ -2250,7 +2235,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="E26" sqref="E26:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4305,7 +4290,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="E21" t="s">
         <v>435</v>
@@ -4522,7 +4507,7 @@
   <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4534,7 +4519,8 @@
     <col min="6" max="6" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" customWidth="1"/>
     <col min="16" max="16" width="11.7109375" customWidth="1"/>
   </cols>
@@ -4547,37 +4533,37 @@
         <v>504</v>
       </c>
       <c r="C1" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="D1" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="F1" t="s">
         <v>504</v>
       </c>
       <c r="G1" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="H1" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J1" t="s">
         <v>505</v>
       </c>
       <c r="K1" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="L1" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="N1" t="s">
         <v>505</v>
       </c>
       <c r="O1" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="P1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -4605,9 +4591,6 @@
       <c r="K2" t="s">
         <v>91</v>
       </c>
-      <c r="M2" t="s">
-        <v>547</v>
-      </c>
       <c r="N2" t="s">
         <v>325</v>
       </c>
@@ -4618,7 +4601,7 @@
         <v>218</v>
       </c>
       <c r="R2" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -4646,9 +4629,6 @@
       <c r="K3" t="s">
         <v>92</v>
       </c>
-      <c r="M3" t="s">
-        <v>548</v>
-      </c>
       <c r="N3" t="s">
         <v>326</v>
       </c>
@@ -4659,7 +4639,7 @@
         <v>219</v>
       </c>
       <c r="R3" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -4679,7 +4659,7 @@
         <v>285</v>
       </c>
       <c r="K4" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="L4" t="s">
         <v>399</v>
@@ -4691,7 +4671,7 @@
         <v>511</v>
       </c>
       <c r="P4" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -4711,7 +4691,7 @@
         <v>286</v>
       </c>
       <c r="K5" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="L5" t="s">
         <v>400</v>
@@ -4723,7 +4703,7 @@
         <v>512</v>
       </c>
       <c r="P5" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -4737,19 +4717,19 @@
         <v>513</v>
       </c>
       <c r="D6" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="F6" t="s">
         <v>329</v>
       </c>
       <c r="G6" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="J6" t="s">
         <v>287</v>
       </c>
       <c r="K6" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="L6" t="s">
         <v>401</v>
@@ -4775,19 +4755,19 @@
         <v>514</v>
       </c>
       <c r="D7" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="F7" t="s">
         <v>330</v>
       </c>
       <c r="G7" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="J7" t="s">
         <v>288</v>
       </c>
       <c r="K7" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="L7" t="s">
         <v>402</v>
@@ -4813,19 +4793,19 @@
         <v>515</v>
       </c>
       <c r="D8" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="F8" t="s">
         <v>331</v>
       </c>
       <c r="G8" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="J8" t="s">
         <v>289</v>
       </c>
       <c r="K8" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="L8" t="s">
         <v>403</v>
@@ -4848,22 +4828,22 @@
         <v>516</v>
       </c>
       <c r="D9" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="F9" t="s">
         <v>332</v>
       </c>
       <c r="G9" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J9" t="s">
         <v>290</v>
       </c>
       <c r="K9" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="L9" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="N9" t="s">
         <v>332</v>
@@ -4889,10 +4869,10 @@
         <v>291</v>
       </c>
       <c r="K10" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="L10" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="N10" t="s">
         <v>333</v>
@@ -4918,10 +4898,10 @@
         <v>292</v>
       </c>
       <c r="K11" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="L11" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="N11" t="s">
         <v>334</v>
@@ -4955,9 +4935,6 @@
       <c r="K12" t="s">
         <v>93</v>
       </c>
-      <c r="M12" t="s">
-        <v>549</v>
-      </c>
       <c r="N12" t="s">
         <v>335</v>
       </c>
@@ -4996,9 +4973,6 @@
       <c r="K13" t="s">
         <v>94</v>
       </c>
-      <c r="M13" t="s">
-        <v>551</v>
-      </c>
       <c r="N13" t="s">
         <v>336</v>
       </c>
@@ -5029,7 +5003,7 @@
         <v>95</v>
       </c>
       <c r="H14" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="J14" t="s">
         <v>293</v>
@@ -5037,8 +5011,11 @@
       <c r="K14" t="s">
         <v>95</v>
       </c>
+      <c r="L14" t="s">
+        <v>220</v>
+      </c>
       <c r="M14" t="s">
-        <v>550</v>
+        <v>223</v>
       </c>
       <c r="N14" t="s">
         <v>337</v>
@@ -5047,7 +5024,7 @@
         <v>95</v>
       </c>
       <c r="P14" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="R14" t="s">
         <v>235</v>
@@ -5073,7 +5050,7 @@
         <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="J15" t="s">
         <v>294</v>
@@ -5088,7 +5065,7 @@
         <v>96</v>
       </c>
       <c r="P15" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="R15" t="s">
         <v>236</v>
@@ -5123,7 +5100,7 @@
         <v>377</v>
       </c>
       <c r="P16" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -5155,7 +5132,7 @@
         <v>378</v>
       </c>
       <c r="P17" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -5190,7 +5167,7 @@
         <v>509</v>
       </c>
       <c r="P18" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -5225,7 +5202,7 @@
         <v>508</v>
       </c>
       <c r="P19" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -5260,7 +5237,7 @@
         <v>506</v>
       </c>
       <c r="P20" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -5295,7 +5272,7 @@
         <v>507</v>
       </c>
       <c r="P21" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -5347,7 +5324,7 @@
         <v>305</v>
       </c>
       <c r="K23" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="L23" t="s">
         <v>398</v>
@@ -5379,7 +5356,7 @@
         <v>97</v>
       </c>
       <c r="H24" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="J24" t="s">
         <v>301</v>
@@ -5394,7 +5371,7 @@
         <v>97</v>
       </c>
       <c r="P24" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="R24" t="s">
         <v>239</v>
@@ -5432,10 +5409,10 @@
         <v>98</v>
       </c>
       <c r="P25" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="R25" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -5455,7 +5432,7 @@
         <v>99</v>
       </c>
       <c r="H26" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="J26" t="s">
         <v>300</v>
@@ -5463,6 +5440,12 @@
       <c r="K26" t="s">
         <v>99</v>
       </c>
+      <c r="L26" t="s">
+        <v>221</v>
+      </c>
+      <c r="M26" t="s">
+        <v>224</v>
+      </c>
       <c r="N26" t="s">
         <v>338</v>
       </c>
@@ -5470,10 +5453,10 @@
         <v>99</v>
       </c>
       <c r="P26" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="R26" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -5508,10 +5491,10 @@
         <v>100</v>
       </c>
       <c r="P27" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="R27" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -5534,7 +5517,7 @@
         <v>351</v>
       </c>
       <c r="P28" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -5557,7 +5540,7 @@
         <v>352</v>
       </c>
       <c r="P29" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -5580,7 +5563,7 @@
         <v>353</v>
       </c>
       <c r="P30" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -5603,7 +5586,7 @@
         <v>354</v>
       </c>
       <c r="P31" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -5626,7 +5609,7 @@
         <v>355</v>
       </c>
       <c r="P32" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -5649,7 +5632,7 @@
         <v>356</v>
       </c>
       <c r="P33" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -5724,7 +5707,7 @@
         <v>101</v>
       </c>
       <c r="P36" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="R36" t="s">
         <v>208</v>
@@ -5741,7 +5724,7 @@
         <v>217</v>
       </c>
       <c r="D37" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="F37" t="s">
         <v>360</v>
@@ -5762,10 +5745,10 @@
         <v>217</v>
       </c>
       <c r="P37" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="R37" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -5800,7 +5783,7 @@
         <v>365</v>
       </c>
       <c r="P38" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="R38" t="s">
         <v>202</v>
@@ -5838,7 +5821,7 @@
         <v>366</v>
       </c>
       <c r="P39" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="R39" t="s">
         <v>203</v>
@@ -5876,7 +5859,7 @@
         <v>510</v>
       </c>
       <c r="P40" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="R40" t="s">
         <v>204</v>
@@ -5914,7 +5897,7 @@
         <v>368</v>
       </c>
       <c r="P41" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="R41" t="s">
         <v>205</v>
@@ -5986,7 +5969,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6005,28 +5988,28 @@
         <v>532</v>
       </c>
       <c r="D1" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="E1" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="G1" t="s">
         <v>531</v>
       </c>
       <c r="H1" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="I1" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="J1" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="K1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="L1" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -6099,10 +6082,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="G6" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -6110,13 +6093,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -6166,7 +6149,7 @@
       <c r="G10" t="s">
         <v>542</v>
       </c>
-      <c r="L10">
+      <c r="J10">
         <v>3</v>
       </c>
     </row>
@@ -6178,7 +6161,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="G11" t="s">
         <v>543</v>
@@ -6189,13 +6172,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -6207,7 +6190,7 @@
         <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="H14">
         <f>SUM(H2:H11)</f>
@@ -6219,7 +6202,7 @@
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K14">
         <f>SUM(K2:K11)</f>
@@ -6227,12 +6210,12 @@
       </c>
       <c r="L14">
         <f>SUM(L2:L11)</f>
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="H15">
         <f>16-H14</f>
@@ -6244,7 +6227,7 @@
       </c>
       <c r="J15">
         <f>16-J14</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K15">
         <f>16-K14</f>
@@ -6253,10 +6236,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="G17" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PMod 2 (JP5) assigned to XCore 2.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="625">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -2235,7 +2235,7 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:F26"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4506,8 +4506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4600,9 +4600,6 @@
       <c r="P2" t="s">
         <v>218</v>
       </c>
-      <c r="R2" t="s">
-        <v>551</v>
-      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -4638,9 +4635,6 @@
       <c r="P3" t="s">
         <v>219</v>
       </c>
-      <c r="R3" t="s">
-        <v>552</v>
-      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -5058,6 +5052,9 @@
       <c r="K15" t="s">
         <v>96</v>
       </c>
+      <c r="L15" t="s">
+        <v>552</v>
+      </c>
       <c r="N15" t="s">
         <v>341</v>
       </c>
@@ -5364,6 +5361,9 @@
       <c r="K24" t="s">
         <v>97</v>
       </c>
+      <c r="L24" t="s">
+        <v>420</v>
+      </c>
       <c r="N24" t="s">
         <v>339</v>
       </c>
@@ -5484,6 +5484,9 @@
       <c r="K27" t="s">
         <v>100</v>
       </c>
+      <c r="L27" t="s">
+        <v>204</v>
+      </c>
       <c r="N27" t="s">
         <v>350</v>
       </c>
@@ -5612,7 +5615,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>491</v>
       </c>
@@ -5635,7 +5638,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>492</v>
       </c>
@@ -5655,7 +5658,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>493</v>
       </c>
@@ -5675,7 +5678,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>494</v>
       </c>
@@ -5700,6 +5703,9 @@
       <c r="K36" t="s">
         <v>101</v>
       </c>
+      <c r="L36" t="s">
+        <v>202</v>
+      </c>
       <c r="N36" t="s">
         <v>359</v>
       </c>
@@ -5709,11 +5715,8 @@
       <c r="P36" t="s">
         <v>606</v>
       </c>
-      <c r="R36" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>495</v>
       </c>
@@ -5738,6 +5741,9 @@
       <c r="K37" t="s">
         <v>217</v>
       </c>
+      <c r="L37" t="s">
+        <v>203</v>
+      </c>
       <c r="N37" t="s">
         <v>360</v>
       </c>
@@ -5747,11 +5753,8 @@
       <c r="P37" t="s">
         <v>607</v>
       </c>
-      <c r="R37" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>496</v>
       </c>
@@ -5776,6 +5779,9 @@
       <c r="K38" t="s">
         <v>365</v>
       </c>
+      <c r="L38" t="s">
+        <v>551</v>
+      </c>
       <c r="N38" t="s">
         <v>361</v>
       </c>
@@ -5785,11 +5791,8 @@
       <c r="P38" t="s">
         <v>608</v>
       </c>
-      <c r="R38" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>497</v>
       </c>
@@ -5814,6 +5817,9 @@
       <c r="K39" t="s">
         <v>366</v>
       </c>
+      <c r="L39" t="s">
+        <v>550</v>
+      </c>
       <c r="N39" t="s">
         <v>362</v>
       </c>
@@ -5823,11 +5829,8 @@
       <c r="P39" t="s">
         <v>609</v>
       </c>
-      <c r="R39" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>498</v>
       </c>
@@ -5852,6 +5855,9 @@
       <c r="K40" t="s">
         <v>510</v>
       </c>
+      <c r="L40" t="s">
+        <v>208</v>
+      </c>
       <c r="N40" t="s">
         <v>363</v>
       </c>
@@ -5861,11 +5867,8 @@
       <c r="P40" t="s">
         <v>613</v>
       </c>
-      <c r="R40" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>499</v>
       </c>
@@ -5890,6 +5893,9 @@
       <c r="K41" t="s">
         <v>368</v>
       </c>
+      <c r="L41" t="s">
+        <v>205</v>
+      </c>
       <c r="N41" t="s">
         <v>364</v>
       </c>
@@ -5899,11 +5905,8 @@
       <c r="P41" t="s">
         <v>614</v>
       </c>
-      <c r="R41" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>500</v>
       </c>
@@ -5917,7 +5920,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>501</v>
       </c>
@@ -5931,7 +5934,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>502</v>
       </c>
@@ -5945,7 +5948,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>503</v>
       </c>
@@ -5969,7 +5972,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6053,7 +6056,7 @@
       <c r="G4" t="s">
         <v>535</v>
       </c>
-      <c r="L4">
+      <c r="J4">
         <v>8</v>
       </c>
     </row>
@@ -6202,7 +6205,7 @@
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="K14">
         <f>SUM(K2:K11)</f>
@@ -6210,7 +6213,7 @@
       </c>
       <c r="L14">
         <f>SUM(L2:L11)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -6227,7 +6230,7 @@
       </c>
       <c r="J15">
         <f>16-J14</f>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="K15">
         <f>16-K14</f>

</xml_diff>

<commit_message>
Upgraded JP1 to a full XSYS input connector like the XK-1A board.
XLink signals not yet assigned, either X0LB or X0LA...

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="628">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1894,6 +1894,15 @@
   </si>
   <si>
     <t>UEXT_TXD</t>
+  </si>
+  <si>
+    <t>XSYS UART</t>
+  </si>
+  <si>
+    <t>XSYS_UART_TX</t>
+  </si>
+  <si>
+    <t>XSYS_UART_RX</t>
   </si>
 </sst>
 </file>
@@ -4506,8 +4515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4990,6 +4999,9 @@
       <c r="C14" t="s">
         <v>95</v>
       </c>
+      <c r="D14" t="s">
+        <v>544</v>
+      </c>
       <c r="F14" t="s">
         <v>337</v>
       </c>
@@ -5035,7 +5047,7 @@
         <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>544</v>
+        <v>192</v>
       </c>
       <c r="F15" t="s">
         <v>341</v>
@@ -5344,7 +5356,7 @@
         <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F24" t="s">
         <v>339</v>
@@ -5388,7 +5400,7 @@
         <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>187</v>
+        <v>626</v>
       </c>
       <c r="F25" t="s">
         <v>340</v>
@@ -5425,6 +5437,9 @@
       <c r="C26" t="s">
         <v>99</v>
       </c>
+      <c r="D26" t="s">
+        <v>545</v>
+      </c>
       <c r="F26" t="s">
         <v>338</v>
       </c>
@@ -5470,7 +5485,7 @@
         <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>186</v>
+        <v>627</v>
       </c>
       <c r="F27" t="s">
         <v>350</v>
@@ -5765,7 +5780,7 @@
         <v>365</v>
       </c>
       <c r="D38" t="s">
-        <v>546</v>
+        <v>189</v>
       </c>
       <c r="F38" t="s">
         <v>361</v>
@@ -5803,7 +5818,7 @@
         <v>366</v>
       </c>
       <c r="D39" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F39" t="s">
         <v>362</v>
@@ -5841,7 +5856,7 @@
         <v>510</v>
       </c>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F40" t="s">
         <v>363</v>
@@ -5879,7 +5894,7 @@
         <v>368</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F41" t="s">
         <v>364</v>
@@ -5969,10 +5984,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6187,53 +6202,69 @@
         <v>2</v>
       </c>
     </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>625</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>625</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f>SUM(B2:B12)</f>
-        <v>53</v>
-      </c>
-      <c r="G14" t="s">
-        <v>600</v>
-      </c>
-      <c r="H14">
-        <f>SUM(H2:H11)</f>
-        <v>14</v>
-      </c>
-      <c r="I14">
-        <f t="shared" ref="I14:J14" si="0">SUM(I2:I11)</f>
-        <v>2</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="K14">
-        <f>SUM(K2:K11)</f>
-        <v>16</v>
-      </c>
-      <c r="L14">
-        <f>SUM(L2:L11)</f>
-        <v>8</v>
+        <f>SUM(B2:B13)</f>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
+        <v>600</v>
+      </c>
+      <c r="H15">
+        <f>SUM(H2:H13)</f>
+        <v>16</v>
+      </c>
+      <c r="I15">
+        <f>SUM(I2:I13)</f>
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <f>SUM(J2:J13)</f>
+        <v>11</v>
+      </c>
+      <c r="K15">
+        <f>SUM(K2:K13)</f>
+        <v>16</v>
+      </c>
+      <c r="L15">
+        <f>SUM(L2:L13)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
         <v>610</v>
       </c>
-      <c r="H15">
-        <f>16-H14</f>
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <f>16-I14</f>
-        <v>14</v>
-      </c>
-      <c r="J15">
-        <f>16-J14</f>
+      <c r="H16">
+        <f>16-H15</f>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>16-I15</f>
+        <v>12</v>
+      </c>
+      <c r="J16">
+        <f>16-J15</f>
         <v>5</v>
       </c>
-      <c r="K15">
-        <f>16-K14</f>
+      <c r="K16">
+        <f>16-K15</f>
         <v>0</v>
       </c>
     </row>
@@ -6241,7 +6272,9 @@
       <c r="A17" t="s">
         <v>594</v>
       </c>
-      <c r="G17" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
         <v>595</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pmod 1 signals assigned.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="628">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -4513,10 +4513,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4534,7 +4534,7 @@
     <col min="16" max="16" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>459</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>460</v>
       </c>
@@ -4594,6 +4594,9 @@
       <c r="G2" t="s">
         <v>91</v>
       </c>
+      <c r="H2" t="s">
+        <v>236</v>
+      </c>
       <c r="J2" t="s">
         <v>281</v>
       </c>
@@ -4610,7 +4613,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>461</v>
       </c>
@@ -4629,6 +4632,9 @@
       <c r="G3" t="s">
         <v>92</v>
       </c>
+      <c r="H3" t="s">
+        <v>235</v>
+      </c>
       <c r="J3" t="s">
         <v>282</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>462</v>
       </c>
@@ -4677,7 +4683,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>463</v>
       </c>
@@ -4709,7 +4715,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>464</v>
       </c>
@@ -4747,7 +4753,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -4785,7 +4791,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>466</v>
       </c>
@@ -4820,7 +4826,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>467</v>
       </c>
@@ -4855,7 +4861,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>468</v>
       </c>
@@ -4884,7 +4890,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>469</v>
       </c>
@@ -4913,7 +4919,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>470</v>
       </c>
@@ -4932,6 +4938,9 @@
       <c r="G12" t="s">
         <v>93</v>
       </c>
+      <c r="H12" t="s">
+        <v>234</v>
+      </c>
       <c r="J12" t="s">
         <v>283</v>
       </c>
@@ -4947,11 +4956,8 @@
       <c r="P12" t="s">
         <v>457</v>
       </c>
-      <c r="R12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>471</v>
       </c>
@@ -4970,6 +4976,9 @@
       <c r="G13" t="s">
         <v>94</v>
       </c>
+      <c r="H13" t="s">
+        <v>233</v>
+      </c>
       <c r="J13" t="s">
         <v>284</v>
       </c>
@@ -4985,11 +4994,8 @@
       <c r="P13" t="s">
         <v>458</v>
       </c>
-      <c r="R13" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>472</v>
       </c>
@@ -5032,11 +5038,8 @@
       <c r="P14" t="s">
         <v>602</v>
       </c>
-      <c r="R14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>473</v>
       </c>
@@ -5076,11 +5079,8 @@
       <c r="P15" t="s">
         <v>604</v>
       </c>
-      <c r="R15" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>474</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>475</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>476</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>477</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>478</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>479</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>480</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>481</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>482</v>
       </c>
@@ -5385,11 +5385,8 @@
       <c r="P24" t="s">
         <v>603</v>
       </c>
-      <c r="R24" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>483</v>
       </c>
@@ -5423,11 +5420,8 @@
       <c r="P25" t="s">
         <v>605</v>
       </c>
-      <c r="R25" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>484</v>
       </c>
@@ -5470,11 +5464,8 @@
       <c r="P26" t="s">
         <v>601</v>
       </c>
-      <c r="R26" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>485</v>
       </c>
@@ -5493,6 +5484,9 @@
       <c r="G27" t="s">
         <v>100</v>
       </c>
+      <c r="H27" t="s">
+        <v>548</v>
+      </c>
       <c r="J27" t="s">
         <v>306</v>
       </c>
@@ -5511,11 +5505,8 @@
       <c r="P27" t="s">
         <v>612</v>
       </c>
-      <c r="R27" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>486</v>
       </c>
@@ -5538,7 +5529,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>487</v>
       </c>
@@ -5561,7 +5552,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>488</v>
       </c>
@@ -5584,7 +5575,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>489</v>
       </c>
@@ -5607,7 +5598,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>490</v>
       </c>
@@ -5826,6 +5817,9 @@
       <c r="G39" t="s">
         <v>366</v>
       </c>
+      <c r="H39" t="s">
+        <v>549</v>
+      </c>
       <c r="J39" t="s">
         <v>316</v>
       </c>
@@ -5864,6 +5858,9 @@
       <c r="G40" t="s">
         <v>510</v>
       </c>
+      <c r="H40" t="s">
+        <v>547</v>
+      </c>
       <c r="J40" t="s">
         <v>319</v>
       </c>
@@ -5901,6 +5898,9 @@
       </c>
       <c r="G41" t="s">
         <v>368</v>
+      </c>
+      <c r="H41" t="s">
+        <v>239</v>
       </c>
       <c r="J41" t="s">
         <v>320</v>
@@ -5987,7 +5987,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6054,10 +6054,13 @@
       <c r="B3">
         <v>8</v>
       </c>
+      <c r="D3" t="s">
+        <v>537</v>
+      </c>
       <c r="G3" t="s">
         <v>534</v>
       </c>
-      <c r="L3">
+      <c r="I3">
         <v>8</v>
       </c>
     </row>
@@ -6067,6 +6070,9 @@
       </c>
       <c r="B4">
         <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>539</v>
       </c>
       <c r="G4" t="s">
         <v>535</v>
@@ -6232,7 +6238,7 @@
       </c>
       <c r="I15">
         <f>SUM(I2:I13)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J15">
         <f>SUM(J2:J13)</f>
@@ -6244,7 +6250,7 @@
       </c>
       <c r="L15">
         <f>SUM(L2:L13)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -6257,7 +6263,7 @@
       </c>
       <c r="I16">
         <f>16-I15</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J16">
         <f>16-J15</f>

</xml_diff>

<commit_message>
Shifted Pmod 1 signal assignments to make use of X1_P1M and free up X1_P1D.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4516,7 +4516,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4595,7 +4595,7 @@
         <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J2" t="s">
         <v>281</v>
@@ -4633,7 +4633,7 @@
         <v>92</v>
       </c>
       <c r="H3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J3" t="s">
         <v>282</v>
@@ -4939,7 +4939,7 @@
         <v>93</v>
       </c>
       <c r="H12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J12" t="s">
         <v>283</v>
@@ -4976,9 +4976,6 @@
       <c r="G13" t="s">
         <v>94</v>
       </c>
-      <c r="H13" t="s">
-        <v>233</v>
-      </c>
       <c r="J13" t="s">
         <v>284</v>
       </c>
@@ -5485,7 +5482,7 @@
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="J27" t="s">
         <v>306</v>
@@ -5779,6 +5776,9 @@
       <c r="G38" t="s">
         <v>365</v>
       </c>
+      <c r="H38" t="s">
+        <v>549</v>
+      </c>
       <c r="J38" t="s">
         <v>315</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>366</v>
       </c>
       <c r="H39" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J39" t="s">
         <v>316</v>
@@ -5859,7 +5859,7 @@
         <v>510</v>
       </c>
       <c r="H40" t="s">
-        <v>547</v>
+        <v>239</v>
       </c>
       <c r="J40" t="s">
         <v>319</v>
@@ -5900,7 +5900,7 @@
         <v>368</v>
       </c>
       <c r="H41" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="J41" t="s">
         <v>320</v>

</xml_diff>

<commit_message>
Rewrote URDB.xn with all changes in the xmos-dualchip branch.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="628">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -4516,7 +4516,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5396,6 +5396,9 @@
       <c r="D25" t="s">
         <v>626</v>
       </c>
+      <c r="E25" t="s">
+        <v>223</v>
+      </c>
       <c r="F25" t="s">
         <v>340</v>
       </c>
@@ -5449,9 +5452,6 @@
       <c r="L26" t="s">
         <v>221</v>
       </c>
-      <c r="M26" t="s">
-        <v>224</v>
-      </c>
       <c r="N26" t="s">
         <v>338</v>
       </c>
@@ -5474,6 +5474,9 @@
       </c>
       <c r="D27" t="s">
         <v>627</v>
+      </c>
+      <c r="E27" t="s">
+        <v>224</v>
       </c>
       <c r="F27" t="s">
         <v>350</v>

</xml_diff>

<commit_message>
Pulled PC13 off of JP24 and replaced it with PD7.
This frees up PC13 for its one and only alternate function: RTC_AF1.

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="632">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1338,9 +1338,6 @@
     <t>PC14</t>
   </si>
   <si>
-    <t>PC13</t>
-  </si>
-  <si>
     <t>PE6</t>
   </si>
   <si>
@@ -1903,6 +1900,21 @@
   </si>
   <si>
     <t>XSYS_UART_RX</t>
+  </si>
+  <si>
+    <t>PD7</t>
+  </si>
+  <si>
+    <t>PD6</t>
+  </si>
+  <si>
+    <t>PD5</t>
+  </si>
+  <si>
+    <t>U2_TX</t>
+  </si>
+  <si>
+    <t>U2_RX</t>
   </si>
 </sst>
 </file>
@@ -2731,7 +2743,7 @@
         <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F15" t="s">
         <v>223</v>
@@ -3033,7 +3045,7 @@
         <v>98</v>
       </c>
       <c r="E25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F25" t="s">
         <v>224</v>
@@ -4073,10 +4085,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4244,7 +4256,7 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E16" t="s">
         <v>430</v>
@@ -4255,7 +4267,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E17" t="s">
         <v>431</v>
@@ -4266,7 +4278,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E18" t="s">
         <v>432</v>
@@ -4299,7 +4311,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E21" t="s">
         <v>435</v>
@@ -4310,7 +4322,7 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E22" t="s">
         <v>436</v>
@@ -4361,7 +4373,7 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -4369,7 +4381,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>422</v>
+        <v>442</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -4393,7 +4405,10 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>445</v>
+        <v>448</v>
+      </c>
+      <c r="E32" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -4412,10 +4427,7 @@
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>450</v>
-      </c>
-      <c r="E34" t="s">
-        <v>452</v>
+        <v>627</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4423,7 +4435,10 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>446</v>
+        <v>628</v>
+      </c>
+      <c r="E35" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -4431,7 +4446,10 @@
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>447</v>
+        <v>629</v>
+      </c>
+      <c r="E36" t="s">
+        <v>630</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4439,7 +4457,7 @@
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4447,6 +4465,22 @@
         <v>36</v>
       </c>
       <c r="D38" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
         <v>66</v>
       </c>
     </row>
@@ -4515,8 +4549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4536,48 +4570,48 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B1" t="s">
+        <v>503</v>
+      </c>
+      <c r="C1" t="s">
+        <v>574</v>
+      </c>
+      <c r="D1" t="s">
+        <v>572</v>
+      </c>
+      <c r="F1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G1" t="s">
+        <v>567</v>
+      </c>
+      <c r="H1" t="s">
+        <v>573</v>
+      </c>
+      <c r="J1" t="s">
         <v>504</v>
       </c>
-      <c r="C1" t="s">
-        <v>575</v>
-      </c>
-      <c r="D1" t="s">
-        <v>573</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
+        <v>568</v>
+      </c>
+      <c r="L1" t="s">
+        <v>570</v>
+      </c>
+      <c r="N1" t="s">
         <v>504</v>
       </c>
-      <c r="G1" t="s">
-        <v>568</v>
-      </c>
-      <c r="H1" t="s">
-        <v>574</v>
-      </c>
-      <c r="J1" t="s">
-        <v>505</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>569</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>571</v>
-      </c>
-      <c r="N1" t="s">
-        <v>505</v>
-      </c>
-      <c r="O1" t="s">
-        <v>570</v>
-      </c>
-      <c r="P1" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B2" t="s">
         <v>281</v>
@@ -4615,7 +4649,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B3" t="s">
         <v>282</v>
@@ -4653,13 +4687,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B4" t="s">
         <v>285</v>
       </c>
       <c r="C4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F4" t="s">
         <v>327</v>
@@ -4668,7 +4702,7 @@
         <v>285</v>
       </c>
       <c r="K4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L4" t="s">
         <v>399</v>
@@ -4677,21 +4711,21 @@
         <v>327</v>
       </c>
       <c r="O4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="P4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B5" t="s">
         <v>286</v>
       </c>
       <c r="C5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F5" t="s">
         <v>328</v>
@@ -4700,7 +4734,7 @@
         <v>286</v>
       </c>
       <c r="K5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L5" t="s">
         <v>400</v>
@@ -4709,36 +4743,36 @@
         <v>328</v>
       </c>
       <c r="O5" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="P5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B6" t="s">
         <v>287</v>
       </c>
       <c r="C6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F6" t="s">
         <v>329</v>
       </c>
       <c r="G6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="J6" t="s">
         <v>287</v>
       </c>
       <c r="K6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L6" t="s">
         <v>401</v>
@@ -4747,7 +4781,7 @@
         <v>329</v>
       </c>
       <c r="O6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="P6" t="s">
         <v>229</v>
@@ -4755,28 +4789,28 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B7" t="s">
         <v>288</v>
       </c>
       <c r="C7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F7" t="s">
         <v>330</v>
       </c>
       <c r="G7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="J7" t="s">
         <v>288</v>
       </c>
       <c r="K7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L7" t="s">
         <v>402</v>
@@ -4785,7 +4819,7 @@
         <v>330</v>
       </c>
       <c r="O7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="P7" t="s">
         <v>230</v>
@@ -4793,28 +4827,28 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B8" t="s">
         <v>289</v>
       </c>
       <c r="C8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F8" t="s">
         <v>331</v>
       </c>
       <c r="G8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J8" t="s">
         <v>289</v>
       </c>
       <c r="K8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L8" t="s">
         <v>403</v>
@@ -4823,53 +4857,53 @@
         <v>331</v>
       </c>
       <c r="O8" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B9" t="s">
         <v>290</v>
       </c>
       <c r="C9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F9" t="s">
         <v>332</v>
       </c>
       <c r="G9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J9" t="s">
         <v>290</v>
       </c>
       <c r="K9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="N9" t="s">
         <v>332</v>
       </c>
       <c r="O9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B10" t="s">
         <v>291</v>
       </c>
       <c r="C10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F10" t="s">
         <v>333</v>
@@ -4878,27 +4912,27 @@
         <v>291</v>
       </c>
       <c r="K10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L10" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="N10" t="s">
         <v>333</v>
       </c>
       <c r="O10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B11" t="s">
         <v>292</v>
       </c>
       <c r="C11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F11" t="s">
         <v>334</v>
@@ -4907,21 +4941,21 @@
         <v>292</v>
       </c>
       <c r="K11" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L11" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="N11" t="s">
         <v>334</v>
       </c>
       <c r="O11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B12" t="s">
         <v>283</v>
@@ -4954,12 +4988,12 @@
         <v>93</v>
       </c>
       <c r="P12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B13" t="s">
         <v>284</v>
@@ -4989,12 +5023,12 @@
         <v>94</v>
       </c>
       <c r="P13" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B14" t="s">
         <v>293</v>
@@ -5003,7 +5037,7 @@
         <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F14" t="s">
         <v>337</v>
@@ -5012,7 +5046,7 @@
         <v>95</v>
       </c>
       <c r="H14" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="J14" t="s">
         <v>293</v>
@@ -5033,12 +5067,12 @@
         <v>95</v>
       </c>
       <c r="P14" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B15" t="s">
         <v>294</v>
@@ -5056,7 +5090,7 @@
         <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="J15" t="s">
         <v>294</v>
@@ -5065,7 +5099,7 @@
         <v>96</v>
       </c>
       <c r="L15" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="N15" t="s">
         <v>341</v>
@@ -5074,12 +5108,12 @@
         <v>96</v>
       </c>
       <c r="P15" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B16" t="s">
         <v>295</v>
@@ -5106,12 +5140,12 @@
         <v>377</v>
       </c>
       <c r="P16" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B17" t="s">
         <v>296</v>
@@ -5138,152 +5172,152 @@
         <v>378</v>
       </c>
       <c r="P17" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B18" t="s">
         <v>297</v>
       </c>
       <c r="C18" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E18" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F18" t="s">
         <v>344</v>
       </c>
       <c r="G18" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J18" t="s">
         <v>297</v>
       </c>
       <c r="K18" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="N18" t="s">
         <v>344</v>
       </c>
       <c r="O18" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="P18" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B19" t="s">
         <v>298</v>
       </c>
       <c r="C19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E19" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F19" t="s">
         <v>345</v>
       </c>
       <c r="G19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J19" t="s">
         <v>298</v>
       </c>
       <c r="K19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="N19" t="s">
         <v>345</v>
       </c>
       <c r="O19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="P19" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B20" t="s">
         <v>302</v>
       </c>
       <c r="C20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F20" t="s">
         <v>346</v>
       </c>
       <c r="G20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J20" t="s">
         <v>302</v>
       </c>
       <c r="K20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="N20" t="s">
         <v>346</v>
       </c>
       <c r="O20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="P20" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B21" t="s">
         <v>303</v>
       </c>
       <c r="C21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E21" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F21" t="s">
         <v>347</v>
       </c>
       <c r="G21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J21" t="s">
         <v>303</v>
       </c>
       <c r="K21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="N21" t="s">
         <v>347</v>
       </c>
       <c r="O21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="P21" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B22" t="s">
         <v>304</v>
@@ -5312,7 +5346,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B23" t="s">
         <v>305</v>
@@ -5330,7 +5364,7 @@
         <v>305</v>
       </c>
       <c r="K23" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L23" t="s">
         <v>398</v>
@@ -5344,7 +5378,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B24" t="s">
         <v>301</v>
@@ -5353,7 +5387,7 @@
         <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F24" t="s">
         <v>339</v>
@@ -5362,7 +5396,7 @@
         <v>97</v>
       </c>
       <c r="H24" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J24" t="s">
         <v>301</v>
@@ -5380,12 +5414,12 @@
         <v>97</v>
       </c>
       <c r="P24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B25" t="s">
         <v>299</v>
@@ -5394,7 +5428,7 @@
         <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E25" t="s">
         <v>223</v>
@@ -5418,12 +5452,12 @@
         <v>98</v>
       </c>
       <c r="P25" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B26" t="s">
         <v>300</v>
@@ -5432,7 +5466,7 @@
         <v>99</v>
       </c>
       <c r="D26" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F26" t="s">
         <v>338</v>
@@ -5441,7 +5475,7 @@
         <v>99</v>
       </c>
       <c r="H26" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="J26" t="s">
         <v>300</v>
@@ -5459,12 +5493,12 @@
         <v>99</v>
       </c>
       <c r="P26" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B27" t="s">
         <v>306</v>
@@ -5473,7 +5507,7 @@
         <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E27" t="s">
         <v>224</v>
@@ -5485,7 +5519,7 @@
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="J27" t="s">
         <v>306</v>
@@ -5503,18 +5537,18 @@
         <v>100</v>
       </c>
       <c r="P27" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B28" t="s">
         <v>307</v>
       </c>
       <c r="C28" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F28" t="s">
         <v>351</v>
@@ -5526,18 +5560,18 @@
         <v>351</v>
       </c>
       <c r="P28" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B29" t="s">
         <v>308</v>
       </c>
       <c r="C29" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F29" t="s">
         <v>352</v>
@@ -5549,18 +5583,18 @@
         <v>352</v>
       </c>
       <c r="P29" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B30" t="s">
         <v>309</v>
       </c>
       <c r="C30" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F30" t="s">
         <v>353</v>
@@ -5572,18 +5606,18 @@
         <v>353</v>
       </c>
       <c r="P30" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B31" t="s">
         <v>310</v>
       </c>
       <c r="C31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F31" t="s">
         <v>354</v>
@@ -5595,18 +5629,18 @@
         <v>354</v>
       </c>
       <c r="P31" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B32" t="s">
         <v>311</v>
       </c>
       <c r="C32" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F32" t="s">
         <v>355</v>
@@ -5618,18 +5652,18 @@
         <v>355</v>
       </c>
       <c r="P32" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B33" t="s">
         <v>312</v>
       </c>
       <c r="C33" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F33" t="s">
         <v>356</v>
@@ -5641,18 +5675,18 @@
         <v>356</v>
       </c>
       <c r="P33" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B34" t="s">
         <v>313</v>
       </c>
       <c r="C34" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F34" t="s">
         <v>357</v>
@@ -5666,13 +5700,13 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B35" t="s">
         <v>314</v>
       </c>
       <c r="C35" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F35" t="s">
         <v>358</v>
@@ -5686,7 +5720,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B36" t="s">
         <v>317</v>
@@ -5719,12 +5753,12 @@
         <v>101</v>
       </c>
       <c r="P36" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B37" t="s">
         <v>318</v>
@@ -5733,7 +5767,7 @@
         <v>217</v>
       </c>
       <c r="D37" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F37" t="s">
         <v>360</v>
@@ -5757,12 +5791,12 @@
         <v>217</v>
       </c>
       <c r="P37" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B38" t="s">
         <v>315</v>
@@ -5780,7 +5814,7 @@
         <v>365</v>
       </c>
       <c r="H38" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J38" t="s">
         <v>315</v>
@@ -5789,7 +5823,7 @@
         <v>365</v>
       </c>
       <c r="L38" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="N38" t="s">
         <v>361</v>
@@ -5798,12 +5832,12 @@
         <v>365</v>
       </c>
       <c r="P38" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B39" t="s">
         <v>316</v>
@@ -5821,7 +5855,7 @@
         <v>366</v>
       </c>
       <c r="H39" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="J39" t="s">
         <v>316</v>
@@ -5830,7 +5864,7 @@
         <v>366</v>
       </c>
       <c r="L39" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N39" t="s">
         <v>362</v>
@@ -5839,18 +5873,18 @@
         <v>366</v>
       </c>
       <c r="P39" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B40" t="s">
         <v>319</v>
       </c>
       <c r="C40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D40" t="s">
         <v>187</v>
@@ -5859,7 +5893,7 @@
         <v>363</v>
       </c>
       <c r="G40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H40" t="s">
         <v>239</v>
@@ -5868,7 +5902,7 @@
         <v>319</v>
       </c>
       <c r="K40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L40" t="s">
         <v>208</v>
@@ -5877,15 +5911,15 @@
         <v>363</v>
       </c>
       <c r="O40" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="P40" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B41" t="s">
         <v>320</v>
@@ -5921,12 +5955,12 @@
         <v>368</v>
       </c>
       <c r="P41" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B42" t="s">
         <v>321</v>
@@ -5940,7 +5974,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B43" t="s">
         <v>322</v>
@@ -5954,7 +5988,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B44" t="s">
         <v>323</v>
@@ -5968,7 +6002,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B45" t="s">
         <v>324</v>
@@ -5990,7 +6024,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6003,48 +6037,48 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B1" t="s">
         <v>531</v>
       </c>
-      <c r="B1" t="s">
-        <v>532</v>
-      </c>
       <c r="D1" t="s">
+        <v>579</v>
+      </c>
+      <c r="E1" t="s">
         <v>580</v>
       </c>
-      <c r="E1" t="s">
-        <v>581</v>
-      </c>
       <c r="G1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="H1" t="s">
+        <v>595</v>
+      </c>
+      <c r="I1" t="s">
         <v>596</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>597</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>598</v>
       </c>
-      <c r="K1" t="s">
-        <v>599</v>
-      </c>
       <c r="L1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -6052,16 +6086,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I3">
         <v>8</v>
@@ -6069,16 +6103,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J4">
         <v>8</v>
@@ -6086,16 +6120,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H5">
         <v>6</v>
@@ -6103,16 +6137,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G6" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -6120,13 +6154,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -6134,16 +6168,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
+        <v>538</v>
+      </c>
+      <c r="G8" t="s">
         <v>539</v>
-      </c>
-      <c r="G8" t="s">
-        <v>540</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -6151,16 +6185,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G9" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K9">
         <v>9</v>
@@ -6168,13 +6202,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J10">
         <v>3</v>
@@ -6182,16 +6216,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G11" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="K11">
         <v>4</v>
@@ -6199,13 +6233,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -6213,13 +6247,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H13">
         <v>2</v>
@@ -6233,7 +6267,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H15">
         <f>SUM(H2:H13)</f>
@@ -6258,7 +6292,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="H16">
         <f>16-H15</f>
@@ -6279,12 +6313,12 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reassigned Pmod B signals to make use of all possible X1 1-bit ports.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Connections" sheetId="1" r:id="rId1"/>
@@ -4087,7 +4087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -4549,8 +4549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4628,9 +4628,6 @@
       <c r="G2" t="s">
         <v>91</v>
       </c>
-      <c r="H2" t="s">
-        <v>235</v>
-      </c>
       <c r="J2" t="s">
         <v>281</v>
       </c>
@@ -4666,9 +4663,6 @@
       <c r="G3" t="s">
         <v>92</v>
       </c>
-      <c r="H3" t="s">
-        <v>234</v>
-      </c>
       <c r="J3" t="s">
         <v>282</v>
       </c>
@@ -4972,9 +4966,6 @@
       <c r="G12" t="s">
         <v>93</v>
       </c>
-      <c r="H12" t="s">
-        <v>233</v>
-      </c>
       <c r="J12" t="s">
         <v>283</v>
       </c>
@@ -5439,6 +5430,9 @@
       <c r="G25" t="s">
         <v>98</v>
       </c>
+      <c r="H25" t="s">
+        <v>548</v>
+      </c>
       <c r="J25" t="s">
         <v>299</v>
       </c>
@@ -5519,7 +5513,7 @@
         <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>546</v>
+        <v>235</v>
       </c>
       <c r="J27" t="s">
         <v>306</v>
@@ -5737,6 +5731,9 @@
       <c r="G36" t="s">
         <v>101</v>
       </c>
+      <c r="H36" t="s">
+        <v>547</v>
+      </c>
       <c r="J36" t="s">
         <v>317</v>
       </c>
@@ -5775,6 +5772,9 @@
       <c r="G37" t="s">
         <v>217</v>
       </c>
+      <c r="H37" t="s">
+        <v>546</v>
+      </c>
       <c r="J37" t="s">
         <v>318</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>365</v>
       </c>
       <c r="H38" t="s">
-        <v>548</v>
+        <v>239</v>
       </c>
       <c r="J38" t="s">
         <v>315</v>
@@ -5855,7 +5855,7 @@
         <v>366</v>
       </c>
       <c r="H39" t="s">
-        <v>547</v>
+        <v>236</v>
       </c>
       <c r="J39" t="s">
         <v>316</v>
@@ -5896,7 +5896,7 @@
         <v>509</v>
       </c>
       <c r="H40" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="J40" t="s">
         <v>319</v>
@@ -5937,7 +5937,7 @@
         <v>368</v>
       </c>
       <c r="H41" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J41" t="s">
         <v>320</v>

</xml_diff>

<commit_message>
Shifted PWM signal assignments by one pin to use all available pins.
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Dualchip" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="458">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1389,6 +1389,9 @@
   </si>
   <si>
     <t>U2_RX</t>
+  </si>
+  <si>
+    <t>P16A14</t>
   </si>
 </sst>
 </file>
@@ -1729,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1882,7 @@
         <v>409</v>
       </c>
       <c r="L4" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="N4" t="s">
         <v>186</v>
@@ -1911,7 +1914,7 @@
         <v>410</v>
       </c>
       <c r="L5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N5" t="s">
         <v>187</v>
@@ -1949,7 +1952,7 @@
         <v>411</v>
       </c>
       <c r="L6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N6" t="s">
         <v>188</v>
@@ -1987,7 +1990,7 @@
         <v>412</v>
       </c>
       <c r="L7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="N7" t="s">
         <v>189</v>
@@ -2025,7 +2028,7 @@
         <v>413</v>
       </c>
       <c r="L8" t="s">
-        <v>236</v>
+        <v>387</v>
       </c>
       <c r="N8" t="s">
         <v>190</v>
@@ -2060,7 +2063,7 @@
         <v>414</v>
       </c>
       <c r="L9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="N9" t="s">
         <v>191</v>
@@ -2089,7 +2092,7 @@
         <v>415</v>
       </c>
       <c r="L10" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N10" t="s">
         <v>192</v>
@@ -2117,9 +2120,6 @@
       <c r="K11" t="s">
         <v>416</v>
       </c>
-      <c r="L11" t="s">
-        <v>389</v>
-      </c>
       <c r="N11" t="s">
         <v>193</v>
       </c>
@@ -2506,7 +2506,10 @@
         <v>163</v>
       </c>
       <c r="K22" t="s">
-        <v>229</v>
+        <v>457</v>
+      </c>
+      <c r="L22" t="s">
+        <v>231</v>
       </c>
       <c r="N22" t="s">
         <v>207</v>
@@ -2538,7 +2541,7 @@
         <v>417</v>
       </c>
       <c r="L23" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N23" t="s">
         <v>208</v>
@@ -3203,7 +3206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Major revision to the motor driver systems and associated cleanup.
-JP24 renamed to JP2.
-JP25 renamed to JP22.
-4th encoder added. Encoders are numbered 1-4, JP24-JP27.
-The encoders are each connected to a 4-bit port. This change makes
the encoders compatible with the existing XMOS quadrature encoder libraries.
-The third VNH2SP30 has been removed.
-Added a LN298N dual 2A H-bridge as the new IC3.
-The direction of the H-bridge motors is controlled through a shift register (IC7).
-Added a LV8549M 1A bipolar stepper driver.
-Reverse polarity protection circuit placed on-board.
-IMU interrupt signals shifted to all use the same 4-bit port (X3P4A).

Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Dualchip" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="479">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -290,9 +290,6 @@
     <t>Motor 1</t>
   </si>
   <si>
-    <t>Motor 2</t>
-  </si>
-  <si>
     <t>P1A</t>
   </si>
   <si>
@@ -767,9 +764,6 @@
     <t>PC4</t>
   </si>
   <si>
-    <t>PC5</t>
-  </si>
-  <si>
     <t>DAC0</t>
   </si>
   <si>
@@ -1157,30 +1151,6 @@
     <t>IC2_DIAGA</t>
   </si>
   <si>
-    <t>IC3_DIAGB</t>
-  </si>
-  <si>
-    <t>IC3_DIAGA</t>
-  </si>
-  <si>
-    <t>IC1_INB</t>
-  </si>
-  <si>
-    <t>IC1_INA</t>
-  </si>
-  <si>
-    <t>IC3_INB</t>
-  </si>
-  <si>
-    <t>IC3_INA</t>
-  </si>
-  <si>
-    <t>IC2_INB</t>
-  </si>
-  <si>
-    <t>IC2_INA</t>
-  </si>
-  <si>
     <t>IC1_PWM</t>
   </si>
   <si>
@@ -1295,15 +1265,6 @@
     <t>Total 1-bits</t>
   </si>
   <si>
-    <t>ENC0_B</t>
-  </si>
-  <si>
-    <t>ENC0_A</t>
-  </si>
-  <si>
-    <t>ENC0_Z</t>
-  </si>
-  <si>
     <t>ENC1_B</t>
   </si>
   <si>
@@ -1392,6 +1353,108 @@
   </si>
   <si>
     <t>P16A14</t>
+  </si>
+  <si>
+    <t>VNH2SP30 inputs</t>
+  </si>
+  <si>
+    <t>L298N inputs</t>
+  </si>
+  <si>
+    <t>Encoder 1</t>
+  </si>
+  <si>
+    <t>Encoder 2</t>
+  </si>
+  <si>
+    <t>Encoder 3</t>
+  </si>
+  <si>
+    <t>Encoder 4</t>
+  </si>
+  <si>
+    <t>IMU ints</t>
+  </si>
+  <si>
+    <t>U13 DRDY</t>
+  </si>
+  <si>
+    <t>P4E</t>
+  </si>
+  <si>
+    <t>P4A</t>
+  </si>
+  <si>
+    <t>P4B</t>
+  </si>
+  <si>
+    <t>P4C</t>
+  </si>
+  <si>
+    <t>P4D</t>
+  </si>
+  <si>
+    <t>P4F</t>
+  </si>
+  <si>
+    <t>IC7</t>
+  </si>
+  <si>
+    <t>VNH2SP30 DIAG</t>
+  </si>
+  <si>
+    <t>ENC3_Z</t>
+  </si>
+  <si>
+    <t>ENC3_B</t>
+  </si>
+  <si>
+    <t>ENC3_A</t>
+  </si>
+  <si>
+    <t>ENC4_A</t>
+  </si>
+  <si>
+    <t>ENC4_B</t>
+  </si>
+  <si>
+    <t>ENC4_Z</t>
+  </si>
+  <si>
+    <t>P4D0</t>
+  </si>
+  <si>
+    <t>P4D1</t>
+  </si>
+  <si>
+    <t>P4D2</t>
+  </si>
+  <si>
+    <t>P4D3</t>
+  </si>
+  <si>
+    <t>IC7_CLK</t>
+  </si>
+  <si>
+    <t>IC7_CLR</t>
+  </si>
+  <si>
+    <t>IC7_DATA</t>
+  </si>
+  <si>
+    <t>IC8_ENA</t>
+  </si>
+  <si>
+    <t>IC8_IN1</t>
+  </si>
+  <si>
+    <t>IC8_IN2</t>
+  </si>
+  <si>
+    <t>LN298 CSB</t>
+  </si>
+  <si>
+    <t>LN298 CSA</t>
   </si>
 </sst>
 </file>
@@ -1732,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,1448 +1816,1472 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C1" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="D1" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="F1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G1" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="H1" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="J1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="K1" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="L1" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="N1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="O1" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="P1" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K4" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="L4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="P4" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K5" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="L5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="P5" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D6" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G6" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="J6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K6" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="L6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P6" t="s">
-        <v>133</v>
+        <v>464</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D7" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="F7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G7" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="J7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K7" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="L7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P7" t="s">
-        <v>134</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D8" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="F8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G8" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="J8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K8" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="L8" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="N8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O8" t="s">
-        <v>339</v>
+        <v>337</v>
+      </c>
+      <c r="P8" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D9" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G9" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="J9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K9" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="L9" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="N9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K10" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="L10" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="N10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O10" t="s">
-        <v>341</v>
+        <v>339</v>
+      </c>
+      <c r="P10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K11" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="N11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O11" t="s">
-        <v>342</v>
+        <v>340</v>
+      </c>
+      <c r="P11" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H14" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="J14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P14" t="s">
-        <v>426</v>
+        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="J15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L15" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="N15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O15" t="s">
-        <v>96</v>
-      </c>
-      <c r="P15" t="s">
-        <v>428</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P16" t="s">
-        <v>390</v>
+        <v>419</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P17" t="s">
-        <v>377</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E18" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K18" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O18" t="s">
-        <v>333</v>
+        <v>467</v>
       </c>
       <c r="P18" t="s">
-        <v>391</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E19" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="N19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O19" t="s">
-        <v>332</v>
+        <v>468</v>
       </c>
       <c r="P19" t="s">
-        <v>378</v>
+        <v>462</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E20" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K20" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O20" t="s">
-        <v>330</v>
+        <v>469</v>
       </c>
       <c r="P20" t="s">
-        <v>379</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E21" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K21" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="N21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O21" t="s">
-        <v>331</v>
-      </c>
-      <c r="P21" t="s">
-        <v>380</v>
+        <v>470</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K22" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="L22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O22" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="P22" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K23" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="L23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H24" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="J24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P24" t="s">
-        <v>427</v>
+        <v>471</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="E25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H25" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="J25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O25" t="s">
-        <v>98</v>
-      </c>
-      <c r="P25" t="s">
-        <v>429</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D26" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H26" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="J26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P26" t="s">
-        <v>425</v>
+        <v>473</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="E27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P27" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C28" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N28" t="s">
-        <v>210</v>
+        <v>209</v>
+      </c>
+      <c r="O28" t="s">
+        <v>347</v>
       </c>
       <c r="P28" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N29" t="s">
-        <v>211</v>
+        <v>210</v>
+      </c>
+      <c r="O29" t="s">
+        <v>348</v>
       </c>
       <c r="P29" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N30" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="O30" t="s">
+        <v>341</v>
       </c>
       <c r="P30" t="s">
-        <v>385</v>
+        <v>417</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C31" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N31" t="s">
-        <v>213</v>
+        <v>212</v>
+      </c>
+      <c r="O31" t="s">
+        <v>342</v>
       </c>
       <c r="P31" t="s">
-        <v>386</v>
+        <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C32" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N32" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="O32" t="s">
+        <v>343</v>
       </c>
       <c r="P32" t="s">
-        <v>383</v>
+        <v>416</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C33" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N33" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="O33" t="s">
+        <v>345</v>
       </c>
       <c r="P33" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F34" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N34" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="O34" t="s">
+        <v>346</v>
+      </c>
+      <c r="P34" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H36" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O36" t="s">
-        <v>101</v>
-      </c>
-      <c r="P36" t="s">
-        <v>430</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D37" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="F37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H37" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P37" t="s">
-        <v>431</v>
+        <v>476</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L38" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="N38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P38" t="s">
-        <v>432</v>
+        <v>475</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L39" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P39" t="s">
-        <v>433</v>
+        <v>474</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C40" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G40" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K40" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O40" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="P40" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P41" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3204,15 +3291,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" customWidth="1"/>
@@ -3220,48 +3308,48 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D1" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="E1" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="G1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H1" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="I1" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="J1" t="s">
+        <v>412</v>
+      </c>
+      <c r="K1" t="s">
+        <v>413</v>
+      </c>
+      <c r="L1" t="s">
         <v>422</v>
-      </c>
-      <c r="K1" t="s">
-        <v>423</v>
-      </c>
-      <c r="L1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -3269,16 +3357,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I3">
         <v>8</v>
@@ -3286,16 +3374,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G4" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J4">
         <v>8</v>
@@ -3303,16 +3391,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H5">
         <v>6</v>
@@ -3320,16 +3408,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="G6" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="K6">
         <v>3</v>
@@ -3337,13 +3425,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="I7">
         <v>2</v>
@@ -3351,16 +3439,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -3368,16 +3456,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="D9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G9" t="s">
         <v>363</v>
-      </c>
-      <c r="G9" t="s">
-        <v>365</v>
       </c>
       <c r="K9">
         <v>9</v>
@@ -3385,13 +3473,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="J10">
         <v>3</v>
@@ -3399,16 +3487,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="G11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="K11">
         <v>4</v>
@@ -3416,13 +3504,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -3430,13 +3518,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="H13">
         <v>2</v>
@@ -3450,7 +3538,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="H15">
         <f>SUM(H2:H13)</f>
@@ -3475,7 +3563,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="H16">
         <f>16-H15</f>
@@ -3496,12 +3584,81 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>419</v>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>460</v>
+      </c>
+      <c r="B24" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>447</v>
+      </c>
+      <c r="B25" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>448</v>
+      </c>
+      <c r="B26" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>449</v>
+      </c>
+      <c r="B27" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>450</v>
+      </c>
+      <c r="B28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>451</v>
+      </c>
+      <c r="B29" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>445</v>
+      </c>
+      <c r="B32" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>446</v>
+      </c>
+      <c r="B33" t="s">
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -3513,7 +3670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3569,7 +3726,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3577,16 +3734,13 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
       <c r="D8" t="s">
         <v>28</v>
       </c>
@@ -3595,9 +3749,6 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
@@ -3607,7 +3758,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3615,7 +3766,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>477</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3655,7 +3806,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
@@ -3665,11 +3816,8 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
-        <v>249</v>
-      </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3677,7 +3825,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3734,7 +3882,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3750,7 +3898,7 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>478</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3758,12 +3906,12 @@
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3788,10 +3936,10 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3921,10 +4069,10 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
+        <v>242</v>
+      </c>
+      <c r="D44" t="s">
         <v>243</v>
-      </c>
-      <c r="D44" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3935,7 +4083,7 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -3947,7 +4095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -4116,10 +4264,10 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4127,10 +4275,10 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E17" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -4138,10 +4286,10 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4152,7 +4300,7 @@
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -4163,7 +4311,7 @@
         <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -4171,10 +4319,10 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="E21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -4182,10 +4330,10 @@
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E22" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4193,7 +4341,7 @@
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -4201,7 +4349,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -4209,7 +4357,7 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -4217,7 +4365,7 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -4225,7 +4373,7 @@
         <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -4233,7 +4381,7 @@
         <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -4241,7 +4389,7 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -4249,7 +4397,7 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -4257,7 +4405,7 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -4265,10 +4413,10 @@
         <v>30</v>
       </c>
       <c r="D32" t="s">
+        <v>271</v>
+      </c>
+      <c r="E32" t="s">
         <v>273</v>
-      </c>
-      <c r="E32" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -4276,10 +4424,10 @@
         <v>31</v>
       </c>
       <c r="D33" t="s">
+        <v>272</v>
+      </c>
+      <c r="E33" t="s">
         <v>274</v>
-      </c>
-      <c r="E33" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -4287,7 +4435,7 @@
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4295,10 +4443,10 @@
         <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="E35" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -4306,10 +4454,10 @@
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="E36" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4317,7 +4465,7 @@
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4325,7 +4473,7 @@
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -4333,7 +4481,7 @@
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -4366,38 +4514,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
         <v>105</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>106</v>
-      </c>
-      <c r="C2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
         <v>108</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final connections made to ethernet controller (OSC1 and !INT).
Signed-off-by: Joe Baker <jbaker0428@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentation/signal connections.xlsx
+++ b/Documentation/signal connections.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="XMOS Dualchip" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="481">
   <si>
     <t>ADCIN 0</t>
   </si>
@@ -1455,6 +1455,12 @@
   </si>
   <si>
     <t>LN298 CSA</t>
+  </si>
+  <si>
+    <t>ETH_OSC1</t>
+  </si>
+  <si>
+    <t>ETH_!INT</t>
   </si>
 </sst>
 </file>
@@ -1795,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,6 +1944,12 @@
       <c r="F4" t="s">
         <v>185</v>
       </c>
+      <c r="G4" t="s">
+        <v>333</v>
+      </c>
+      <c r="H4" t="s">
+        <v>479</v>
+      </c>
       <c r="J4" t="s">
         <v>143</v>
       </c>
@@ -2006,7 +2018,10 @@
         <v>187</v>
       </c>
       <c r="G6" t="s">
-        <v>390</v>
+        <v>335</v>
+      </c>
+      <c r="H6" t="s">
+        <v>480</v>
       </c>
       <c r="J6" t="s">
         <v>145</v>
@@ -2043,9 +2058,6 @@
       <c r="F7" t="s">
         <v>188</v>
       </c>
-      <c r="G7" t="s">
-        <v>391</v>
-      </c>
       <c r="J7" t="s">
         <v>146</v>
       </c>
@@ -2081,9 +2093,6 @@
       <c r="F8" t="s">
         <v>189</v>
       </c>
-      <c r="G8" t="s">
-        <v>392</v>
-      </c>
       <c r="J8" t="s">
         <v>147</v>
       </c>
@@ -2118,9 +2127,6 @@
       </c>
       <c r="F9" t="s">
         <v>190</v>
-      </c>
-      <c r="G9" t="s">
-        <v>393</v>
       </c>
       <c r="J9" t="s">
         <v>148</v>
@@ -4095,7 +4101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>

</xml_diff>